<commit_message>
kati 1 njesite doen
</commit_message>
<xml_diff>
--- a/5-Njësite-banesore/regjistri/22-Koordinatat-për-pjesë-të-ndertesës.xlsx-2602-0-Albnori.xlsx
+++ b/5-Njësite-banesore/regjistri/22-Koordinatat-për-pjesë-të-ndertesës.xlsx-2602-0-Albnori.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$86</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$109</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -680,6 +680,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -734,6 +739,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -778,14 +786,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -809,15 +809,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>451310</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>16719</xdr:rowOff>
+      <xdr:colOff>424096</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>166397</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>371474</xdr:colOff>
+      <xdr:colOff>344260</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>685801</xdr:rowOff>
+      <xdr:rowOff>644979</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -847,8 +847,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4375610" y="207219"/>
-          <a:ext cx="856335" cy="669082"/>
+          <a:off x="4479025" y="166397"/>
+          <a:ext cx="859056" cy="669082"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1086,6 +1086,325 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4586737" y="2598311"/>
+          <a:ext cx="3051603" cy="298800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Sistemi koordinat: KosovaRef01</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>424096</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>166397</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>344260</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>644979</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F399456-FFFA-4806-B53B-2B24D3A1E278}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4479025" y="166397"/>
+          <a:ext cx="859056" cy="669082"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>6569</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>13138</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2975170" cy="298800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="TextBox 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E91F6037-E9CB-49EA-8E58-E0677C590B64}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1231212" y="2326352"/>
+          <a:ext cx="2975170" cy="298800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Komuna: Ferizaj</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>839686</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>43127</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2953749" cy="298800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="TextBox 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07937452-2E79-4669-8F05-2069DFF859A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4894615" y="2356341"/>
+          <a:ext cx="2953749" cy="298800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Zona Kadastrale: Ferizaj</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>606643</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>89338</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3298607" cy="298800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="TextBox 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD9F1684-A2E1-4EF0-89C9-1E368E9A0FDD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1218964" y="2593052"/>
+          <a:ext cx="3298607" cy="298800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Numri</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> i njësis kadastrale</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>: 02602-0</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>842998</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>105246</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3051603" cy="298800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="TextBox 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87D2CC83-FE69-4C93-84EB-099D36DB81C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4897927" y="2608960"/>
           <a:ext cx="3051603" cy="298800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1425,10 +1744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K86"/>
+  <dimension ref="A1:K109"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="D43" sqref="C32:H51"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A81" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="U80" sqref="U80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1444,112 +1763,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="52"/>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
+      <c r="A1" s="55"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
     </row>
     <row r="2" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="52"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
     </row>
     <row r="4" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="51"/>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="51"/>
-      <c r="B5" s="51"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="51"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="51"/>
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="51"/>
+      <c r="A6" s="54"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="42"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="44"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="47"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="45"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="47"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="50"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="48"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="50"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="53"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
@@ -2000,10 +2319,10 @@
       <c r="E33" s="4">
         <v>4691722.8739999998</v>
       </c>
-      <c r="F33" s="53">
+      <c r="F33" s="56">
         <v>620.11199999999997</v>
       </c>
-      <c r="G33" s="53" t="s">
+      <c r="G33" s="56" t="s">
         <v>11</v>
       </c>
       <c r="H33" s="11" t="s">
@@ -2021,8 +2340,8 @@
       <c r="E34" s="4">
         <v>4691720.0990000004</v>
       </c>
-      <c r="F34" s="53"/>
-      <c r="G34" s="53"/>
+      <c r="F34" s="56"/>
+      <c r="G34" s="56"/>
       <c r="H34" s="11" t="s">
         <v>8</v>
       </c>
@@ -2038,8 +2357,8 @@
       <c r="E35" s="4">
         <v>4691719.3229999999</v>
       </c>
-      <c r="F35" s="53"/>
-      <c r="G35" s="53"/>
+      <c r="F35" s="56"/>
+      <c r="G35" s="56"/>
       <c r="H35" s="11" t="s">
         <v>8</v>
       </c>
@@ -2055,8 +2374,8 @@
       <c r="E36" s="4">
         <v>4691715.5049999999</v>
       </c>
-      <c r="F36" s="53"/>
-      <c r="G36" s="53"/>
+      <c r="F36" s="56"/>
+      <c r="G36" s="56"/>
       <c r="H36" s="11" t="s">
         <v>8</v>
       </c>
@@ -2072,8 +2391,8 @@
       <c r="E37" s="4">
         <v>4691715.8310000002</v>
       </c>
-      <c r="F37" s="53"/>
-      <c r="G37" s="53"/>
+      <c r="F37" s="56"/>
+      <c r="G37" s="56"/>
       <c r="H37" s="11" t="s">
         <v>8</v>
       </c>
@@ -2090,8 +2409,8 @@
       <c r="E38" s="4">
         <v>4691714.1189999999</v>
       </c>
-      <c r="F38" s="53"/>
-      <c r="G38" s="53"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="56"/>
       <c r="H38" s="11" t="s">
         <v>8</v>
       </c>
@@ -2109,8 +2428,8 @@
       <c r="E39" s="4">
         <v>4691711.4588000001</v>
       </c>
-      <c r="F39" s="53"/>
-      <c r="G39" s="53"/>
+      <c r="F39" s="56"/>
+      <c r="G39" s="56"/>
       <c r="H39" s="11" t="s">
         <v>8</v>
       </c>
@@ -2128,8 +2447,8 @@
       <c r="E40" s="4">
         <v>4691713.7060000002</v>
       </c>
-      <c r="F40" s="53"/>
-      <c r="G40" s="53"/>
+      <c r="F40" s="56"/>
+      <c r="G40" s="56"/>
       <c r="H40" s="11" t="s">
         <v>8</v>
       </c>
@@ -2138,18 +2457,18 @@
     </row>
     <row r="41" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
-      <c r="C41" s="69">
+      <c r="C41" s="36">
         <v>12</v>
       </c>
-      <c r="D41" s="70">
+      <c r="D41" s="37">
         <v>7513129.4539999999</v>
       </c>
-      <c r="E41" s="70">
+      <c r="E41" s="37">
         <v>4691712.6560000004</v>
       </c>
-      <c r="F41" s="71"/>
-      <c r="G41" s="71"/>
-      <c r="H41" s="72" t="s">
+      <c r="F41" s="57"/>
+      <c r="G41" s="57"/>
+      <c r="H41" s="38" t="s">
         <v>8</v>
       </c>
       <c r="I41" s="10"/>
@@ -2157,18 +2476,18 @@
     </row>
     <row r="42" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
-      <c r="C42" s="69">
+      <c r="C42" s="36">
         <v>13</v>
       </c>
-      <c r="D42" s="70">
+      <c r="D42" s="37">
         <v>7513129.1720000003</v>
       </c>
-      <c r="E42" s="70">
+      <c r="E42" s="37">
         <v>4691712.0049999999</v>
       </c>
-      <c r="F42" s="71"/>
-      <c r="G42" s="71"/>
-      <c r="H42" s="72" t="s">
+      <c r="F42" s="57"/>
+      <c r="G42" s="57"/>
+      <c r="H42" s="38" t="s">
         <v>8</v>
       </c>
       <c r="I42" s="10"/>
@@ -2176,18 +2495,18 @@
     </row>
     <row r="43" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
-      <c r="C43" s="69">
+      <c r="C43" s="36">
         <v>14</v>
       </c>
-      <c r="D43" s="70">
+      <c r="D43" s="37">
         <v>7513129.6200000001</v>
       </c>
-      <c r="E43" s="70">
+      <c r="E43" s="37">
         <v>4691710.9950000001</v>
       </c>
-      <c r="F43" s="71"/>
-      <c r="G43" s="71"/>
-      <c r="H43" s="72" t="s">
+      <c r="F43" s="57"/>
+      <c r="G43" s="57"/>
+      <c r="H43" s="38" t="s">
         <v>8</v>
       </c>
       <c r="I43" s="10"/>
@@ -2195,18 +2514,18 @@
     </row>
     <row r="44" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
-      <c r="C44" s="69">
+      <c r="C44" s="36">
         <v>15</v>
       </c>
-      <c r="D44" s="70">
+      <c r="D44" s="37">
         <v>7513132.6849999996</v>
       </c>
-      <c r="E44" s="70">
+      <c r="E44" s="37">
         <v>4691707.6550000003</v>
       </c>
-      <c r="F44" s="71"/>
-      <c r="G44" s="71"/>
-      <c r="H44" s="72" t="s">
+      <c r="F44" s="57"/>
+      <c r="G44" s="57"/>
+      <c r="H44" s="38" t="s">
         <v>8</v>
       </c>
       <c r="I44" s="10"/>
@@ -2214,18 +2533,18 @@
     </row>
     <row r="45" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
-      <c r="C45" s="69">
+      <c r="C45" s="36">
         <v>65</v>
       </c>
-      <c r="D45" s="70">
+      <c r="D45" s="37">
         <v>7513134.1550000003</v>
       </c>
-      <c r="E45" s="70">
+      <c r="E45" s="37">
         <v>4691707.0219999999</v>
       </c>
-      <c r="F45" s="71"/>
-      <c r="G45" s="71"/>
-      <c r="H45" s="72" t="s">
+      <c r="F45" s="57"/>
+      <c r="G45" s="57"/>
+      <c r="H45" s="38" t="s">
         <v>8</v>
       </c>
       <c r="I45" s="10"/>
@@ -2233,18 +2552,18 @@
     </row>
     <row r="46" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
-      <c r="C46" s="69">
+      <c r="C46" s="36">
         <v>67</v>
       </c>
-      <c r="D46" s="70">
+      <c r="D46" s="37">
         <v>7513135.8569999998</v>
       </c>
-      <c r="E46" s="70">
+      <c r="E46" s="37">
         <v>4691707.7450000001</v>
       </c>
-      <c r="F46" s="71"/>
-      <c r="G46" s="71"/>
-      <c r="H46" s="72" t="s">
+      <c r="F46" s="57"/>
+      <c r="G46" s="57"/>
+      <c r="H46" s="38" t="s">
         <v>8</v>
       </c>
       <c r="I46" s="10"/>
@@ -2252,18 +2571,18 @@
     </row>
     <row r="47" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
-      <c r="C47" s="69">
+      <c r="C47" s="36">
         <v>68</v>
       </c>
-      <c r="D47" s="70">
+      <c r="D47" s="37">
         <v>7513143.2529999996</v>
       </c>
-      <c r="E47" s="70">
+      <c r="E47" s="37">
         <v>4691714.4639999997</v>
       </c>
-      <c r="F47" s="71"/>
-      <c r="G47" s="71"/>
-      <c r="H47" s="72" t="s">
+      <c r="F47" s="57"/>
+      <c r="G47" s="57"/>
+      <c r="H47" s="38" t="s">
         <v>8</v>
       </c>
       <c r="I47" s="10"/>
@@ -2271,18 +2590,18 @@
     </row>
     <row r="48" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
-      <c r="C48" s="69">
+      <c r="C48" s="36">
         <v>101</v>
       </c>
-      <c r="D48" s="70">
+      <c r="D48" s="37">
         <v>7513132.5939999996</v>
       </c>
-      <c r="E48" s="70">
+      <c r="E48" s="37">
         <v>4691715.5387000004</v>
       </c>
-      <c r="F48" s="71"/>
-      <c r="G48" s="71"/>
-      <c r="H48" s="72" t="s">
+      <c r="F48" s="57"/>
+      <c r="G48" s="57"/>
+      <c r="H48" s="38" t="s">
         <v>8</v>
       </c>
       <c r="I48" s="10"/>
@@ -2290,18 +2609,18 @@
     </row>
     <row r="49" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
-      <c r="C49" s="69">
+      <c r="C49" s="36">
         <v>102</v>
       </c>
-      <c r="D49" s="70">
+      <c r="D49" s="37">
         <v>7513131.9008999998</v>
       </c>
-      <c r="E49" s="70">
+      <c r="E49" s="37">
         <v>4691716.2944</v>
       </c>
-      <c r="F49" s="71"/>
-      <c r="G49" s="71"/>
-      <c r="H49" s="72" t="s">
+      <c r="F49" s="57"/>
+      <c r="G49" s="57"/>
+      <c r="H49" s="38" t="s">
         <v>8</v>
       </c>
       <c r="I49" s="10"/>
@@ -2309,18 +2628,18 @@
     </row>
     <row r="50" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
-      <c r="C50" s="69">
+      <c r="C50" s="36">
         <v>103</v>
       </c>
-      <c r="D50" s="70">
+      <c r="D50" s="37">
         <v>7513132.1218999997</v>
       </c>
-      <c r="E50" s="70">
+      <c r="E50" s="37">
         <v>4691716.4972000001</v>
       </c>
-      <c r="F50" s="71"/>
-      <c r="G50" s="71"/>
-      <c r="H50" s="72" t="s">
+      <c r="F50" s="57"/>
+      <c r="G50" s="57"/>
+      <c r="H50" s="38" t="s">
         <v>8</v>
       </c>
       <c r="I50" s="10"/>
@@ -2338,15 +2657,15 @@
       <c r="E51" s="7">
         <v>4691717.4923</v>
       </c>
-      <c r="F51" s="54"/>
-      <c r="G51" s="54"/>
+      <c r="F51" s="58"/>
+      <c r="G51" s="58"/>
       <c r="H51" s="12" t="s">
         <v>8</v>
       </c>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="J52" s="1"/>
@@ -2355,625 +2674,791 @@
     <row r="53" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
-      <c r="C53" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E53" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F53" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G53" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H53" s="13" t="s">
-        <v>3</v>
-      </c>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
     </row>
     <row r="54" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
-      <c r="C54" s="5">
-        <v>14</v>
-      </c>
-      <c r="D54" s="4">
-        <v>7510834.5436000004</v>
-      </c>
-      <c r="E54" s="4">
-        <v>4693744.8530999999</v>
-      </c>
-      <c r="F54" s="56">
-        <v>584.09</v>
-      </c>
-      <c r="G54" s="56" t="s">
-        <v>20</v>
-      </c>
-      <c r="H54" s="27" t="s">
-        <v>8</v>
-      </c>
+      <c r="C54" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="59"/>
+      <c r="E54" s="59"/>
+      <c r="F54" s="59"/>
+      <c r="G54" s="59"/>
+      <c r="H54" s="59"/>
+      <c r="I54" s="59"/>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
     </row>
     <row r="55" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
-      <c r="C55" s="5">
-        <v>91</v>
-      </c>
-      <c r="D55" s="4">
-        <v>7510831.7971999999</v>
-      </c>
-      <c r="E55" s="4">
-        <v>4693766.6201999998</v>
-      </c>
-      <c r="F55" s="56"/>
-      <c r="G55" s="56"/>
-      <c r="H55" s="27" t="s">
-        <v>8</v>
-      </c>
+      <c r="C55" s="59"/>
+      <c r="D55" s="59"/>
+      <c r="E55" s="59"/>
+      <c r="F55" s="59"/>
+      <c r="G55" s="59"/>
+      <c r="H55" s="59"/>
+      <c r="I55" s="59"/>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
     </row>
     <row r="56" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
-      <c r="C56" s="5">
-        <v>92</v>
-      </c>
-      <c r="D56" s="4">
-        <v>7510822.3084000004</v>
-      </c>
-      <c r="E56" s="4">
-        <v>4693757.18</v>
-      </c>
-      <c r="F56" s="56"/>
-      <c r="G56" s="56"/>
-      <c r="H56" s="27" t="s">
-        <v>8</v>
-      </c>
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
     </row>
     <row r="57" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
-      <c r="C57" s="5">
-        <v>95</v>
-      </c>
-      <c r="D57" s="4">
-        <v>7510843.9336000001</v>
-      </c>
-      <c r="E57" s="4">
-        <v>4693754.3136</v>
-      </c>
-      <c r="F57" s="56"/>
-      <c r="G57" s="56"/>
-      <c r="H57" s="27" t="s">
-        <v>8</v>
-      </c>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
     </row>
     <row r="58" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
-      <c r="C58" s="5">
-        <v>96</v>
-      </c>
-      <c r="D58" s="4">
-        <v>7510827.6716</v>
-      </c>
-      <c r="E58" s="4">
-        <v>4693753.6573000001</v>
-      </c>
-      <c r="F58" s="56"/>
-      <c r="G58" s="56"/>
-      <c r="H58" s="27" t="s">
-        <v>8</v>
-      </c>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
     </row>
     <row r="59" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
-      <c r="C59" s="5">
-        <v>97</v>
-      </c>
-      <c r="D59" s="4">
-        <v>7510831.7936000004</v>
-      </c>
-      <c r="E59" s="4">
-        <v>4693757.7377000004</v>
-      </c>
-      <c r="F59" s="56"/>
-      <c r="G59" s="56"/>
-      <c r="H59" s="27" t="s">
-        <v>8</v>
-      </c>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
     </row>
     <row r="60" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
-      <c r="C60" s="5">
-        <v>98</v>
-      </c>
-      <c r="D60" s="4">
-        <v>7510835.1705</v>
-      </c>
-      <c r="E60" s="4">
-        <v>4693754.3263999997</v>
-      </c>
-      <c r="F60" s="56"/>
-      <c r="G60" s="56"/>
-      <c r="H60" s="27" t="s">
-        <v>8</v>
-      </c>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
     </row>
     <row r="61" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
-      <c r="C61" s="5">
-        <v>99</v>
-      </c>
-      <c r="D61" s="4">
-        <v>7510831.0484999996</v>
-      </c>
-      <c r="E61" s="4">
-        <v>4693750.2460000003</v>
-      </c>
-      <c r="F61" s="56"/>
-      <c r="G61" s="56"/>
-      <c r="H61" s="27" t="s">
-        <v>8</v>
-      </c>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
     </row>
     <row r="62" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
-      <c r="C62" s="5">
-        <v>100</v>
-      </c>
-      <c r="D62" s="4">
-        <v>7510833.4488000004</v>
-      </c>
-      <c r="E62" s="4">
-        <v>4693756.0656000003</v>
-      </c>
-      <c r="F62" s="56"/>
-      <c r="G62" s="56"/>
-      <c r="H62" s="27" t="s">
-        <v>8</v>
-      </c>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
     </row>
     <row r="63" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
-      <c r="C63" s="5">
-        <v>101</v>
-      </c>
-      <c r="D63" s="4">
-        <v>7510838.6793999998</v>
-      </c>
-      <c r="E63" s="4">
-        <v>4693761.3486000001</v>
-      </c>
-      <c r="F63" s="56"/>
-      <c r="G63" s="56"/>
-      <c r="H63" s="27" t="s">
-        <v>8</v>
-      </c>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
     </row>
     <row r="64" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
-      <c r="C64" s="5">
-        <v>102</v>
-      </c>
-      <c r="D64" s="4">
-        <v>7510827.4069999997</v>
-      </c>
-      <c r="E64" s="4">
-        <v>4693753.9248000002</v>
-      </c>
-      <c r="F64" s="56"/>
-      <c r="G64" s="56"/>
-      <c r="H64" s="27" t="s">
-        <v>8</v>
-      </c>
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
     </row>
-    <row r="65" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
-      <c r="C65" s="5">
-        <v>103</v>
-      </c>
-      <c r="D65" s="4">
-        <v>7510826.4649999999</v>
-      </c>
-      <c r="E65" s="4">
-        <v>4693752.9923</v>
-      </c>
-      <c r="F65" s="56"/>
-      <c r="G65" s="56"/>
-      <c r="H65" s="27" t="s">
-        <v>8</v>
-      </c>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
     </row>
     <row r="66" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="5">
-        <v>104</v>
-      </c>
-      <c r="D66" s="4">
-        <v>7510828.4380000001</v>
-      </c>
-      <c r="E66" s="4">
-        <v>4693751.0044999998</v>
-      </c>
-      <c r="F66" s="56"/>
-      <c r="G66" s="56"/>
-      <c r="H66" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="J66" s="1"/>
-      <c r="K66" s="1"/>
-    </row>
-    <row r="67" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="5">
-        <v>105</v>
-      </c>
-      <c r="D67" s="4">
-        <v>7510830.3949999996</v>
-      </c>
-      <c r="E67" s="4">
-        <v>4693749.0327000003</v>
-      </c>
-      <c r="F67" s="56"/>
-      <c r="G67" s="56"/>
-      <c r="H67" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="J67" s="1"/>
-      <c r="K67" s="1"/>
-    </row>
-    <row r="68" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="5">
-        <v>106</v>
-      </c>
-      <c r="D68" s="4">
-        <v>7510831.3317</v>
-      </c>
-      <c r="E68" s="4">
-        <v>4693749.9599000001</v>
-      </c>
-      <c r="F68" s="56"/>
-      <c r="G68" s="56"/>
-      <c r="H68" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="I68" s="1"/>
-      <c r="J68" s="1"/>
-      <c r="K68" s="1"/>
-    </row>
-    <row r="69" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="5">
-        <v>107</v>
-      </c>
-      <c r="D69" s="4">
-        <v>7510830.8696999997</v>
-      </c>
-      <c r="E69" s="4">
-        <v>4693756.8230999997</v>
-      </c>
-      <c r="F69" s="56"/>
-      <c r="G69" s="56"/>
-      <c r="H69" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="I69" s="1"/>
-      <c r="J69" s="1"/>
-      <c r="K69" s="1"/>
-    </row>
-    <row r="70" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="5">
-        <v>108</v>
-      </c>
-      <c r="D70" s="4">
-        <v>7510834.2466000002</v>
-      </c>
-      <c r="E70" s="4">
-        <v>4693753.4117999999</v>
-      </c>
-      <c r="F70" s="56"/>
-      <c r="G70" s="56"/>
-      <c r="H70" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="I70" s="1"/>
-      <c r="J70" s="1"/>
-      <c r="K70" s="1"/>
-    </row>
-    <row r="71" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C71" s="5">
-        <v>109</v>
-      </c>
-      <c r="D71" s="4">
-        <v>7510832.6496000001</v>
-      </c>
-      <c r="E71" s="4">
-        <v>4693767.4611</v>
-      </c>
-      <c r="F71" s="56"/>
-      <c r="G71" s="56"/>
-      <c r="H71" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="K71" s="1"/>
-    </row>
-    <row r="72" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C72" s="5">
-        <v>110</v>
-      </c>
-      <c r="D72" s="4">
-        <v>7510844.7790999999</v>
-      </c>
-      <c r="E72" s="4">
-        <v>4693755.1654000003</v>
-      </c>
-      <c r="F72" s="56"/>
-      <c r="G72" s="56"/>
-      <c r="H72" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="K72" s="1"/>
-    </row>
-    <row r="73" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="6">
-        <v>111</v>
-      </c>
-      <c r="D73" s="7">
-        <v>7510829.3679</v>
-      </c>
-      <c r="E73" s="7">
-        <v>4693751.9436999997</v>
-      </c>
-      <c r="F73" s="57"/>
-      <c r="G73" s="57"/>
-      <c r="H73" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="I73" s="1"/>
-      <c r="J73" s="1"/>
-      <c r="K73" s="1"/>
-    </row>
-    <row r="74" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="29"/>
-      <c r="D74" s="30"/>
-      <c r="E74" s="30"/>
-      <c r="F74" s="31"/>
-      <c r="G74" s="31"/>
-      <c r="H74" s="26"/>
-      <c r="I74" s="1"/>
-      <c r="J74" s="1"/>
-      <c r="K74" s="1"/>
-    </row>
-    <row r="75" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="55" t="s">
-        <v>9</v>
-      </c>
-      <c r="D75" s="55"/>
-      <c r="E75" s="55"/>
-      <c r="F75" s="55"/>
-      <c r="G75" s="55"/>
-      <c r="H75" s="55"/>
-      <c r="I75" s="55"/>
-      <c r="J75" s="1"/>
-      <c r="K75" s="1"/>
-    </row>
-    <row r="76" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
-      <c r="C76" s="55"/>
-      <c r="D76" s="55"/>
-      <c r="E76" s="55"/>
-      <c r="F76" s="55"/>
-      <c r="G76" s="55"/>
-      <c r="H76" s="55"/>
-      <c r="I76" s="55"/>
-      <c r="J76" s="1"/>
-      <c r="K76" s="1"/>
-    </row>
-    <row r="77" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
-      <c r="C77" s="25"/>
-      <c r="D77" s="25"/>
-      <c r="E77" s="25"/>
-      <c r="F77" s="25"/>
-      <c r="G77" s="25"/>
-      <c r="H77" s="25"/>
-      <c r="I77" s="25"/>
-      <c r="J77" s="1"/>
-      <c r="K77" s="1"/>
+      <c r="A66" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="F66" s="63"/>
+      <c r="G66" s="64"/>
+      <c r="H66" s="65" t="s">
+        <v>6</v>
+      </c>
+      <c r="I66" s="66"/>
+      <c r="J66" s="69"/>
+      <c r="K66" s="70"/>
+    </row>
+    <row r="67" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67" s="40"/>
+      <c r="C67" s="40"/>
+      <c r="D67" s="41"/>
+      <c r="E67" s="42">
+        <v>152</v>
+      </c>
+      <c r="F67" s="43"/>
+      <c r="G67" s="44"/>
+      <c r="H67" s="67"/>
+      <c r="I67" s="68"/>
+      <c r="J67" s="71"/>
+      <c r="K67" s="72"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" s="55"/>
+      <c r="B68" s="55"/>
+      <c r="C68" s="55"/>
+      <c r="D68" s="55"/>
+      <c r="E68" s="55"/>
+      <c r="F68" s="55"/>
+      <c r="G68" s="55"/>
+      <c r="H68" s="55"/>
+      <c r="I68" s="55"/>
+      <c r="J68" s="55"/>
+      <c r="K68" s="55"/>
+    </row>
+    <row r="69" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="55"/>
+      <c r="B69" s="55"/>
+      <c r="C69" s="55"/>
+      <c r="D69" s="55"/>
+      <c r="E69" s="55"/>
+      <c r="F69" s="55"/>
+      <c r="G69" s="55"/>
+      <c r="H69" s="55"/>
+      <c r="I69" s="55"/>
+      <c r="J69" s="55"/>
+      <c r="K69" s="55"/>
+    </row>
+    <row r="70" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="B70" s="54"/>
+      <c r="C70" s="54"/>
+      <c r="D70" s="54"/>
+      <c r="E70" s="54"/>
+      <c r="F70" s="54"/>
+      <c r="G70" s="54"/>
+      <c r="H70" s="54"/>
+      <c r="I70" s="54"/>
+      <c r="J70" s="54"/>
+      <c r="K70" s="54"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" s="54"/>
+      <c r="B71" s="54"/>
+      <c r="C71" s="54"/>
+      <c r="D71" s="54"/>
+      <c r="E71" s="54"/>
+      <c r="F71" s="54"/>
+      <c r="G71" s="54"/>
+      <c r="H71" s="54"/>
+      <c r="I71" s="54"/>
+      <c r="J71" s="54"/>
+      <c r="K71" s="54"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" s="54"/>
+      <c r="B72" s="54"/>
+      <c r="C72" s="54"/>
+      <c r="D72" s="54"/>
+      <c r="E72" s="54"/>
+      <c r="F72" s="54"/>
+      <c r="G72" s="54"/>
+      <c r="H72" s="54"/>
+      <c r="I72" s="54"/>
+      <c r="J72" s="54"/>
+      <c r="K72" s="54"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" s="54"/>
+      <c r="B73" s="54"/>
+      <c r="C73" s="54"/>
+      <c r="D73" s="54"/>
+      <c r="E73" s="54"/>
+      <c r="F73" s="54"/>
+      <c r="G73" s="54"/>
+      <c r="H73" s="54"/>
+      <c r="I73" s="54"/>
+      <c r="J73" s="54"/>
+      <c r="K73" s="54"/>
+    </row>
+    <row r="74" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C75" s="45"/>
+      <c r="D75" s="46"/>
+      <c r="E75" s="46"/>
+      <c r="F75" s="46"/>
+      <c r="G75" s="46"/>
+      <c r="H75" s="46"/>
+      <c r="I75" s="47"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C76" s="48"/>
+      <c r="D76" s="49"/>
+      <c r="E76" s="49"/>
+      <c r="F76" s="49"/>
+      <c r="G76" s="49"/>
+      <c r="H76" s="49"/>
+      <c r="I76" s="50"/>
+    </row>
+    <row r="77" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C77" s="51"/>
+      <c r="D77" s="52"/>
+      <c r="E77" s="52"/>
+      <c r="F77" s="52"/>
+      <c r="G77" s="52"/>
+      <c r="H77" s="52"/>
+      <c r="I77" s="53"/>
     </row>
     <row r="78" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
-      <c r="C78" s="25"/>
-      <c r="D78" s="25"/>
-      <c r="E78" s="25"/>
-      <c r="F78" s="25"/>
-      <c r="G78" s="25"/>
-      <c r="H78" s="25"/>
-      <c r="I78" s="25"/>
+      <c r="C78" s="29"/>
+      <c r="D78" s="30"/>
+      <c r="E78" s="30"/>
+      <c r="F78" s="31"/>
+      <c r="G78" s="31"/>
+      <c r="H78" s="26"/>
+      <c r="I78" s="1"/>
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
     </row>
-    <row r="79" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="25"/>
-      <c r="D79" s="25"/>
-      <c r="E79" s="25"/>
-      <c r="F79" s="25"/>
-      <c r="G79" s="25"/>
-      <c r="H79" s="25"/>
-      <c r="I79" s="25"/>
+      <c r="H79" s="26"/>
+      <c r="I79" s="1"/>
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
     </row>
     <row r="80" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
-      <c r="C80" s="25"/>
-      <c r="D80" s="25"/>
-      <c r="E80" s="25"/>
-      <c r="F80" s="25"/>
-      <c r="G80" s="25"/>
-      <c r="H80" s="25"/>
-      <c r="I80" s="25"/>
+      <c r="C80" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D80" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E80" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F80" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G80" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H80" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I80" s="1"/>
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
     </row>
     <row r="81" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
-      <c r="B81" s="1"/>
-      <c r="C81" s="25"/>
-      <c r="D81" s="25"/>
-      <c r="E81" s="25"/>
-      <c r="F81" s="25"/>
-      <c r="G81" s="25"/>
-      <c r="H81" s="25"/>
-      <c r="I81" s="25"/>
+      <c r="C81" s="5">
+        <v>1</v>
+      </c>
+      <c r="D81" s="4">
+        <v>7513135.568</v>
+      </c>
+      <c r="E81" s="4">
+        <v>4691722.8739999998</v>
+      </c>
+      <c r="F81" s="60">
+        <v>623.17399999999998</v>
+      </c>
+      <c r="G81" s="60" t="s">
+        <v>20</v>
+      </c>
+      <c r="H81" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="I81" s="1"/>
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
     </row>
     <row r="82" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
-      <c r="C82" s="25"/>
-      <c r="D82" s="25"/>
-      <c r="E82" s="25"/>
-      <c r="F82" s="25"/>
-      <c r="G82" s="25"/>
-      <c r="H82" s="25"/>
-      <c r="I82" s="25"/>
+      <c r="C82" s="5">
+        <v>2</v>
+      </c>
+      <c r="D82" s="4">
+        <v>7513132.5010000002</v>
+      </c>
+      <c r="E82" s="4">
+        <v>4691720.0990000004</v>
+      </c>
+      <c r="F82" s="60"/>
+      <c r="G82" s="60"/>
+      <c r="H82" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="I82" s="1"/>
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
     </row>
     <row r="83" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="25"/>
-      <c r="D83" s="25"/>
-      <c r="E83" s="25"/>
-      <c r="F83" s="25"/>
-      <c r="G83" s="25"/>
-      <c r="H83" s="25"/>
-      <c r="I83" s="25"/>
+      <c r="C83" s="5">
+        <v>7</v>
+      </c>
+      <c r="D83" s="4">
+        <v>7513128.9859999996</v>
+      </c>
+      <c r="E83" s="4">
+        <v>4691715.5049999999</v>
+      </c>
+      <c r="F83" s="60"/>
+      <c r="G83" s="60"/>
+      <c r="H83" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="I83" s="1"/>
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
     </row>
-    <row r="84" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
-      <c r="C84" s="25"/>
-      <c r="D84" s="25"/>
-      <c r="E84" s="25"/>
-      <c r="F84" s="25"/>
-      <c r="G84" s="25"/>
-      <c r="H84" s="25"/>
-      <c r="I84" s="25"/>
+      <c r="C84" s="5">
+        <v>23</v>
+      </c>
+      <c r="D84" s="4">
+        <v>7513133.25</v>
+      </c>
+      <c r="E84" s="4">
+        <v>4691719.318</v>
+      </c>
+      <c r="F84" s="60"/>
+      <c r="G84" s="60"/>
+      <c r="H84" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="I84" s="1"/>
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
     </row>
     <row r="85" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A85" s="2" t="s">
+      <c r="A85" s="1"/>
+      <c r="C85" s="5">
+        <v>24</v>
+      </c>
+      <c r="D85" s="4">
+        <v>7513127.2779999999</v>
+      </c>
+      <c r="E85" s="4">
+        <v>4691713.9479999999</v>
+      </c>
+      <c r="F85" s="60"/>
+      <c r="G85" s="60"/>
+      <c r="H85" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="I85" s="1"/>
+      <c r="J85" s="1"/>
+      <c r="K85" s="1"/>
+    </row>
+    <row r="86" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A86" s="1"/>
+      <c r="C86" s="5">
+        <v>25</v>
+      </c>
+      <c r="D86" s="4">
+        <v>7513127.3820000002</v>
+      </c>
+      <c r="E86" s="4">
+        <v>4691712.1909999996</v>
+      </c>
+      <c r="F86" s="60"/>
+      <c r="G86" s="60"/>
+      <c r="H86" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="I86" s="1"/>
+      <c r="J86" s="1"/>
+      <c r="K86" s="1"/>
+    </row>
+    <row r="87" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A87" s="1"/>
+      <c r="C87" s="5">
+        <v>26</v>
+      </c>
+      <c r="D87" s="4">
+        <v>7513128.142</v>
+      </c>
+      <c r="E87" s="4">
+        <v>4691711.0889999997</v>
+      </c>
+      <c r="F87" s="60"/>
+      <c r="G87" s="60"/>
+      <c r="H87" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="I87" s="1"/>
+      <c r="J87" s="1"/>
+      <c r="K87" s="1"/>
+    </row>
+    <row r="88" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A88" s="1"/>
+      <c r="C88" s="5">
+        <v>27</v>
+      </c>
+      <c r="D88" s="4">
+        <v>7513132.0240000002</v>
+      </c>
+      <c r="E88" s="4">
+        <v>4691706.8949999996</v>
+      </c>
+      <c r="F88" s="60"/>
+      <c r="G88" s="60"/>
+      <c r="H88" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="I88" s="1"/>
+      <c r="J88" s="1"/>
+      <c r="K88" s="1"/>
+    </row>
+    <row r="89" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A89" s="1"/>
+      <c r="C89" s="5">
+        <v>28</v>
+      </c>
+      <c r="D89" s="4">
+        <v>7513133.5190000003</v>
+      </c>
+      <c r="E89" s="4">
+        <v>4691706.18</v>
+      </c>
+      <c r="F89" s="60"/>
+      <c r="G89" s="60"/>
+      <c r="H89" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="I89" s="1"/>
+      <c r="J89" s="1"/>
+      <c r="K89" s="1"/>
+    </row>
+    <row r="90" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A90" s="1"/>
+      <c r="C90" s="5">
+        <v>65</v>
+      </c>
+      <c r="D90" s="4">
+        <v>7513134.1436999999</v>
+      </c>
+      <c r="E90" s="4">
+        <v>4691706.1939000003</v>
+      </c>
+      <c r="F90" s="60"/>
+      <c r="G90" s="60"/>
+      <c r="H90" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="I90" s="1"/>
+      <c r="J90" s="1"/>
+      <c r="K90" s="1"/>
+    </row>
+    <row r="91" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A91" s="1"/>
+      <c r="C91" s="5">
+        <v>67</v>
+      </c>
+      <c r="D91" s="4">
+        <v>7513135.8569999998</v>
+      </c>
+      <c r="E91" s="4">
+        <v>4691707.7450000001</v>
+      </c>
+      <c r="F91" s="60"/>
+      <c r="G91" s="60"/>
+      <c r="H91" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="I91" s="1"/>
+      <c r="J91" s="1"/>
+      <c r="K91" s="1"/>
+    </row>
+    <row r="92" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A92" s="1"/>
+      <c r="C92" s="5">
+        <v>68</v>
+      </c>
+      <c r="D92" s="4">
+        <v>7513143.2529999996</v>
+      </c>
+      <c r="E92" s="4">
+        <v>4691714.4639999997</v>
+      </c>
+      <c r="F92" s="60"/>
+      <c r="G92" s="60"/>
+      <c r="H92" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="I92" s="1"/>
+      <c r="J92" s="1"/>
+      <c r="K92" s="1"/>
+    </row>
+    <row r="93" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A93" s="1"/>
+      <c r="C93" s="5">
+        <v>106</v>
+      </c>
+      <c r="D93" s="4">
+        <v>7513136.3592999997</v>
+      </c>
+      <c r="E93" s="4">
+        <v>4691715.8525</v>
+      </c>
+      <c r="F93" s="60"/>
+      <c r="G93" s="60"/>
+      <c r="H93" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="I93" s="1"/>
+      <c r="J93" s="1"/>
+      <c r="K93" s="1"/>
+    </row>
+    <row r="94" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A94" s="1"/>
+      <c r="C94" s="5">
+        <v>107</v>
+      </c>
+      <c r="D94" s="4">
+        <v>7513132.6316</v>
+      </c>
+      <c r="E94" s="4">
+        <v>4691712.5202000001</v>
+      </c>
+      <c r="F94" s="60"/>
+      <c r="G94" s="60"/>
+      <c r="H94" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="I94" s="1"/>
+      <c r="J94" s="1"/>
+      <c r="K94" s="1"/>
+    </row>
+    <row r="95" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="6">
+        <v>108</v>
+      </c>
+      <c r="D95" s="7">
+        <v>7513129.5292999996</v>
+      </c>
+      <c r="E95" s="7">
+        <v>4691715.9907</v>
+      </c>
+      <c r="F95" s="61"/>
+      <c r="G95" s="61"/>
+      <c r="H95" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="I95" s="1"/>
+      <c r="J95" s="1"/>
+      <c r="K95" s="1"/>
+    </row>
+    <row r="96" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="29"/>
+      <c r="D96" s="30"/>
+      <c r="E96" s="30"/>
+      <c r="F96" s="31"/>
+      <c r="G96" s="31"/>
+      <c r="H96" s="26"/>
+      <c r="I96" s="1"/>
+      <c r="J96" s="1"/>
+      <c r="K96" s="1"/>
+    </row>
+    <row r="97" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+      <c r="C97" s="29"/>
+      <c r="D97" s="30"/>
+      <c r="E97" s="30"/>
+      <c r="F97" s="31"/>
+      <c r="G97" s="31"/>
+      <c r="H97" s="26"/>
+      <c r="I97" s="1"/>
+      <c r="J97" s="1"/>
+      <c r="K97" s="1"/>
+    </row>
+    <row r="98" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="29"/>
+      <c r="D98" s="30"/>
+      <c r="E98" s="30"/>
+      <c r="F98" s="31"/>
+      <c r="G98" s="31"/>
+      <c r="H98" s="26"/>
+      <c r="I98" s="1"/>
+      <c r="J98" s="1"/>
+      <c r="K98" s="1"/>
+    </row>
+    <row r="99" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
+      <c r="C99" s="29"/>
+      <c r="D99" s="30"/>
+      <c r="E99" s="30"/>
+      <c r="F99" s="31"/>
+      <c r="G99" s="31"/>
+      <c r="H99" s="26"/>
+      <c r="I99" s="1"/>
+      <c r="J99" s="1"/>
+      <c r="K99" s="1"/>
+    </row>
+    <row r="100" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
+      <c r="J100" s="1"/>
+      <c r="K100" s="1"/>
+    </row>
+    <row r="101" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
+      <c r="J101" s="1"/>
+      <c r="K101" s="1"/>
+    </row>
+    <row r="102" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
+      <c r="C102" s="25"/>
+      <c r="D102" s="25"/>
+      <c r="E102" s="25"/>
+      <c r="F102" s="25"/>
+      <c r="G102" s="25"/>
+      <c r="H102" s="25"/>
+      <c r="I102" s="25"/>
+      <c r="J102" s="1"/>
+      <c r="K102" s="1"/>
+    </row>
+    <row r="103" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+      <c r="C103" s="25"/>
+      <c r="D103" s="25"/>
+      <c r="E103" s="25"/>
+      <c r="F103" s="25"/>
+      <c r="G103" s="25"/>
+      <c r="H103" s="25"/>
+      <c r="I103" s="25"/>
+      <c r="J103" s="1"/>
+      <c r="K103" s="1"/>
+    </row>
+    <row r="104" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="25"/>
+      <c r="D104" s="25"/>
+      <c r="E104" s="25"/>
+      <c r="F104" s="25"/>
+      <c r="G104" s="25"/>
+      <c r="H104" s="25"/>
+      <c r="I104" s="25"/>
+      <c r="J104" s="1"/>
+      <c r="K104" s="1"/>
+    </row>
+    <row r="105" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+      <c r="C105" s="25"/>
+      <c r="D105" s="25"/>
+      <c r="E105" s="25"/>
+      <c r="F105" s="25"/>
+      <c r="G105" s="25"/>
+      <c r="H105" s="25"/>
+      <c r="I105" s="25"/>
+      <c r="J105" s="1"/>
+      <c r="K105" s="1"/>
+    </row>
+    <row r="106" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
+      <c r="C106" s="25"/>
+      <c r="D106" s="25"/>
+      <c r="E106" s="25"/>
+      <c r="F106" s="25"/>
+      <c r="G106" s="25"/>
+      <c r="H106" s="25"/>
+      <c r="I106" s="25"/>
+      <c r="J106" s="1"/>
+      <c r="K106" s="1"/>
+    </row>
+    <row r="107" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+      <c r="C107" s="25"/>
+      <c r="D107" s="25"/>
+      <c r="E107" s="25"/>
+      <c r="F107" s="25"/>
+      <c r="G107" s="25"/>
+      <c r="H107" s="25"/>
+      <c r="I107" s="25"/>
+      <c r="J107" s="1"/>
+      <c r="K107" s="1"/>
+    </row>
+    <row r="108" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A108" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B85" s="3"/>
-      <c r="C85" s="3"/>
-      <c r="D85" s="3"/>
-      <c r="E85" s="58" t="s">
+      <c r="B108" s="3"/>
+      <c r="C108" s="3"/>
+      <c r="D108" s="3"/>
+      <c r="E108" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="F85" s="59"/>
-      <c r="G85" s="60"/>
-      <c r="H85" s="61" t="s">
+      <c r="F108" s="63"/>
+      <c r="G108" s="64"/>
+      <c r="H108" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="I85" s="62"/>
-      <c r="J85" s="65"/>
-      <c r="K85" s="66"/>
-    </row>
-    <row r="86" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="36" t="s">
+      <c r="I108" s="66"/>
+      <c r="J108" s="69"/>
+      <c r="K108" s="70"/>
+    </row>
+    <row r="109" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A109" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B86" s="37"/>
-      <c r="C86" s="37"/>
-      <c r="D86" s="38"/>
-      <c r="E86" s="39">
+      <c r="B109" s="40"/>
+      <c r="C109" s="40"/>
+      <c r="D109" s="41"/>
+      <c r="E109" s="42">
         <v>152</v>
       </c>
-      <c r="F86" s="40"/>
-      <c r="G86" s="41"/>
-      <c r="H86" s="63"/>
-      <c r="I86" s="64"/>
-      <c r="J86" s="67"/>
-      <c r="K86" s="68"/>
+      <c r="F109" s="43"/>
+      <c r="G109" s="44"/>
+      <c r="H109" s="67"/>
+      <c r="I109" s="68"/>
+      <c r="J109" s="71"/>
+      <c r="K109" s="72"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A86:D86"/>
-    <mergeCell ref="E86:G86"/>
+  <mergeCells count="21">
+    <mergeCell ref="A68:K69"/>
+    <mergeCell ref="A70:K73"/>
+    <mergeCell ref="C75:I77"/>
+    <mergeCell ref="E108:G108"/>
+    <mergeCell ref="H108:I109"/>
+    <mergeCell ref="J108:K109"/>
+    <mergeCell ref="A109:D109"/>
+    <mergeCell ref="E109:G109"/>
+    <mergeCell ref="A67:D67"/>
+    <mergeCell ref="E67:G67"/>
     <mergeCell ref="C8:I10"/>
     <mergeCell ref="A3:K6"/>
     <mergeCell ref="A1:K2"/>
     <mergeCell ref="F33:F51"/>
     <mergeCell ref="G33:G51"/>
-    <mergeCell ref="C75:I76"/>
-    <mergeCell ref="F54:F73"/>
-    <mergeCell ref="G54:G73"/>
-    <mergeCell ref="E85:G85"/>
-    <mergeCell ref="H85:I86"/>
-    <mergeCell ref="J85:K86"/>
+    <mergeCell ref="C54:I55"/>
+    <mergeCell ref="F81:F95"/>
+    <mergeCell ref="G81:G95"/>
+    <mergeCell ref="E66:G66"/>
+    <mergeCell ref="H66:I67"/>
+    <mergeCell ref="J66:K67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="60" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
kati 2 njesite done
</commit_message>
<xml_diff>
--- a/5-Njësite-banesore/regjistri/22-Koordinatat-për-pjesë-të-ndertesës.xlsx-2602-0-Albnori.xlsx
+++ b/5-Njësite-banesore/regjistri/22-Koordinatat-për-pjesë-të-ndertesës.xlsx-2602-0-Albnori.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$109</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$130</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="24">
   <si>
     <t>Nr</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>Hyrje</t>
+  </si>
+  <si>
+    <t>KATI2</t>
   </si>
 </sst>
 </file>
@@ -591,7 +594,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -650,9 +653,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1744,10 +1744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K109"/>
+  <dimension ref="A1:K130"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A81" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="U80" sqref="U80"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A65" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="W74" sqref="W74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1763,112 +1763,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55"/>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
+      <c r="A1" s="54"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
     </row>
     <row r="2" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="55"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
+      <c r="A2" s="54"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
     </row>
     <row r="4" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="54"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
+      <c r="A4" s="53"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="54"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="54"/>
-      <c r="K5" s="54"/>
+      <c r="A5" s="53"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53"/>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="54"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
+      <c r="A6" s="53"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="45"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="47"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="46"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="48"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="50"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="49"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="51"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="53"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="52"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
@@ -1987,278 +1987,278 @@
       </c>
     </row>
     <row r="18" spans="3:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C18" s="32">
+      <c r="C18" s="31">
         <v>11</v>
       </c>
-      <c r="D18" s="33">
+      <c r="D18" s="32">
         <v>7513130.5959999999</v>
       </c>
-      <c r="E18" s="33">
+      <c r="E18" s="32">
         <v>4691713.7060000002</v>
       </c>
-      <c r="F18" s="33">
+      <c r="F18" s="32">
         <v>620.11199999999997</v>
       </c>
-      <c r="G18" s="34">
+      <c r="G18" s="33">
         <v>40</v>
       </c>
-      <c r="H18" s="34" t="s">
+      <c r="H18" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I18" s="35" t="s">
+      <c r="I18" s="34" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="3:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C19" s="32">
+      <c r="C19" s="31">
         <v>12</v>
       </c>
-      <c r="D19" s="33">
+      <c r="D19" s="32">
         <v>7513129.4539999999</v>
       </c>
-      <c r="E19" s="33">
+      <c r="E19" s="32">
         <v>4691712.6560000004</v>
       </c>
-      <c r="F19" s="33">
+      <c r="F19" s="32">
         <v>620.11199999999997</v>
       </c>
-      <c r="G19" s="34">
+      <c r="G19" s="33">
         <v>40</v>
       </c>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I19" s="35" t="s">
+      <c r="I19" s="34" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="20" spans="3:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C20" s="32">
+      <c r="C20" s="31">
         <v>13</v>
       </c>
-      <c r="D20" s="33">
+      <c r="D20" s="32">
         <v>7513129.1720000003</v>
       </c>
-      <c r="E20" s="33">
+      <c r="E20" s="32">
         <v>4691712.0049999999</v>
       </c>
-      <c r="F20" s="33">
+      <c r="F20" s="32">
         <v>620.11199999999997</v>
       </c>
-      <c r="G20" s="34">
+      <c r="G20" s="33">
         <v>40</v>
       </c>
-      <c r="H20" s="34" t="s">
+      <c r="H20" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I20" s="35" t="s">
+      <c r="I20" s="34" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="3:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C21" s="32">
+      <c r="C21" s="31">
         <v>14</v>
       </c>
-      <c r="D21" s="33">
+      <c r="D21" s="32">
         <v>7513129.6200000001</v>
       </c>
-      <c r="E21" s="33">
+      <c r="E21" s="32">
         <v>4691710.9950000001</v>
       </c>
-      <c r="F21" s="33">
+      <c r="F21" s="32">
         <v>620.11199999999997</v>
       </c>
-      <c r="G21" s="34">
+      <c r="G21" s="33">
         <v>40</v>
       </c>
-      <c r="H21" s="34" t="s">
+      <c r="H21" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I21" s="35" t="s">
+      <c r="I21" s="34" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="22" spans="3:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C22" s="32">
+      <c r="C22" s="31">
         <v>15</v>
       </c>
-      <c r="D22" s="33">
+      <c r="D22" s="32">
         <v>7513132.6849999996</v>
       </c>
-      <c r="E22" s="33">
+      <c r="E22" s="32">
         <v>4691707.6550000003</v>
       </c>
-      <c r="F22" s="33">
+      <c r="F22" s="32">
         <v>620.11199999999997</v>
       </c>
-      <c r="G22" s="34">
+      <c r="G22" s="33">
         <v>40</v>
       </c>
-      <c r="H22" s="34" t="s">
+      <c r="H22" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I22" s="35" t="s">
+      <c r="I22" s="34" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="3:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C23" s="32">
+      <c r="C23" s="31">
         <v>65</v>
       </c>
-      <c r="D23" s="33">
+      <c r="D23" s="32">
         <v>7513134.1550000003</v>
       </c>
-      <c r="E23" s="33">
+      <c r="E23" s="32">
         <v>4691707.0219999999</v>
       </c>
-      <c r="F23" s="33">
+      <c r="F23" s="32">
         <v>620.11199999999997</v>
       </c>
-      <c r="G23" s="34">
+      <c r="G23" s="33">
         <v>40</v>
       </c>
-      <c r="H23" s="34" t="s">
+      <c r="H23" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I23" s="35" t="s">
+      <c r="I23" s="34" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="24" spans="3:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C24" s="32">
+      <c r="C24" s="31">
         <v>67</v>
       </c>
-      <c r="D24" s="33">
+      <c r="D24" s="32">
         <v>7513135.8569999998</v>
       </c>
-      <c r="E24" s="33">
+      <c r="E24" s="32">
         <v>4691707.7450000001</v>
       </c>
-      <c r="F24" s="33">
+      <c r="F24" s="32">
         <v>620.11199999999997</v>
       </c>
-      <c r="G24" s="34">
+      <c r="G24" s="33">
         <v>40</v>
       </c>
-      <c r="H24" s="34" t="s">
+      <c r="H24" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I24" s="35" t="s">
+      <c r="I24" s="34" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="25" spans="3:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C25" s="32">
+      <c r="C25" s="31">
         <v>68</v>
       </c>
-      <c r="D25" s="33">
+      <c r="D25" s="32">
         <v>7513143.2529999996</v>
       </c>
-      <c r="E25" s="33">
+      <c r="E25" s="32">
         <v>4691714.4639999997</v>
       </c>
-      <c r="F25" s="33">
+      <c r="F25" s="32">
         <v>620.11199999999997</v>
       </c>
-      <c r="G25" s="34">
+      <c r="G25" s="33">
         <v>40</v>
       </c>
-      <c r="H25" s="34" t="s">
+      <c r="H25" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I25" s="35" t="s">
+      <c r="I25" s="34" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="26" spans="3:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C26" s="32">
-        <v>8</v>
-      </c>
-      <c r="D26" s="33">
+      <c r="C26" s="31">
+        <v>8</v>
+      </c>
+      <c r="D26" s="32">
         <v>7513128.7640000004</v>
       </c>
-      <c r="E26" s="33">
+      <c r="E26" s="32">
         <v>4691715.8310000002</v>
       </c>
-      <c r="F26" s="33">
+      <c r="F26" s="32">
         <v>620.11199999999997</v>
       </c>
-      <c r="G26" s="34">
+      <c r="G26" s="33">
         <v>40</v>
       </c>
-      <c r="H26" s="34" t="s">
+      <c r="H26" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I26" s="35" t="s">
+      <c r="I26" s="34" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="27" spans="3:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C27" s="32">
+      <c r="C27" s="31">
         <v>9</v>
       </c>
-      <c r="D27" s="33">
+      <c r="D27" s="32">
         <v>7513126.8399999999</v>
       </c>
-      <c r="E27" s="33">
+      <c r="E27" s="32">
         <v>4691714.1189999999</v>
       </c>
-      <c r="F27" s="33">
+      <c r="F27" s="32">
         <v>620.11199999999997</v>
       </c>
-      <c r="G27" s="34">
+      <c r="G27" s="33">
         <v>40</v>
       </c>
-      <c r="H27" s="34" t="s">
+      <c r="H27" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I27" s="35" t="s">
+      <c r="I27" s="34" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="28" spans="3:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C28" s="32">
+      <c r="C28" s="31">
         <v>10</v>
       </c>
-      <c r="D28" s="33">
+      <c r="D28" s="32">
         <v>7513129.2566</v>
       </c>
-      <c r="E28" s="33">
+      <c r="E28" s="32">
         <v>4691711.4588000001</v>
       </c>
-      <c r="F28" s="33">
+      <c r="F28" s="32">
         <v>620.11199999999997</v>
       </c>
-      <c r="G28" s="34">
+      <c r="G28" s="33">
         <v>40</v>
       </c>
-      <c r="H28" s="34" t="s">
+      <c r="H28" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I28" s="35" t="s">
+      <c r="I28" s="34" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="29" spans="3:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C29" s="32">
+      <c r="C29" s="31">
         <v>98</v>
       </c>
-      <c r="D29" s="33">
+      <c r="D29" s="32">
         <v>7513129.7910000002</v>
       </c>
-      <c r="E29" s="33">
+      <c r="E29" s="32">
         <v>4691714.6054999996</v>
       </c>
-      <c r="F29" s="33">
+      <c r="F29" s="32">
         <v>620.11199999999997</v>
       </c>
-      <c r="G29" s="34">
+      <c r="G29" s="33">
         <v>40</v>
       </c>
-      <c r="H29" s="34" t="s">
+      <c r="H29" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I29" s="35" t="s">
+      <c r="I29" s="34" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2319,10 +2319,10 @@
       <c r="E33" s="4">
         <v>4691722.8739999998</v>
       </c>
-      <c r="F33" s="56">
+      <c r="F33" s="55">
         <v>620.11199999999997</v>
       </c>
-      <c r="G33" s="56" t="s">
+      <c r="G33" s="55" t="s">
         <v>11</v>
       </c>
       <c r="H33" s="11" t="s">
@@ -2340,8 +2340,8 @@
       <c r="E34" s="4">
         <v>4691720.0990000004</v>
       </c>
-      <c r="F34" s="56"/>
-      <c r="G34" s="56"/>
+      <c r="F34" s="55"/>
+      <c r="G34" s="55"/>
       <c r="H34" s="11" t="s">
         <v>8</v>
       </c>
@@ -2357,8 +2357,8 @@
       <c r="E35" s="4">
         <v>4691719.3229999999</v>
       </c>
-      <c r="F35" s="56"/>
-      <c r="G35" s="56"/>
+      <c r="F35" s="55"/>
+      <c r="G35" s="55"/>
       <c r="H35" s="11" t="s">
         <v>8</v>
       </c>
@@ -2374,8 +2374,8 @@
       <c r="E36" s="4">
         <v>4691715.5049999999</v>
       </c>
-      <c r="F36" s="56"/>
-      <c r="G36" s="56"/>
+      <c r="F36" s="55"/>
+      <c r="G36" s="55"/>
       <c r="H36" s="11" t="s">
         <v>8</v>
       </c>
@@ -2391,8 +2391,8 @@
       <c r="E37" s="4">
         <v>4691715.8310000002</v>
       </c>
-      <c r="F37" s="56"/>
-      <c r="G37" s="56"/>
+      <c r="F37" s="55"/>
+      <c r="G37" s="55"/>
       <c r="H37" s="11" t="s">
         <v>8</v>
       </c>
@@ -2409,8 +2409,8 @@
       <c r="E38" s="4">
         <v>4691714.1189999999</v>
       </c>
-      <c r="F38" s="56"/>
-      <c r="G38" s="56"/>
+      <c r="F38" s="55"/>
+      <c r="G38" s="55"/>
       <c r="H38" s="11" t="s">
         <v>8</v>
       </c>
@@ -2428,8 +2428,8 @@
       <c r="E39" s="4">
         <v>4691711.4588000001</v>
       </c>
-      <c r="F39" s="56"/>
-      <c r="G39" s="56"/>
+      <c r="F39" s="55"/>
+      <c r="G39" s="55"/>
       <c r="H39" s="11" t="s">
         <v>8</v>
       </c>
@@ -2447,8 +2447,8 @@
       <c r="E40" s="4">
         <v>4691713.7060000002</v>
       </c>
-      <c r="F40" s="56"/>
-      <c r="G40" s="56"/>
+      <c r="F40" s="55"/>
+      <c r="G40" s="55"/>
       <c r="H40" s="11" t="s">
         <v>8</v>
       </c>
@@ -2457,18 +2457,18 @@
     </row>
     <row r="41" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
-      <c r="C41" s="36">
+      <c r="C41" s="35">
         <v>12</v>
       </c>
-      <c r="D41" s="37">
+      <c r="D41" s="36">
         <v>7513129.4539999999</v>
       </c>
-      <c r="E41" s="37">
+      <c r="E41" s="36">
         <v>4691712.6560000004</v>
       </c>
-      <c r="F41" s="57"/>
-      <c r="G41" s="57"/>
-      <c r="H41" s="38" t="s">
+      <c r="F41" s="56"/>
+      <c r="G41" s="56"/>
+      <c r="H41" s="37" t="s">
         <v>8</v>
       </c>
       <c r="I41" s="10"/>
@@ -2476,18 +2476,18 @@
     </row>
     <row r="42" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
-      <c r="C42" s="36">
+      <c r="C42" s="35">
         <v>13</v>
       </c>
-      <c r="D42" s="37">
+      <c r="D42" s="36">
         <v>7513129.1720000003</v>
       </c>
-      <c r="E42" s="37">
+      <c r="E42" s="36">
         <v>4691712.0049999999</v>
       </c>
-      <c r="F42" s="57"/>
-      <c r="G42" s="57"/>
-      <c r="H42" s="38" t="s">
+      <c r="F42" s="56"/>
+      <c r="G42" s="56"/>
+      <c r="H42" s="37" t="s">
         <v>8</v>
       </c>
       <c r="I42" s="10"/>
@@ -2495,18 +2495,18 @@
     </row>
     <row r="43" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
-      <c r="C43" s="36">
+      <c r="C43" s="35">
         <v>14</v>
       </c>
-      <c r="D43" s="37">
+      <c r="D43" s="36">
         <v>7513129.6200000001</v>
       </c>
-      <c r="E43" s="37">
+      <c r="E43" s="36">
         <v>4691710.9950000001</v>
       </c>
-      <c r="F43" s="57"/>
-      <c r="G43" s="57"/>
-      <c r="H43" s="38" t="s">
+      <c r="F43" s="56"/>
+      <c r="G43" s="56"/>
+      <c r="H43" s="37" t="s">
         <v>8</v>
       </c>
       <c r="I43" s="10"/>
@@ -2514,18 +2514,18 @@
     </row>
     <row r="44" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
-      <c r="C44" s="36">
+      <c r="C44" s="35">
         <v>15</v>
       </c>
-      <c r="D44" s="37">
+      <c r="D44" s="36">
         <v>7513132.6849999996</v>
       </c>
-      <c r="E44" s="37">
+      <c r="E44" s="36">
         <v>4691707.6550000003</v>
       </c>
-      <c r="F44" s="57"/>
-      <c r="G44" s="57"/>
-      <c r="H44" s="38" t="s">
+      <c r="F44" s="56"/>
+      <c r="G44" s="56"/>
+      <c r="H44" s="37" t="s">
         <v>8</v>
       </c>
       <c r="I44" s="10"/>
@@ -2533,18 +2533,18 @@
     </row>
     <row r="45" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
-      <c r="C45" s="36">
+      <c r="C45" s="35">
         <v>65</v>
       </c>
-      <c r="D45" s="37">
+      <c r="D45" s="36">
         <v>7513134.1550000003</v>
       </c>
-      <c r="E45" s="37">
+      <c r="E45" s="36">
         <v>4691707.0219999999</v>
       </c>
-      <c r="F45" s="57"/>
-      <c r="G45" s="57"/>
-      <c r="H45" s="38" t="s">
+      <c r="F45" s="56"/>
+      <c r="G45" s="56"/>
+      <c r="H45" s="37" t="s">
         <v>8</v>
       </c>
       <c r="I45" s="10"/>
@@ -2552,18 +2552,18 @@
     </row>
     <row r="46" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
-      <c r="C46" s="36">
+      <c r="C46" s="35">
         <v>67</v>
       </c>
-      <c r="D46" s="37">
+      <c r="D46" s="36">
         <v>7513135.8569999998</v>
       </c>
-      <c r="E46" s="37">
+      <c r="E46" s="36">
         <v>4691707.7450000001</v>
       </c>
-      <c r="F46" s="57"/>
-      <c r="G46" s="57"/>
-      <c r="H46" s="38" t="s">
+      <c r="F46" s="56"/>
+      <c r="G46" s="56"/>
+      <c r="H46" s="37" t="s">
         <v>8</v>
       </c>
       <c r="I46" s="10"/>
@@ -2571,18 +2571,18 @@
     </row>
     <row r="47" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
-      <c r="C47" s="36">
+      <c r="C47" s="35">
         <v>68</v>
       </c>
-      <c r="D47" s="37">
+      <c r="D47" s="36">
         <v>7513143.2529999996</v>
       </c>
-      <c r="E47" s="37">
+      <c r="E47" s="36">
         <v>4691714.4639999997</v>
       </c>
-      <c r="F47" s="57"/>
-      <c r="G47" s="57"/>
-      <c r="H47" s="38" t="s">
+      <c r="F47" s="56"/>
+      <c r="G47" s="56"/>
+      <c r="H47" s="37" t="s">
         <v>8</v>
       </c>
       <c r="I47" s="10"/>
@@ -2590,18 +2590,18 @@
     </row>
     <row r="48" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
-      <c r="C48" s="36">
+      <c r="C48" s="35">
         <v>101</v>
       </c>
-      <c r="D48" s="37">
+      <c r="D48" s="36">
         <v>7513132.5939999996</v>
       </c>
-      <c r="E48" s="37">
+      <c r="E48" s="36">
         <v>4691715.5387000004</v>
       </c>
-      <c r="F48" s="57"/>
-      <c r="G48" s="57"/>
-      <c r="H48" s="38" t="s">
+      <c r="F48" s="56"/>
+      <c r="G48" s="56"/>
+      <c r="H48" s="37" t="s">
         <v>8</v>
       </c>
       <c r="I48" s="10"/>
@@ -2609,18 +2609,18 @@
     </row>
     <row r="49" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
-      <c r="C49" s="36">
+      <c r="C49" s="35">
         <v>102</v>
       </c>
-      <c r="D49" s="37">
+      <c r="D49" s="36">
         <v>7513131.9008999998</v>
       </c>
-      <c r="E49" s="37">
+      <c r="E49" s="36">
         <v>4691716.2944</v>
       </c>
-      <c r="F49" s="57"/>
-      <c r="G49" s="57"/>
-      <c r="H49" s="38" t="s">
+      <c r="F49" s="56"/>
+      <c r="G49" s="56"/>
+      <c r="H49" s="37" t="s">
         <v>8</v>
       </c>
       <c r="I49" s="10"/>
@@ -2628,18 +2628,18 @@
     </row>
     <row r="50" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
-      <c r="C50" s="36">
+      <c r="C50" s="35">
         <v>103</v>
       </c>
-      <c r="D50" s="37">
+      <c r="D50" s="36">
         <v>7513132.1218999997</v>
       </c>
-      <c r="E50" s="37">
+      <c r="E50" s="36">
         <v>4691716.4972000001</v>
       </c>
-      <c r="F50" s="57"/>
-      <c r="G50" s="57"/>
-      <c r="H50" s="38" t="s">
+      <c r="F50" s="56"/>
+      <c r="G50" s="56"/>
+      <c r="H50" s="37" t="s">
         <v>8</v>
       </c>
       <c r="I50" s="10"/>
@@ -2657,8 +2657,8 @@
       <c r="E51" s="7">
         <v>4691717.4923</v>
       </c>
-      <c r="F51" s="58"/>
-      <c r="G51" s="58"/>
+      <c r="F51" s="57"/>
+      <c r="G51" s="57"/>
       <c r="H51" s="12" t="s">
         <v>8</v>
       </c>
@@ -2680,28 +2680,28 @@
     <row r="54" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
-      <c r="C54" s="59" t="s">
+      <c r="C54" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="D54" s="59"/>
-      <c r="E54" s="59"/>
-      <c r="F54" s="59"/>
-      <c r="G54" s="59"/>
-      <c r="H54" s="59"/>
-      <c r="I54" s="59"/>
+      <c r="D54" s="58"/>
+      <c r="E54" s="58"/>
+      <c r="F54" s="58"/>
+      <c r="G54" s="58"/>
+      <c r="H54" s="58"/>
+      <c r="I54" s="58"/>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
     </row>
     <row r="55" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
-      <c r="C55" s="59"/>
-      <c r="D55" s="59"/>
-      <c r="E55" s="59"/>
-      <c r="F55" s="59"/>
-      <c r="G55" s="59"/>
-      <c r="H55" s="59"/>
-      <c r="I55" s="59"/>
+      <c r="C55" s="58"/>
+      <c r="D55" s="58"/>
+      <c r="E55" s="58"/>
+      <c r="F55" s="58"/>
+      <c r="G55" s="58"/>
+      <c r="H55" s="58"/>
+      <c r="I55" s="58"/>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
     </row>
@@ -2772,182 +2772,199 @@
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
-      <c r="E66" s="62" t="s">
+      <c r="E66" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="F66" s="63"/>
-      <c r="G66" s="64"/>
-      <c r="H66" s="65" t="s">
+      <c r="F66" s="62"/>
+      <c r="G66" s="63"/>
+      <c r="H66" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="I66" s="66"/>
-      <c r="J66" s="69"/>
-      <c r="K66" s="70"/>
+      <c r="I66" s="65"/>
+      <c r="J66" s="68"/>
+      <c r="K66" s="69"/>
     </row>
     <row r="67" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="39" t="s">
+      <c r="A67" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B67" s="40"/>
-      <c r="C67" s="40"/>
-      <c r="D67" s="41"/>
-      <c r="E67" s="42">
+      <c r="B67" s="39"/>
+      <c r="C67" s="39"/>
+      <c r="D67" s="40"/>
+      <c r="E67" s="41">
         <v>152</v>
       </c>
-      <c r="F67" s="43"/>
-      <c r="G67" s="44"/>
-      <c r="H67" s="67"/>
-      <c r="I67" s="68"/>
-      <c r="J67" s="71"/>
-      <c r="K67" s="72"/>
+      <c r="F67" s="42"/>
+      <c r="G67" s="43"/>
+      <c r="H67" s="66"/>
+      <c r="I67" s="67"/>
+      <c r="J67" s="70"/>
+      <c r="K67" s="71"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="55"/>
-      <c r="B68" s="55"/>
-      <c r="C68" s="55"/>
-      <c r="D68" s="55"/>
-      <c r="E68" s="55"/>
-      <c r="F68" s="55"/>
-      <c r="G68" s="55"/>
-      <c r="H68" s="55"/>
-      <c r="I68" s="55"/>
-      <c r="J68" s="55"/>
-      <c r="K68" s="55"/>
+      <c r="A68" s="54"/>
+      <c r="B68" s="54"/>
+      <c r="C68" s="54"/>
+      <c r="D68" s="54"/>
+      <c r="E68" s="54"/>
+      <c r="F68" s="54"/>
+      <c r="G68" s="54"/>
+      <c r="H68" s="54"/>
+      <c r="I68" s="54"/>
+      <c r="J68" s="54"/>
+      <c r="K68" s="54"/>
     </row>
     <row r="69" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="55"/>
-      <c r="B69" s="55"/>
-      <c r="C69" s="55"/>
-      <c r="D69" s="55"/>
-      <c r="E69" s="55"/>
-      <c r="F69" s="55"/>
-      <c r="G69" s="55"/>
-      <c r="H69" s="55"/>
-      <c r="I69" s="55"/>
-      <c r="J69" s="55"/>
-      <c r="K69" s="55"/>
+      <c r="A69" s="54"/>
+      <c r="B69" s="54"/>
+      <c r="C69" s="54"/>
+      <c r="D69" s="54"/>
+      <c r="E69" s="54"/>
+      <c r="F69" s="54"/>
+      <c r="G69" s="54"/>
+      <c r="H69" s="54"/>
+      <c r="I69" s="54"/>
+      <c r="J69" s="54"/>
+      <c r="K69" s="54"/>
     </row>
     <row r="70" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="54" t="s">
+      <c r="A70" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="B70" s="54"/>
-      <c r="C70" s="54"/>
-      <c r="D70" s="54"/>
-      <c r="E70" s="54"/>
-      <c r="F70" s="54"/>
-      <c r="G70" s="54"/>
-      <c r="H70" s="54"/>
-      <c r="I70" s="54"/>
-      <c r="J70" s="54"/>
-      <c r="K70" s="54"/>
+      <c r="B70" s="53"/>
+      <c r="C70" s="53"/>
+      <c r="D70" s="53"/>
+      <c r="E70" s="53"/>
+      <c r="F70" s="53"/>
+      <c r="G70" s="53"/>
+      <c r="H70" s="53"/>
+      <c r="I70" s="53"/>
+      <c r="J70" s="53"/>
+      <c r="K70" s="53"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="54"/>
-      <c r="B71" s="54"/>
-      <c r="C71" s="54"/>
-      <c r="D71" s="54"/>
-      <c r="E71" s="54"/>
-      <c r="F71" s="54"/>
-      <c r="G71" s="54"/>
-      <c r="H71" s="54"/>
-      <c r="I71" s="54"/>
-      <c r="J71" s="54"/>
-      <c r="K71" s="54"/>
+      <c r="A71" s="53"/>
+      <c r="B71" s="53"/>
+      <c r="C71" s="53"/>
+      <c r="D71" s="53"/>
+      <c r="E71" s="53"/>
+      <c r="F71" s="53"/>
+      <c r="G71" s="53"/>
+      <c r="H71" s="53"/>
+      <c r="I71" s="53"/>
+      <c r="J71" s="53"/>
+      <c r="K71" s="53"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" s="54"/>
-      <c r="B72" s="54"/>
-      <c r="C72" s="54"/>
-      <c r="D72" s="54"/>
-      <c r="E72" s="54"/>
-      <c r="F72" s="54"/>
-      <c r="G72" s="54"/>
-      <c r="H72" s="54"/>
-      <c r="I72" s="54"/>
-      <c r="J72" s="54"/>
-      <c r="K72" s="54"/>
+      <c r="A72" s="53"/>
+      <c r="B72" s="53"/>
+      <c r="C72" s="53"/>
+      <c r="D72" s="53"/>
+      <c r="E72" s="53"/>
+      <c r="F72" s="53"/>
+      <c r="G72" s="53"/>
+      <c r="H72" s="53"/>
+      <c r="I72" s="53"/>
+      <c r="J72" s="53"/>
+      <c r="K72" s="53"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A73" s="54"/>
-      <c r="B73" s="54"/>
-      <c r="C73" s="54"/>
-      <c r="D73" s="54"/>
-      <c r="E73" s="54"/>
-      <c r="F73" s="54"/>
-      <c r="G73" s="54"/>
-      <c r="H73" s="54"/>
-      <c r="I73" s="54"/>
-      <c r="J73" s="54"/>
-      <c r="K73" s="54"/>
+      <c r="A73" s="53"/>
+      <c r="B73" s="53"/>
+      <c r="C73" s="53"/>
+      <c r="D73" s="53"/>
+      <c r="E73" s="53"/>
+      <c r="F73" s="53"/>
+      <c r="G73" s="53"/>
+      <c r="H73" s="53"/>
+      <c r="I73" s="53"/>
+      <c r="J73" s="53"/>
+      <c r="K73" s="53"/>
     </row>
     <row r="74" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C75" s="45"/>
-      <c r="D75" s="46"/>
-      <c r="E75" s="46"/>
-      <c r="F75" s="46"/>
-      <c r="G75" s="46"/>
-      <c r="H75" s="46"/>
-      <c r="I75" s="47"/>
+      <c r="C75" s="44"/>
+      <c r="D75" s="45"/>
+      <c r="E75" s="45"/>
+      <c r="F75" s="45"/>
+      <c r="G75" s="45"/>
+      <c r="H75" s="45"/>
+      <c r="I75" s="46"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C76" s="48"/>
-      <c r="D76" s="49"/>
-      <c r="E76" s="49"/>
-      <c r="F76" s="49"/>
-      <c r="G76" s="49"/>
-      <c r="H76" s="49"/>
-      <c r="I76" s="50"/>
+      <c r="C76" s="47"/>
+      <c r="D76" s="48"/>
+      <c r="E76" s="48"/>
+      <c r="F76" s="48"/>
+      <c r="G76" s="48"/>
+      <c r="H76" s="48"/>
+      <c r="I76" s="49"/>
     </row>
     <row r="77" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C77" s="51"/>
-      <c r="D77" s="52"/>
-      <c r="E77" s="52"/>
-      <c r="F77" s="52"/>
-      <c r="G77" s="52"/>
-      <c r="H77" s="52"/>
-      <c r="I77" s="53"/>
-    </row>
-    <row r="78" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C77" s="50"/>
+      <c r="D77" s="51"/>
+      <c r="E77" s="51"/>
+      <c r="F77" s="51"/>
+      <c r="G77" s="51"/>
+      <c r="H77" s="51"/>
+      <c r="I77" s="52"/>
+    </row>
+    <row r="78" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
-      <c r="C78" s="29"/>
-      <c r="D78" s="30"/>
-      <c r="E78" s="30"/>
-      <c r="F78" s="31"/>
-      <c r="G78" s="31"/>
-      <c r="H78" s="26"/>
+      <c r="C78" s="28"/>
+      <c r="D78" s="29"/>
+      <c r="E78" s="29"/>
+      <c r="F78" s="30"/>
+      <c r="G78" s="30"/>
+      <c r="H78" s="25"/>
       <c r="I78" s="1"/>
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
     </row>
-    <row r="79" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
-      <c r="H79" s="26"/>
+      <c r="C79" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D79" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E79" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F79" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G79" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H79" s="13" t="s">
+        <v>3</v>
+      </c>
       <c r="I79" s="1"/>
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
     </row>
     <row r="80" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
-      <c r="C80" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D80" s="9" t="s">
+      <c r="C80" s="5">
         <v>1</v>
       </c>
-      <c r="E80" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F80" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G80" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H80" s="13" t="s">
-        <v>3</v>
+      <c r="D80" s="4">
+        <v>7513135.568</v>
+      </c>
+      <c r="E80" s="4">
+        <v>4691722.8739999998</v>
+      </c>
+      <c r="F80" s="59">
+        <v>623.17399999999998</v>
+      </c>
+      <c r="G80" s="59" t="s">
+        <v>20</v>
+      </c>
+      <c r="H80" s="26" t="s">
+        <v>8</v>
       </c>
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
@@ -2956,21 +2973,17 @@
     <row r="81" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="C81" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D81" s="4">
-        <v>7513135.568</v>
+        <v>7513132.5010000002</v>
       </c>
       <c r="E81" s="4">
-        <v>4691722.8739999998</v>
-      </c>
-      <c r="F81" s="60">
-        <v>623.17399999999998</v>
-      </c>
-      <c r="G81" s="60" t="s">
-        <v>20</v>
-      </c>
-      <c r="H81" s="27" t="s">
+        <v>4691720.0990000004</v>
+      </c>
+      <c r="F81" s="59"/>
+      <c r="G81" s="59"/>
+      <c r="H81" s="26" t="s">
         <v>8</v>
       </c>
       <c r="I81" s="1"/>
@@ -2980,17 +2993,17 @@
     <row r="82" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="C82" s="5">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D82" s="4">
-        <v>7513132.5010000002</v>
+        <v>7513128.9859999996</v>
       </c>
       <c r="E82" s="4">
-        <v>4691720.0990000004</v>
-      </c>
-      <c r="F82" s="60"/>
-      <c r="G82" s="60"/>
-      <c r="H82" s="27" t="s">
+        <v>4691715.5049999999</v>
+      </c>
+      <c r="F82" s="59"/>
+      <c r="G82" s="59"/>
+      <c r="H82" s="26" t="s">
         <v>8</v>
       </c>
       <c r="I82" s="1"/>
@@ -3000,17 +3013,17 @@
     <row r="83" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
       <c r="C83" s="5">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D83" s="4">
-        <v>7513128.9859999996</v>
+        <v>7513133.25</v>
       </c>
       <c r="E83" s="4">
-        <v>4691715.5049999999</v>
-      </c>
-      <c r="F83" s="60"/>
-      <c r="G83" s="60"/>
-      <c r="H83" s="27" t="s">
+        <v>4691719.318</v>
+      </c>
+      <c r="F83" s="59"/>
+      <c r="G83" s="59"/>
+      <c r="H83" s="26" t="s">
         <v>8</v>
       </c>
       <c r="I83" s="1"/>
@@ -3020,17 +3033,17 @@
     <row r="84" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
       <c r="C84" s="5">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D84" s="4">
-        <v>7513133.25</v>
+        <v>7513127.2779999999</v>
       </c>
       <c r="E84" s="4">
-        <v>4691719.318</v>
-      </c>
-      <c r="F84" s="60"/>
-      <c r="G84" s="60"/>
-      <c r="H84" s="27" t="s">
+        <v>4691713.9479999999</v>
+      </c>
+      <c r="F84" s="59"/>
+      <c r="G84" s="59"/>
+      <c r="H84" s="26" t="s">
         <v>8</v>
       </c>
       <c r="I84" s="1"/>
@@ -3040,17 +3053,17 @@
     <row r="85" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="C85" s="5">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D85" s="4">
-        <v>7513127.2779999999</v>
+        <v>7513127.3820000002</v>
       </c>
       <c r="E85" s="4">
-        <v>4691713.9479999999</v>
-      </c>
-      <c r="F85" s="60"/>
-      <c r="G85" s="60"/>
-      <c r="H85" s="27" t="s">
+        <v>4691712.1909999996</v>
+      </c>
+      <c r="F85" s="59"/>
+      <c r="G85" s="59"/>
+      <c r="H85" s="26" t="s">
         <v>8</v>
       </c>
       <c r="I85" s="1"/>
@@ -3060,17 +3073,17 @@
     <row r="86" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
       <c r="C86" s="5">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D86" s="4">
-        <v>7513127.3820000002</v>
+        <v>7513128.142</v>
       </c>
       <c r="E86" s="4">
-        <v>4691712.1909999996</v>
-      </c>
-      <c r="F86" s="60"/>
-      <c r="G86" s="60"/>
-      <c r="H86" s="27" t="s">
+        <v>4691711.0889999997</v>
+      </c>
+      <c r="F86" s="59"/>
+      <c r="G86" s="59"/>
+      <c r="H86" s="26" t="s">
         <v>8</v>
       </c>
       <c r="I86" s="1"/>
@@ -3080,17 +3093,17 @@
     <row r="87" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
       <c r="C87" s="5">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D87" s="4">
-        <v>7513128.142</v>
+        <v>7513132.0240000002</v>
       </c>
       <c r="E87" s="4">
-        <v>4691711.0889999997</v>
-      </c>
-      <c r="F87" s="60"/>
-      <c r="G87" s="60"/>
-      <c r="H87" s="27" t="s">
+        <v>4691706.8949999996</v>
+      </c>
+      <c r="F87" s="59"/>
+      <c r="G87" s="59"/>
+      <c r="H87" s="26" t="s">
         <v>8</v>
       </c>
       <c r="I87" s="1"/>
@@ -3100,17 +3113,17 @@
     <row r="88" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
       <c r="C88" s="5">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D88" s="4">
-        <v>7513132.0240000002</v>
+        <v>7513133.5190000003</v>
       </c>
       <c r="E88" s="4">
-        <v>4691706.8949999996</v>
-      </c>
-      <c r="F88" s="60"/>
-      <c r="G88" s="60"/>
-      <c r="H88" s="27" t="s">
+        <v>4691706.18</v>
+      </c>
+      <c r="F88" s="59"/>
+      <c r="G88" s="59"/>
+      <c r="H88" s="26" t="s">
         <v>8</v>
       </c>
       <c r="I88" s="1"/>
@@ -3120,17 +3133,17 @@
     <row r="89" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
       <c r="C89" s="5">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="D89" s="4">
-        <v>7513133.5190000003</v>
+        <v>7513134.1436999999</v>
       </c>
       <c r="E89" s="4">
-        <v>4691706.18</v>
-      </c>
-      <c r="F89" s="60"/>
-      <c r="G89" s="60"/>
-      <c r="H89" s="27" t="s">
+        <v>4691706.1939000003</v>
+      </c>
+      <c r="F89" s="59"/>
+      <c r="G89" s="59"/>
+      <c r="H89" s="26" t="s">
         <v>8</v>
       </c>
       <c r="I89" s="1"/>
@@ -3140,17 +3153,17 @@
     <row r="90" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
       <c r="C90" s="5">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D90" s="4">
-        <v>7513134.1436999999</v>
+        <v>7513135.8569999998</v>
       </c>
       <c r="E90" s="4">
-        <v>4691706.1939000003</v>
-      </c>
-      <c r="F90" s="60"/>
-      <c r="G90" s="60"/>
-      <c r="H90" s="27" t="s">
+        <v>4691707.7450000001</v>
+      </c>
+      <c r="F90" s="59"/>
+      <c r="G90" s="59"/>
+      <c r="H90" s="26" t="s">
         <v>8</v>
       </c>
       <c r="I90" s="1"/>
@@ -3160,17 +3173,17 @@
     <row r="91" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A91" s="1"/>
       <c r="C91" s="5">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D91" s="4">
-        <v>7513135.8569999998</v>
+        <v>7513143.2529999996</v>
       </c>
       <c r="E91" s="4">
-        <v>4691707.7450000001</v>
-      </c>
-      <c r="F91" s="60"/>
-      <c r="G91" s="60"/>
-      <c r="H91" s="27" t="s">
+        <v>4691714.4639999997</v>
+      </c>
+      <c r="F91" s="59"/>
+      <c r="G91" s="59"/>
+      <c r="H91" s="26" t="s">
         <v>8</v>
       </c>
       <c r="I91" s="1"/>
@@ -3180,17 +3193,17 @@
     <row r="92" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A92" s="1"/>
       <c r="C92" s="5">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="D92" s="4">
-        <v>7513143.2529999996</v>
+        <v>7513136.3592999997</v>
       </c>
       <c r="E92" s="4">
-        <v>4691714.4639999997</v>
-      </c>
-      <c r="F92" s="60"/>
-      <c r="G92" s="60"/>
-      <c r="H92" s="27" t="s">
+        <v>4691715.8525</v>
+      </c>
+      <c r="F92" s="59"/>
+      <c r="G92" s="59"/>
+      <c r="H92" s="26" t="s">
         <v>8</v>
       </c>
       <c r="I92" s="1"/>
@@ -3200,33 +3213,34 @@
     <row r="93" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A93" s="1"/>
       <c r="C93" s="5">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D93" s="4">
-        <v>7513136.3592999997</v>
+        <v>7513132.6316</v>
       </c>
       <c r="E93" s="4">
-        <v>4691715.8525</v>
-      </c>
-      <c r="F93" s="60"/>
-      <c r="G93" s="60"/>
-      <c r="H93" s="27" t="s">
+        <v>4691712.5202000001</v>
+      </c>
+      <c r="F93" s="59"/>
+      <c r="G93" s="59"/>
+      <c r="H93" s="26" t="s">
         <v>8</v>
       </c>
       <c r="I93" s="1"/>
       <c r="J93" s="1"/>
       <c r="K93" s="1"/>
     </row>
-    <row r="94" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="1"/>
-      <c r="C94" s="5">
-        <v>107</v>
-      </c>
-      <c r="D94" s="4">
-        <v>7513132.6316</v>
-      </c>
-      <c r="E94" s="4">
-        <v>4691712.5202000001</v>
+      <c r="B94" s="1"/>
+      <c r="C94" s="6">
+        <v>108</v>
+      </c>
+      <c r="D94" s="7">
+        <v>7513129.5292999996</v>
+      </c>
+      <c r="E94" s="7">
+        <v>4691715.9907</v>
       </c>
       <c r="F94" s="60"/>
       <c r="G94" s="60"/>
@@ -3240,20 +3254,12 @@
     <row r="95" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
-      <c r="C95" s="6">
-        <v>108</v>
-      </c>
-      <c r="D95" s="7">
-        <v>7513129.5292999996</v>
-      </c>
-      <c r="E95" s="7">
-        <v>4691715.9907</v>
-      </c>
-      <c r="F95" s="61"/>
-      <c r="G95" s="61"/>
-      <c r="H95" s="28" t="s">
-        <v>8</v>
-      </c>
+      <c r="C95" s="28"/>
+      <c r="D95" s="29"/>
+      <c r="E95" s="29"/>
+      <c r="F95" s="30"/>
+      <c r="G95" s="30"/>
+      <c r="H95" s="25"/>
       <c r="I95" s="1"/>
       <c r="J95" s="1"/>
       <c r="K95" s="1"/>
@@ -3261,12 +3267,24 @@
     <row r="96" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
-      <c r="C96" s="29"/>
-      <c r="D96" s="30"/>
-      <c r="E96" s="30"/>
-      <c r="F96" s="31"/>
-      <c r="G96" s="31"/>
-      <c r="H96" s="26"/>
+      <c r="C96" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D96" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E96" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F96" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G96" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H96" s="13" t="s">
+        <v>3</v>
+      </c>
       <c r="I96" s="1"/>
       <c r="J96" s="1"/>
       <c r="K96" s="1"/>
@@ -3274,12 +3292,24 @@
     <row r="97" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
-      <c r="C97" s="29"/>
-      <c r="D97" s="30"/>
-      <c r="E97" s="30"/>
-      <c r="F97" s="31"/>
-      <c r="G97" s="31"/>
-      <c r="H97" s="26"/>
+      <c r="C97" s="5">
+        <v>1</v>
+      </c>
+      <c r="D97" s="4">
+        <v>7513135.568</v>
+      </c>
+      <c r="E97" s="4">
+        <v>4691722.8739999998</v>
+      </c>
+      <c r="F97" s="59">
+        <v>626.09400000000005</v>
+      </c>
+      <c r="G97" s="59" t="s">
+        <v>23</v>
+      </c>
+      <c r="H97" s="26" t="s">
+        <v>8</v>
+      </c>
       <c r="I97" s="1"/>
       <c r="J97" s="1"/>
       <c r="K97" s="1"/>
@@ -3287,12 +3317,20 @@
     <row r="98" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
-      <c r="C98" s="29"/>
-      <c r="D98" s="30"/>
-      <c r="E98" s="30"/>
-      <c r="F98" s="31"/>
-      <c r="G98" s="31"/>
-      <c r="H98" s="26"/>
+      <c r="C98" s="5">
+        <v>2</v>
+      </c>
+      <c r="D98" s="4">
+        <v>7513132.5010000002</v>
+      </c>
+      <c r="E98" s="4">
+        <v>4691720.0990000004</v>
+      </c>
+      <c r="F98" s="59"/>
+      <c r="G98" s="59"/>
+      <c r="H98" s="26" t="s">
+        <v>8</v>
+      </c>
       <c r="I98" s="1"/>
       <c r="J98" s="1"/>
       <c r="K98" s="1"/>
@@ -3300,12 +3338,20 @@
     <row r="99" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
-      <c r="C99" s="29"/>
-      <c r="D99" s="30"/>
-      <c r="E99" s="30"/>
-      <c r="F99" s="31"/>
-      <c r="G99" s="31"/>
-      <c r="H99" s="26"/>
+      <c r="C99" s="5">
+        <v>7</v>
+      </c>
+      <c r="D99" s="4">
+        <v>7513128.9859999996</v>
+      </c>
+      <c r="E99" s="4">
+        <v>4691715.5049999999</v>
+      </c>
+      <c r="F99" s="59"/>
+      <c r="G99" s="59"/>
+      <c r="H99" s="26" t="s">
+        <v>8</v>
+      </c>
       <c r="I99" s="1"/>
       <c r="J99" s="1"/>
       <c r="K99" s="1"/>
@@ -3313,139 +3359,524 @@
     <row r="100" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
+      <c r="C100" s="5">
+        <v>23</v>
+      </c>
+      <c r="D100" s="4">
+        <v>7513133.25</v>
+      </c>
+      <c r="E100" s="4">
+        <v>4691719.318</v>
+      </c>
+      <c r="F100" s="59"/>
+      <c r="G100" s="59"/>
+      <c r="H100" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="I100" s="1"/>
       <c r="J100" s="1"/>
       <c r="K100" s="1"/>
     </row>
     <row r="101" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
+      <c r="C101" s="5">
+        <v>24</v>
+      </c>
+      <c r="D101" s="4">
+        <v>7513127.2779999999</v>
+      </c>
+      <c r="E101" s="4">
+        <v>4691713.9479999999</v>
+      </c>
+      <c r="F101" s="59"/>
+      <c r="G101" s="59"/>
+      <c r="H101" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="I101" s="1"/>
       <c r="J101" s="1"/>
       <c r="K101" s="1"/>
     </row>
     <row r="102" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
-      <c r="C102" s="25"/>
-      <c r="D102" s="25"/>
-      <c r="E102" s="25"/>
-      <c r="F102" s="25"/>
-      <c r="G102" s="25"/>
-      <c r="H102" s="25"/>
-      <c r="I102" s="25"/>
+      <c r="C102" s="5">
+        <v>25</v>
+      </c>
+      <c r="D102" s="4">
+        <v>7513127.3820000002</v>
+      </c>
+      <c r="E102" s="4">
+        <v>4691712.1909999996</v>
+      </c>
+      <c r="F102" s="59"/>
+      <c r="G102" s="59"/>
+      <c r="H102" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="I102" s="1"/>
       <c r="J102" s="1"/>
       <c r="K102" s="1"/>
     </row>
     <row r="103" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
-      <c r="C103" s="25"/>
-      <c r="D103" s="25"/>
-      <c r="E103" s="25"/>
-      <c r="F103" s="25"/>
-      <c r="G103" s="25"/>
-      <c r="H103" s="25"/>
-      <c r="I103" s="25"/>
+      <c r="C103" s="5">
+        <v>26</v>
+      </c>
+      <c r="D103" s="4">
+        <v>7513128.142</v>
+      </c>
+      <c r="E103" s="4">
+        <v>4691711.0889999997</v>
+      </c>
+      <c r="F103" s="59"/>
+      <c r="G103" s="59"/>
+      <c r="H103" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="I103" s="1"/>
       <c r="J103" s="1"/>
       <c r="K103" s="1"/>
     </row>
     <row r="104" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
-      <c r="C104" s="25"/>
-      <c r="D104" s="25"/>
-      <c r="E104" s="25"/>
-      <c r="F104" s="25"/>
-      <c r="G104" s="25"/>
-      <c r="H104" s="25"/>
-      <c r="I104" s="25"/>
+      <c r="C104" s="5">
+        <v>27</v>
+      </c>
+      <c r="D104" s="4">
+        <v>7513132.0240000002</v>
+      </c>
+      <c r="E104" s="4">
+        <v>4691706.8949999996</v>
+      </c>
+      <c r="F104" s="59"/>
+      <c r="G104" s="59"/>
+      <c r="H104" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="I104" s="1"/>
       <c r="J104" s="1"/>
       <c r="K104" s="1"/>
     </row>
     <row r="105" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
-      <c r="C105" s="25"/>
-      <c r="D105" s="25"/>
-      <c r="E105" s="25"/>
-      <c r="F105" s="25"/>
-      <c r="G105" s="25"/>
-      <c r="H105" s="25"/>
-      <c r="I105" s="25"/>
+      <c r="C105" s="5">
+        <v>28</v>
+      </c>
+      <c r="D105" s="4">
+        <v>7513133.5190000003</v>
+      </c>
+      <c r="E105" s="4">
+        <v>4691706.18</v>
+      </c>
+      <c r="F105" s="59"/>
+      <c r="G105" s="59"/>
+      <c r="H105" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="I105" s="1"/>
       <c r="J105" s="1"/>
       <c r="K105" s="1"/>
     </row>
     <row r="106" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
-      <c r="C106" s="25"/>
-      <c r="D106" s="25"/>
-      <c r="E106" s="25"/>
-      <c r="F106" s="25"/>
-      <c r="G106" s="25"/>
-      <c r="H106" s="25"/>
-      <c r="I106" s="25"/>
+      <c r="C106" s="5">
+        <v>65</v>
+      </c>
+      <c r="D106" s="4">
+        <v>7513134.1436999999</v>
+      </c>
+      <c r="E106" s="4">
+        <v>4691706.1939000003</v>
+      </c>
+      <c r="F106" s="59"/>
+      <c r="G106" s="59"/>
+      <c r="H106" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="I106" s="1"/>
       <c r="J106" s="1"/>
       <c r="K106" s="1"/>
     </row>
-    <row r="107" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
-      <c r="C107" s="25"/>
-      <c r="D107" s="25"/>
-      <c r="E107" s="25"/>
-      <c r="F107" s="25"/>
-      <c r="G107" s="25"/>
-      <c r="H107" s="25"/>
-      <c r="I107" s="25"/>
+      <c r="C107" s="5">
+        <v>67</v>
+      </c>
+      <c r="D107" s="4">
+        <v>7513135.8569999998</v>
+      </c>
+      <c r="E107" s="4">
+        <v>4691707.7450000001</v>
+      </c>
+      <c r="F107" s="59"/>
+      <c r="G107" s="59"/>
+      <c r="H107" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="I107" s="1"/>
       <c r="J107" s="1"/>
       <c r="K107" s="1"/>
     </row>
     <row r="108" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A108" s="2" t="s">
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
+      <c r="C108" s="5">
+        <v>68</v>
+      </c>
+      <c r="D108" s="4">
+        <v>7513143.2529999996</v>
+      </c>
+      <c r="E108" s="4">
+        <v>4691714.4639999997</v>
+      </c>
+      <c r="F108" s="59"/>
+      <c r="G108" s="59"/>
+      <c r="H108" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="I108" s="1"/>
+      <c r="J108" s="1"/>
+      <c r="K108" s="1"/>
+    </row>
+    <row r="109" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
+      <c r="C109" s="5">
+        <v>106</v>
+      </c>
+      <c r="D109" s="4">
+        <v>7513136.3592999997</v>
+      </c>
+      <c r="E109" s="4">
+        <v>4691715.8525</v>
+      </c>
+      <c r="F109" s="59"/>
+      <c r="G109" s="59"/>
+      <c r="H109" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="I109" s="1"/>
+      <c r="J109" s="1"/>
+      <c r="K109" s="1"/>
+    </row>
+    <row r="110" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A110" s="1"/>
+      <c r="B110" s="1"/>
+      <c r="C110" s="5">
+        <v>107</v>
+      </c>
+      <c r="D110" s="4">
+        <v>7513132.6316</v>
+      </c>
+      <c r="E110" s="4">
+        <v>4691712.5202000001</v>
+      </c>
+      <c r="F110" s="59"/>
+      <c r="G110" s="59"/>
+      <c r="H110" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="I110" s="1"/>
+      <c r="J110" s="1"/>
+      <c r="K110" s="1"/>
+    </row>
+    <row r="111" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A111" s="1"/>
+      <c r="B111" s="1"/>
+      <c r="C111" s="6">
+        <v>108</v>
+      </c>
+      <c r="D111" s="7">
+        <v>7513129.5292999996</v>
+      </c>
+      <c r="E111" s="7">
+        <v>4691715.9907</v>
+      </c>
+      <c r="F111" s="60"/>
+      <c r="G111" s="60"/>
+      <c r="H111" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="I111" s="1"/>
+      <c r="J111" s="1"/>
+      <c r="K111" s="1"/>
+    </row>
+    <row r="112" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+      <c r="C112" s="28"/>
+      <c r="D112" s="29"/>
+      <c r="E112" s="29"/>
+      <c r="F112" s="30"/>
+      <c r="G112" s="30"/>
+      <c r="H112" s="25"/>
+      <c r="I112" s="1"/>
+      <c r="J112" s="1"/>
+      <c r="K112" s="1"/>
+    </row>
+    <row r="113" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A113" s="1"/>
+      <c r="B113" s="1"/>
+      <c r="C113" s="28"/>
+      <c r="D113" s="29"/>
+      <c r="E113" s="29"/>
+      <c r="F113" s="30"/>
+      <c r="G113" s="30"/>
+      <c r="H113" s="25"/>
+      <c r="I113" s="1"/>
+      <c r="J113" s="1"/>
+      <c r="K113" s="1"/>
+    </row>
+    <row r="114" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
+      <c r="C114" s="28"/>
+      <c r="D114" s="29"/>
+      <c r="E114" s="29"/>
+      <c r="F114" s="30"/>
+      <c r="G114" s="30"/>
+      <c r="H114" s="25"/>
+      <c r="I114" s="1"/>
+      <c r="J114" s="1"/>
+      <c r="K114" s="1"/>
+    </row>
+    <row r="115" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A115" s="1"/>
+      <c r="B115" s="1"/>
+      <c r="C115" s="28"/>
+      <c r="D115" s="29"/>
+      <c r="E115" s="29"/>
+      <c r="F115" s="30"/>
+      <c r="G115" s="30"/>
+      <c r="H115" s="25"/>
+      <c r="I115" s="1"/>
+      <c r="J115" s="1"/>
+      <c r="K115" s="1"/>
+    </row>
+    <row r="116" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A116" s="1"/>
+      <c r="B116" s="1"/>
+      <c r="C116" s="28"/>
+      <c r="D116" s="29"/>
+      <c r="E116" s="29"/>
+      <c r="F116" s="30"/>
+      <c r="G116" s="30"/>
+      <c r="H116" s="25"/>
+      <c r="I116" s="1"/>
+      <c r="J116" s="1"/>
+      <c r="K116" s="1"/>
+    </row>
+    <row r="117" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A117" s="1"/>
+      <c r="B117" s="1"/>
+      <c r="C117" s="28"/>
+      <c r="D117" s="29"/>
+      <c r="E117" s="29"/>
+      <c r="F117" s="30"/>
+      <c r="G117" s="30"/>
+      <c r="H117" s="25"/>
+      <c r="I117" s="1"/>
+      <c r="J117" s="1"/>
+      <c r="K117" s="1"/>
+    </row>
+    <row r="118" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A118" s="1"/>
+      <c r="B118" s="1"/>
+      <c r="C118" s="28"/>
+      <c r="D118" s="29"/>
+      <c r="E118" s="29"/>
+      <c r="F118" s="30"/>
+      <c r="G118" s="30"/>
+      <c r="H118" s="25"/>
+      <c r="I118" s="1"/>
+      <c r="J118" s="1"/>
+      <c r="K118" s="1"/>
+    </row>
+    <row r="119" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A119" s="1"/>
+      <c r="B119" s="1"/>
+      <c r="C119" s="28"/>
+      <c r="D119" s="29"/>
+      <c r="E119" s="29"/>
+      <c r="F119" s="30"/>
+      <c r="G119" s="30"/>
+      <c r="H119" s="25"/>
+      <c r="I119" s="1"/>
+      <c r="J119" s="1"/>
+      <c r="K119" s="1"/>
+    </row>
+    <row r="120" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A120" s="1"/>
+      <c r="B120" s="1"/>
+      <c r="C120" s="28"/>
+      <c r="D120" s="29"/>
+      <c r="E120" s="29"/>
+      <c r="F120" s="30"/>
+      <c r="G120" s="30"/>
+      <c r="H120" s="25"/>
+      <c r="I120" s="1"/>
+      <c r="J120" s="1"/>
+      <c r="K120" s="1"/>
+    </row>
+    <row r="121" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A121" s="1"/>
+      <c r="B121" s="1"/>
+      <c r="C121" s="28"/>
+      <c r="D121" s="29"/>
+      <c r="E121" s="29"/>
+      <c r="F121" s="30"/>
+      <c r="G121" s="30"/>
+      <c r="H121" s="25"/>
+      <c r="I121" s="1"/>
+      <c r="J121" s="1"/>
+      <c r="K121" s="1"/>
+    </row>
+    <row r="122" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A122" s="1"/>
+      <c r="B122" s="1"/>
+      <c r="C122" s="28"/>
+      <c r="D122" s="29"/>
+      <c r="E122" s="29"/>
+      <c r="F122" s="30"/>
+      <c r="G122" s="30"/>
+      <c r="H122" s="25"/>
+      <c r="I122" s="1"/>
+      <c r="J122" s="1"/>
+      <c r="K122" s="1"/>
+    </row>
+    <row r="123" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A123" s="1"/>
+      <c r="B123" s="1"/>
+      <c r="C123" s="28"/>
+      <c r="D123" s="29"/>
+      <c r="E123" s="29"/>
+      <c r="F123" s="30"/>
+      <c r="G123" s="30"/>
+      <c r="H123" s="25"/>
+      <c r="I123" s="1"/>
+      <c r="J123" s="1"/>
+      <c r="K123" s="1"/>
+    </row>
+    <row r="124" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A124" s="1"/>
+      <c r="B124" s="1"/>
+      <c r="C124" s="28"/>
+      <c r="D124" s="29"/>
+      <c r="E124" s="29"/>
+      <c r="F124" s="30"/>
+      <c r="G124" s="30"/>
+      <c r="H124" s="25"/>
+      <c r="I124" s="1"/>
+      <c r="J124" s="1"/>
+      <c r="K124" s="1"/>
+    </row>
+    <row r="125" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A125" s="1"/>
+      <c r="B125" s="1"/>
+      <c r="C125" s="28"/>
+      <c r="D125" s="29"/>
+      <c r="E125" s="29"/>
+      <c r="F125" s="30"/>
+      <c r="G125" s="30"/>
+      <c r="H125" s="25"/>
+      <c r="I125" s="1"/>
+      <c r="J125" s="1"/>
+      <c r="K125" s="1"/>
+    </row>
+    <row r="126" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A126" s="1"/>
+      <c r="B126" s="1"/>
+      <c r="C126" s="28"/>
+      <c r="D126" s="29"/>
+      <c r="E126" s="29"/>
+      <c r="F126" s="30"/>
+      <c r="G126" s="30"/>
+      <c r="H126" s="25"/>
+      <c r="I126" s="1"/>
+      <c r="J126" s="1"/>
+      <c r="K126" s="1"/>
+    </row>
+    <row r="127" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A127" s="1"/>
+      <c r="B127" s="1"/>
+      <c r="C127" s="28"/>
+      <c r="D127" s="29"/>
+      <c r="E127" s="29"/>
+      <c r="F127" s="30"/>
+      <c r="G127" s="30"/>
+      <c r="H127" s="25"/>
+      <c r="I127" s="1"/>
+      <c r="J127" s="1"/>
+      <c r="K127" s="1"/>
+    </row>
+    <row r="128" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A128" s="1"/>
+      <c r="B128" s="1"/>
+      <c r="C128" s="28"/>
+      <c r="D128" s="29"/>
+      <c r="E128" s="29"/>
+      <c r="F128" s="30"/>
+      <c r="G128" s="30"/>
+      <c r="H128" s="25"/>
+      <c r="I128" s="1"/>
+      <c r="J128" s="1"/>
+      <c r="K128" s="1"/>
+    </row>
+    <row r="129" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A129" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B108" s="3"/>
-      <c r="C108" s="3"/>
-      <c r="D108" s="3"/>
-      <c r="E108" s="62" t="s">
+      <c r="B129" s="3"/>
+      <c r="C129" s="3"/>
+      <c r="D129" s="3"/>
+      <c r="E129" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="F108" s="63"/>
-      <c r="G108" s="64"/>
-      <c r="H108" s="65" t="s">
+      <c r="F129" s="62"/>
+      <c r="G129" s="63"/>
+      <c r="H129" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="I108" s="66"/>
-      <c r="J108" s="69"/>
-      <c r="K108" s="70"/>
-    </row>
-    <row r="109" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A109" s="39" t="s">
+      <c r="I129" s="65"/>
+      <c r="J129" s="68"/>
+      <c r="K129" s="69"/>
+    </row>
+    <row r="130" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A130" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B109" s="40"/>
-      <c r="C109" s="40"/>
-      <c r="D109" s="41"/>
-      <c r="E109" s="42">
+      <c r="B130" s="39"/>
+      <c r="C130" s="39"/>
+      <c r="D130" s="40"/>
+      <c r="E130" s="41">
         <v>152</v>
       </c>
-      <c r="F109" s="43"/>
-      <c r="G109" s="44"/>
-      <c r="H109" s="67"/>
-      <c r="I109" s="68"/>
-      <c r="J109" s="71"/>
-      <c r="K109" s="72"/>
+      <c r="F130" s="42"/>
+      <c r="G130" s="43"/>
+      <c r="H130" s="66"/>
+      <c r="I130" s="67"/>
+      <c r="J130" s="70"/>
+      <c r="K130" s="71"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="23">
     <mergeCell ref="A68:K69"/>
     <mergeCell ref="A70:K73"/>
     <mergeCell ref="C75:I77"/>
-    <mergeCell ref="E108:G108"/>
-    <mergeCell ref="H108:I109"/>
-    <mergeCell ref="J108:K109"/>
-    <mergeCell ref="A109:D109"/>
-    <mergeCell ref="E109:G109"/>
+    <mergeCell ref="E129:G129"/>
+    <mergeCell ref="H129:I130"/>
+    <mergeCell ref="J129:K130"/>
+    <mergeCell ref="A130:D130"/>
+    <mergeCell ref="E130:G130"/>
+    <mergeCell ref="F97:F111"/>
+    <mergeCell ref="G97:G111"/>
     <mergeCell ref="A67:D67"/>
     <mergeCell ref="E67:G67"/>
     <mergeCell ref="C8:I10"/>
@@ -3454,8 +3885,8 @@
     <mergeCell ref="F33:F51"/>
     <mergeCell ref="G33:G51"/>
     <mergeCell ref="C54:I55"/>
-    <mergeCell ref="F81:F95"/>
-    <mergeCell ref="G81:G95"/>
+    <mergeCell ref="F80:F94"/>
+    <mergeCell ref="G80:G94"/>
     <mergeCell ref="E66:G66"/>
     <mergeCell ref="H66:I67"/>
     <mergeCell ref="J66:K67"/>

</xml_diff>

<commit_message>
kati nk njesite done
</commit_message>
<xml_diff>
--- a/5-Njësite-banesore/regjistri/22-Koordinatat-për-pjesë-të-ndertesës.xlsx-2602-0-Albnori.xlsx
+++ b/5-Njësite-banesore/regjistri/22-Koordinatat-për-pjesë-të-ndertesës.xlsx-2602-0-Albnori.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="25">
   <si>
     <t>Nr</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>KATI2</t>
+  </si>
+  <si>
+    <t>KATI-NK</t>
   </si>
 </sst>
 </file>
@@ -1190,7 +1193,7 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>6569</xdr:colOff>
-      <xdr:row>74</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>13138</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2975170" cy="298800"/>
@@ -1251,7 +1254,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>839686</xdr:colOff>
-      <xdr:row>74</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>43127</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2953749" cy="298800"/>
@@ -1312,7 +1315,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>606643</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>89338</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3298607" cy="298800"/>
@@ -1387,7 +1390,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>842998</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>105246</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3051603" cy="298800"/>
@@ -1746,8 +1749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K130"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A65" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="W74" sqref="W74"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A121" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77:XFD77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2868,7 +2871,7 @@
       <c r="J72" s="53"/>
       <c r="K72" s="53"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="53"/>
       <c r="B73" s="53"/>
       <c r="C73" s="53"/>
@@ -2881,66 +2884,96 @@
       <c r="J73" s="53"/>
       <c r="K73" s="53"/>
     </row>
-    <row r="74" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C74" s="44"/>
+      <c r="D74" s="45"/>
+      <c r="E74" s="45"/>
+      <c r="F74" s="45"/>
+      <c r="G74" s="45"/>
+      <c r="H74" s="45"/>
+      <c r="I74" s="46"/>
+    </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C75" s="44"/>
-      <c r="D75" s="45"/>
-      <c r="E75" s="45"/>
-      <c r="F75" s="45"/>
-      <c r="G75" s="45"/>
-      <c r="H75" s="45"/>
-      <c r="I75" s="46"/>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C76" s="47"/>
-      <c r="D76" s="48"/>
-      <c r="E76" s="48"/>
-      <c r="F76" s="48"/>
-      <c r="G76" s="48"/>
-      <c r="H76" s="48"/>
-      <c r="I76" s="49"/>
-    </row>
-    <row r="77" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C77" s="50"/>
-      <c r="D77" s="51"/>
-      <c r="E77" s="51"/>
-      <c r="F77" s="51"/>
-      <c r="G77" s="51"/>
-      <c r="H77" s="51"/>
-      <c r="I77" s="52"/>
-    </row>
-    <row r="78" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C75" s="47"/>
+      <c r="D75" s="48"/>
+      <c r="E75" s="48"/>
+      <c r="F75" s="48"/>
+      <c r="G75" s="48"/>
+      <c r="H75" s="48"/>
+      <c r="I75" s="49"/>
+    </row>
+    <row r="76" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C76" s="50"/>
+      <c r="D76" s="51"/>
+      <c r="E76" s="51"/>
+      <c r="F76" s="51"/>
+      <c r="G76" s="51"/>
+      <c r="H76" s="51"/>
+      <c r="I76" s="52"/>
+    </row>
+    <row r="77" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A77" s="1"/>
+      <c r="C77" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D77" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E77" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F77" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G77" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H77" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1"/>
+      <c r="K77" s="1"/>
+    </row>
+    <row r="78" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
-      <c r="C78" s="28"/>
-      <c r="D78" s="29"/>
-      <c r="E78" s="29"/>
-      <c r="F78" s="30"/>
-      <c r="G78" s="30"/>
-      <c r="H78" s="25"/>
+      <c r="C78" s="5">
+        <v>1</v>
+      </c>
+      <c r="D78" s="4">
+        <v>7513135.568</v>
+      </c>
+      <c r="E78" s="4">
+        <v>4691722.8739999998</v>
+      </c>
+      <c r="F78" s="59">
+        <v>623.17399999999998</v>
+      </c>
+      <c r="G78" s="59" t="s">
+        <v>20</v>
+      </c>
+      <c r="H78" s="26" t="s">
+        <v>8</v>
+      </c>
       <c r="I78" s="1"/>
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
     </row>
     <row r="79" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
-      <c r="C79" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D79" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E79" s="9" t="s">
+      <c r="C79" s="5">
         <v>2</v>
       </c>
-      <c r="F79" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G79" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H79" s="13" t="s">
-        <v>3</v>
+      <c r="D79" s="4">
+        <v>7513132.5010000002</v>
+      </c>
+      <c r="E79" s="4">
+        <v>4691720.0990000004</v>
+      </c>
+      <c r="F79" s="59"/>
+      <c r="G79" s="59"/>
+      <c r="H79" s="26" t="s">
+        <v>8</v>
       </c>
       <c r="I79" s="1"/>
       <c r="J79" s="1"/>
@@ -2949,20 +2982,16 @@
     <row r="80" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="C80" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D80" s="4">
-        <v>7513135.568</v>
+        <v>7513128.9859999996</v>
       </c>
       <c r="E80" s="4">
-        <v>4691722.8739999998</v>
-      </c>
-      <c r="F80" s="59">
-        <v>623.17399999999998</v>
-      </c>
-      <c r="G80" s="59" t="s">
-        <v>20</v>
-      </c>
+        <v>4691715.5049999999</v>
+      </c>
+      <c r="F80" s="59"/>
+      <c r="G80" s="59"/>
       <c r="H80" s="26" t="s">
         <v>8</v>
       </c>
@@ -2973,13 +3002,13 @@
     <row r="81" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="C81" s="5">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="D81" s="4">
-        <v>7513132.5010000002</v>
+        <v>7513133.25</v>
       </c>
       <c r="E81" s="4">
-        <v>4691720.0990000004</v>
+        <v>4691719.318</v>
       </c>
       <c r="F81" s="59"/>
       <c r="G81" s="59"/>
@@ -2993,13 +3022,13 @@
     <row r="82" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="C82" s="5">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D82" s="4">
-        <v>7513128.9859999996</v>
+        <v>7513127.2779999999</v>
       </c>
       <c r="E82" s="4">
-        <v>4691715.5049999999</v>
+        <v>4691713.9479999999</v>
       </c>
       <c r="F82" s="59"/>
       <c r="G82" s="59"/>
@@ -3013,13 +3042,13 @@
     <row r="83" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
       <c r="C83" s="5">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D83" s="4">
-        <v>7513133.25</v>
+        <v>7513127.3820000002</v>
       </c>
       <c r="E83" s="4">
-        <v>4691719.318</v>
+        <v>4691712.1909999996</v>
       </c>
       <c r="F83" s="59"/>
       <c r="G83" s="59"/>
@@ -3033,13 +3062,13 @@
     <row r="84" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
       <c r="C84" s="5">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D84" s="4">
-        <v>7513127.2779999999</v>
+        <v>7513128.142</v>
       </c>
       <c r="E84" s="4">
-        <v>4691713.9479999999</v>
+        <v>4691711.0889999997</v>
       </c>
       <c r="F84" s="59"/>
       <c r="G84" s="59"/>
@@ -3053,13 +3082,13 @@
     <row r="85" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="C85" s="5">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D85" s="4">
-        <v>7513127.3820000002</v>
+        <v>7513132.0240000002</v>
       </c>
       <c r="E85" s="4">
-        <v>4691712.1909999996</v>
+        <v>4691706.8949999996</v>
       </c>
       <c r="F85" s="59"/>
       <c r="G85" s="59"/>
@@ -3073,13 +3102,13 @@
     <row r="86" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
       <c r="C86" s="5">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D86" s="4">
-        <v>7513128.142</v>
+        <v>7513133.5190000003</v>
       </c>
       <c r="E86" s="4">
-        <v>4691711.0889999997</v>
+        <v>4691706.18</v>
       </c>
       <c r="F86" s="59"/>
       <c r="G86" s="59"/>
@@ -3093,13 +3122,13 @@
     <row r="87" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
       <c r="C87" s="5">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="D87" s="4">
-        <v>7513132.0240000002</v>
+        <v>7513134.1436999999</v>
       </c>
       <c r="E87" s="4">
-        <v>4691706.8949999996</v>
+        <v>4691706.1939000003</v>
       </c>
       <c r="F87" s="59"/>
       <c r="G87" s="59"/>
@@ -3113,13 +3142,13 @@
     <row r="88" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
       <c r="C88" s="5">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="D88" s="4">
-        <v>7513133.5190000003</v>
+        <v>7513135.8569999998</v>
       </c>
       <c r="E88" s="4">
-        <v>4691706.18</v>
+        <v>4691707.7450000001</v>
       </c>
       <c r="F88" s="59"/>
       <c r="G88" s="59"/>
@@ -3133,13 +3162,13 @@
     <row r="89" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
       <c r="C89" s="5">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D89" s="4">
-        <v>7513134.1436999999</v>
+        <v>7513143.2529999996</v>
       </c>
       <c r="E89" s="4">
-        <v>4691706.1939000003</v>
+        <v>4691714.4639999997</v>
       </c>
       <c r="F89" s="59"/>
       <c r="G89" s="59"/>
@@ -3153,13 +3182,13 @@
     <row r="90" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
       <c r="C90" s="5">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="D90" s="4">
-        <v>7513135.8569999998</v>
+        <v>7513136.3592999997</v>
       </c>
       <c r="E90" s="4">
-        <v>4691707.7450000001</v>
+        <v>4691715.8525</v>
       </c>
       <c r="F90" s="59"/>
       <c r="G90" s="59"/>
@@ -3173,13 +3202,13 @@
     <row r="91" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A91" s="1"/>
       <c r="C91" s="5">
-        <v>68</v>
+        <v>107</v>
       </c>
       <c r="D91" s="4">
-        <v>7513143.2529999996</v>
+        <v>7513132.6316</v>
       </c>
       <c r="E91" s="4">
-        <v>4691714.4639999997</v>
+        <v>4691712.5202000001</v>
       </c>
       <c r="F91" s="59"/>
       <c r="G91" s="59"/>
@@ -3190,76 +3219,86 @@
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
     </row>
-    <row r="92" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="1"/>
-      <c r="C92" s="5">
-        <v>106</v>
-      </c>
-      <c r="D92" s="4">
-        <v>7513136.3592999997</v>
-      </c>
-      <c r="E92" s="4">
-        <v>4691715.8525</v>
-      </c>
-      <c r="F92" s="59"/>
-      <c r="G92" s="59"/>
-      <c r="H92" s="26" t="s">
+      <c r="B92" s="1"/>
+      <c r="C92" s="6">
+        <v>108</v>
+      </c>
+      <c r="D92" s="7">
+        <v>7513129.5292999996</v>
+      </c>
+      <c r="E92" s="7">
+        <v>4691715.9907</v>
+      </c>
+      <c r="F92" s="60"/>
+      <c r="G92" s="60"/>
+      <c r="H92" s="27" t="s">
         <v>8</v>
       </c>
       <c r="I92" s="1"/>
       <c r="J92" s="1"/>
       <c r="K92" s="1"/>
     </row>
-    <row r="93" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="1"/>
-      <c r="C93" s="5">
-        <v>107</v>
-      </c>
-      <c r="D93" s="4">
-        <v>7513132.6316</v>
-      </c>
-      <c r="E93" s="4">
-        <v>4691712.5202000001</v>
-      </c>
-      <c r="F93" s="59"/>
-      <c r="G93" s="59"/>
-      <c r="H93" s="26" t="s">
-        <v>8</v>
-      </c>
+      <c r="B93" s="1"/>
+      <c r="C93" s="28"/>
+      <c r="D93" s="29"/>
+      <c r="E93" s="29"/>
+      <c r="F93" s="30"/>
+      <c r="G93" s="30"/>
+      <c r="H93" s="25"/>
       <c r="I93" s="1"/>
       <c r="J93" s="1"/>
       <c r="K93" s="1"/>
     </row>
-    <row r="94" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
-      <c r="C94" s="6">
-        <v>108</v>
-      </c>
-      <c r="D94" s="7">
-        <v>7513129.5292999996</v>
-      </c>
-      <c r="E94" s="7">
-        <v>4691715.9907</v>
-      </c>
-      <c r="F94" s="60"/>
-      <c r="G94" s="60"/>
-      <c r="H94" s="27" t="s">
-        <v>8</v>
+      <c r="C94" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D94" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E94" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F94" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G94" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H94" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="I94" s="1"/>
       <c r="J94" s="1"/>
       <c r="K94" s="1"/>
     </row>
-    <row r="95" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
-      <c r="C95" s="28"/>
-      <c r="D95" s="29"/>
-      <c r="E95" s="29"/>
-      <c r="F95" s="30"/>
-      <c r="G95" s="30"/>
-      <c r="H95" s="25"/>
+      <c r="C95" s="5">
+        <v>1</v>
+      </c>
+      <c r="D95" s="4">
+        <v>7513135.568</v>
+      </c>
+      <c r="E95" s="4">
+        <v>4691722.8739999998</v>
+      </c>
+      <c r="F95" s="59">
+        <v>626.09400000000005</v>
+      </c>
+      <c r="G95" s="59" t="s">
+        <v>23</v>
+      </c>
+      <c r="H95" s="26" t="s">
+        <v>8</v>
+      </c>
       <c r="I95" s="1"/>
       <c r="J95" s="1"/>
       <c r="K95" s="1"/>
@@ -3267,23 +3306,19 @@
     <row r="96" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
-      <c r="C96" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D96" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E96" s="9" t="s">
+      <c r="C96" s="5">
         <v>2</v>
       </c>
-      <c r="F96" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G96" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H96" s="13" t="s">
-        <v>3</v>
+      <c r="D96" s="4">
+        <v>7513132.5010000002</v>
+      </c>
+      <c r="E96" s="4">
+        <v>4691720.0990000004</v>
+      </c>
+      <c r="F96" s="59"/>
+      <c r="G96" s="59"/>
+      <c r="H96" s="26" t="s">
+        <v>8</v>
       </c>
       <c r="I96" s="1"/>
       <c r="J96" s="1"/>
@@ -3293,20 +3328,16 @@
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D97" s="4">
-        <v>7513135.568</v>
+        <v>7513128.9859999996</v>
       </c>
       <c r="E97" s="4">
-        <v>4691722.8739999998</v>
-      </c>
-      <c r="F97" s="59">
-        <v>626.09400000000005</v>
-      </c>
-      <c r="G97" s="59" t="s">
-        <v>23</v>
-      </c>
+        <v>4691715.5049999999</v>
+      </c>
+      <c r="F97" s="59"/>
+      <c r="G97" s="59"/>
       <c r="H97" s="26" t="s">
         <v>8</v>
       </c>
@@ -3318,13 +3349,13 @@
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="5">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="D98" s="4">
-        <v>7513132.5010000002</v>
+        <v>7513133.25</v>
       </c>
       <c r="E98" s="4">
-        <v>4691720.0990000004</v>
+        <v>4691719.318</v>
       </c>
       <c r="F98" s="59"/>
       <c r="G98" s="59"/>
@@ -3339,13 +3370,13 @@
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="5">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D99" s="4">
-        <v>7513128.9859999996</v>
+        <v>7513127.2779999999</v>
       </c>
       <c r="E99" s="4">
-        <v>4691715.5049999999</v>
+        <v>4691713.9479999999</v>
       </c>
       <c r="F99" s="59"/>
       <c r="G99" s="59"/>
@@ -3360,13 +3391,13 @@
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="5">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D100" s="4">
-        <v>7513133.25</v>
+        <v>7513127.3820000002</v>
       </c>
       <c r="E100" s="4">
-        <v>4691719.318</v>
+        <v>4691712.1909999996</v>
       </c>
       <c r="F100" s="59"/>
       <c r="G100" s="59"/>
@@ -3381,13 +3412,13 @@
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="5">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D101" s="4">
-        <v>7513127.2779999999</v>
+        <v>7513128.142</v>
       </c>
       <c r="E101" s="4">
-        <v>4691713.9479999999</v>
+        <v>4691711.0889999997</v>
       </c>
       <c r="F101" s="59"/>
       <c r="G101" s="59"/>
@@ -3402,13 +3433,13 @@
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="5">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D102" s="4">
-        <v>7513127.3820000002</v>
+        <v>7513132.0240000002</v>
       </c>
       <c r="E102" s="4">
-        <v>4691712.1909999996</v>
+        <v>4691706.8949999996</v>
       </c>
       <c r="F102" s="59"/>
       <c r="G102" s="59"/>
@@ -3423,13 +3454,13 @@
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="5">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D103" s="4">
-        <v>7513128.142</v>
+        <v>7513133.5190000003</v>
       </c>
       <c r="E103" s="4">
-        <v>4691711.0889999997</v>
+        <v>4691706.18</v>
       </c>
       <c r="F103" s="59"/>
       <c r="G103" s="59"/>
@@ -3444,13 +3475,13 @@
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="5">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="D104" s="4">
-        <v>7513132.0240000002</v>
+        <v>7513134.1436999999</v>
       </c>
       <c r="E104" s="4">
-        <v>4691706.8949999996</v>
+        <v>4691706.1939000003</v>
       </c>
       <c r="F104" s="59"/>
       <c r="G104" s="59"/>
@@ -3465,13 +3496,13 @@
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="5">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="D105" s="4">
-        <v>7513133.5190000003</v>
+        <v>7513135.8569999998</v>
       </c>
       <c r="E105" s="4">
-        <v>4691706.18</v>
+        <v>4691707.7450000001</v>
       </c>
       <c r="F105" s="59"/>
       <c r="G105" s="59"/>
@@ -3486,13 +3517,13 @@
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="5">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D106" s="4">
-        <v>7513134.1436999999</v>
+        <v>7513143.2529999996</v>
       </c>
       <c r="E106" s="4">
-        <v>4691706.1939000003</v>
+        <v>4691714.4639999997</v>
       </c>
       <c r="F106" s="59"/>
       <c r="G106" s="59"/>
@@ -3507,13 +3538,13 @@
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="5">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="D107" s="4">
-        <v>7513135.8569999998</v>
+        <v>7513136.3592999997</v>
       </c>
       <c r="E107" s="4">
-        <v>4691707.7450000001</v>
+        <v>4691715.8525</v>
       </c>
       <c r="F107" s="59"/>
       <c r="G107" s="59"/>
@@ -3528,13 +3559,13 @@
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="5">
-        <v>68</v>
+        <v>107</v>
       </c>
       <c r="D108" s="4">
-        <v>7513143.2529999996</v>
+        <v>7513132.6316</v>
       </c>
       <c r="E108" s="4">
-        <v>4691714.4639999997</v>
+        <v>4691712.5202000001</v>
       </c>
       <c r="F108" s="59"/>
       <c r="G108" s="59"/>
@@ -3545,64 +3576,60 @@
       <c r="J108" s="1"/>
       <c r="K108" s="1"/>
     </row>
-    <row r="109" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
-      <c r="C109" s="5">
-        <v>106</v>
-      </c>
-      <c r="D109" s="4">
-        <v>7513136.3592999997</v>
-      </c>
-      <c r="E109" s="4">
-        <v>4691715.8525</v>
-      </c>
-      <c r="F109" s="59"/>
-      <c r="G109" s="59"/>
-      <c r="H109" s="26" t="s">
+      <c r="C109" s="6">
+        <v>108</v>
+      </c>
+      <c r="D109" s="7">
+        <v>7513129.5292999996</v>
+      </c>
+      <c r="E109" s="7">
+        <v>4691715.9907</v>
+      </c>
+      <c r="F109" s="60"/>
+      <c r="G109" s="60"/>
+      <c r="H109" s="27" t="s">
         <v>8</v>
       </c>
       <c r="I109" s="1"/>
       <c r="J109" s="1"/>
       <c r="K109" s="1"/>
     </row>
-    <row r="110" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
-      <c r="C110" s="5">
-        <v>107</v>
-      </c>
-      <c r="D110" s="4">
-        <v>7513132.6316</v>
-      </c>
-      <c r="E110" s="4">
-        <v>4691712.5202000001</v>
-      </c>
-      <c r="F110" s="59"/>
-      <c r="G110" s="59"/>
-      <c r="H110" s="26" t="s">
-        <v>8</v>
-      </c>
+      <c r="C110" s="28"/>
+      <c r="D110" s="29"/>
+      <c r="E110" s="29"/>
+      <c r="F110" s="30"/>
+      <c r="G110" s="30"/>
+      <c r="H110" s="25"/>
       <c r="I110" s="1"/>
       <c r="J110" s="1"/>
       <c r="K110" s="1"/>
     </row>
-    <row r="111" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
-      <c r="C111" s="6">
-        <v>108</v>
-      </c>
-      <c r="D111" s="7">
-        <v>7513129.5292999996</v>
-      </c>
-      <c r="E111" s="7">
-        <v>4691715.9907</v>
-      </c>
-      <c r="F111" s="60"/>
-      <c r="G111" s="60"/>
-      <c r="H111" s="27" t="s">
-        <v>8</v>
+      <c r="C111" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D111" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E111" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F111" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G111" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H111" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="I111" s="1"/>
       <c r="J111" s="1"/>
@@ -3611,12 +3638,24 @@
     <row r="112" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
-      <c r="C112" s="28"/>
-      <c r="D112" s="29"/>
-      <c r="E112" s="29"/>
-      <c r="F112" s="30"/>
-      <c r="G112" s="30"/>
-      <c r="H112" s="25"/>
+      <c r="C112" s="5">
+        <v>42</v>
+      </c>
+      <c r="D112" s="4">
+        <v>7513127.6977000004</v>
+      </c>
+      <c r="E112" s="4">
+        <v>4691714.3306</v>
+      </c>
+      <c r="F112" s="59">
+        <v>629.29999999999995</v>
+      </c>
+      <c r="G112" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="H112" s="26" t="s">
+        <v>8</v>
+      </c>
       <c r="I112" s="1"/>
       <c r="J112" s="1"/>
       <c r="K112" s="1"/>
@@ -3624,12 +3663,20 @@
     <row r="113" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
-      <c r="C113" s="28"/>
-      <c r="D113" s="29"/>
-      <c r="E113" s="29"/>
-      <c r="F113" s="30"/>
-      <c r="G113" s="30"/>
-      <c r="H113" s="25"/>
+      <c r="C113" s="5">
+        <v>43</v>
+      </c>
+      <c r="D113" s="4">
+        <v>7513127.2779999999</v>
+      </c>
+      <c r="E113" s="4">
+        <v>4691713.9479999999</v>
+      </c>
+      <c r="F113" s="59"/>
+      <c r="G113" s="59"/>
+      <c r="H113" s="26" t="s">
+        <v>8</v>
+      </c>
       <c r="I113" s="1"/>
       <c r="J113" s="1"/>
       <c r="K113" s="1"/>
@@ -3637,12 +3684,20 @@
     <row r="114" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
-      <c r="C114" s="28"/>
-      <c r="D114" s="29"/>
-      <c r="E114" s="29"/>
-      <c r="F114" s="30"/>
-      <c r="G114" s="30"/>
-      <c r="H114" s="25"/>
+      <c r="C114" s="5">
+        <v>44</v>
+      </c>
+      <c r="D114" s="4">
+        <v>7513127.3439999996</v>
+      </c>
+      <c r="E114" s="4">
+        <v>4691712.3039999995</v>
+      </c>
+      <c r="F114" s="59"/>
+      <c r="G114" s="59"/>
+      <c r="H114" s="26" t="s">
+        <v>8</v>
+      </c>
       <c r="I114" s="1"/>
       <c r="J114" s="1"/>
       <c r="K114" s="1"/>
@@ -3650,12 +3705,20 @@
     <row r="115" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
-      <c r="C115" s="28"/>
-      <c r="D115" s="29"/>
-      <c r="E115" s="29"/>
-      <c r="F115" s="30"/>
-      <c r="G115" s="30"/>
-      <c r="H115" s="25"/>
+      <c r="C115" s="5">
+        <v>45</v>
+      </c>
+      <c r="D115" s="4">
+        <v>7513128.142</v>
+      </c>
+      <c r="E115" s="4">
+        <v>4691711.0889999997</v>
+      </c>
+      <c r="F115" s="59"/>
+      <c r="G115" s="59"/>
+      <c r="H115" s="26" t="s">
+        <v>8</v>
+      </c>
       <c r="I115" s="1"/>
       <c r="J115" s="1"/>
       <c r="K115" s="1"/>
@@ -3663,12 +3726,20 @@
     <row r="116" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
-      <c r="C116" s="28"/>
-      <c r="D116" s="29"/>
-      <c r="E116" s="29"/>
-      <c r="F116" s="30"/>
-      <c r="G116" s="30"/>
-      <c r="H116" s="25"/>
+      <c r="C116" s="5">
+        <v>47</v>
+      </c>
+      <c r="D116" s="4">
+        <v>7513132.0240000002</v>
+      </c>
+      <c r="E116" s="4">
+        <v>4691706.8949999996</v>
+      </c>
+      <c r="F116" s="59"/>
+      <c r="G116" s="59"/>
+      <c r="H116" s="26" t="s">
+        <v>8</v>
+      </c>
       <c r="I116" s="1"/>
       <c r="J116" s="1"/>
       <c r="K116" s="1"/>
@@ -3676,12 +3747,20 @@
     <row r="117" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
-      <c r="C117" s="28"/>
-      <c r="D117" s="29"/>
-      <c r="E117" s="29"/>
-      <c r="F117" s="30"/>
-      <c r="G117" s="30"/>
-      <c r="H117" s="25"/>
+      <c r="C117" s="5">
+        <v>48</v>
+      </c>
+      <c r="D117" s="4">
+        <v>7513134.6310000001</v>
+      </c>
+      <c r="E117" s="4">
+        <v>4691706.6350999996</v>
+      </c>
+      <c r="F117" s="59"/>
+      <c r="G117" s="59"/>
+      <c r="H117" s="26" t="s">
+        <v>8</v>
+      </c>
       <c r="I117" s="1"/>
       <c r="J117" s="1"/>
       <c r="K117" s="1"/>
@@ -3689,12 +3768,20 @@
     <row r="118" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
-      <c r="C118" s="28"/>
-      <c r="D118" s="29"/>
-      <c r="E118" s="29"/>
-      <c r="F118" s="30"/>
-      <c r="G118" s="30"/>
-      <c r="H118" s="25"/>
+      <c r="C118" s="5">
+        <v>49</v>
+      </c>
+      <c r="D118" s="4">
+        <v>7513134.1436999999</v>
+      </c>
+      <c r="E118" s="4">
+        <v>4691706.1939000003</v>
+      </c>
+      <c r="F118" s="59"/>
+      <c r="G118" s="59"/>
+      <c r="H118" s="26" t="s">
+        <v>8</v>
+      </c>
       <c r="I118" s="1"/>
       <c r="J118" s="1"/>
       <c r="K118" s="1"/>
@@ -3702,12 +3789,20 @@
     <row r="119" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
-      <c r="C119" s="28"/>
-      <c r="D119" s="29"/>
-      <c r="E119" s="29"/>
-      <c r="F119" s="30"/>
-      <c r="G119" s="30"/>
-      <c r="H119" s="25"/>
+      <c r="C119" s="5">
+        <v>50</v>
+      </c>
+      <c r="D119" s="4">
+        <v>7513132.5010000002</v>
+      </c>
+      <c r="E119" s="4">
+        <v>4691720.0990000004</v>
+      </c>
+      <c r="F119" s="59"/>
+      <c r="G119" s="59"/>
+      <c r="H119" s="26" t="s">
+        <v>8</v>
+      </c>
       <c r="I119" s="1"/>
       <c r="J119" s="1"/>
       <c r="K119" s="1"/>
@@ -3715,12 +3810,20 @@
     <row r="120" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
-      <c r="C120" s="28"/>
-      <c r="D120" s="29"/>
-      <c r="E120" s="29"/>
-      <c r="F120" s="30"/>
-      <c r="G120" s="30"/>
-      <c r="H120" s="25"/>
+      <c r="C120" s="5">
+        <v>51</v>
+      </c>
+      <c r="D120" s="4">
+        <v>7513133.2570000002</v>
+      </c>
+      <c r="E120" s="4">
+        <v>4691719.3229999999</v>
+      </c>
+      <c r="F120" s="59"/>
+      <c r="G120" s="59"/>
+      <c r="H120" s="26" t="s">
+        <v>8</v>
+      </c>
       <c r="I120" s="1"/>
       <c r="J120" s="1"/>
       <c r="K120" s="1"/>
@@ -3728,12 +3831,20 @@
     <row r="121" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
-      <c r="C121" s="28"/>
-      <c r="D121" s="29"/>
-      <c r="E121" s="29"/>
-      <c r="F121" s="30"/>
-      <c r="G121" s="30"/>
-      <c r="H121" s="25"/>
+      <c r="C121" s="5">
+        <v>52</v>
+      </c>
+      <c r="D121" s="4">
+        <v>7513135.568</v>
+      </c>
+      <c r="E121" s="4">
+        <v>4691722.8739999998</v>
+      </c>
+      <c r="F121" s="59"/>
+      <c r="G121" s="59"/>
+      <c r="H121" s="26" t="s">
+        <v>8</v>
+      </c>
       <c r="I121" s="1"/>
       <c r="J121" s="1"/>
       <c r="K121" s="1"/>
@@ -3741,12 +3852,20 @@
     <row r="122" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
-      <c r="C122" s="28"/>
-      <c r="D122" s="29"/>
-      <c r="E122" s="29"/>
-      <c r="F122" s="30"/>
-      <c r="G122" s="30"/>
-      <c r="H122" s="25"/>
+      <c r="C122" s="5">
+        <v>78</v>
+      </c>
+      <c r="D122" s="4">
+        <v>7513129.2801999999</v>
+      </c>
+      <c r="E122" s="4">
+        <v>4691715.7680000002</v>
+      </c>
+      <c r="F122" s="59"/>
+      <c r="G122" s="59"/>
+      <c r="H122" s="26" t="s">
+        <v>8</v>
+      </c>
       <c r="I122" s="1"/>
       <c r="J122" s="1"/>
       <c r="K122" s="1"/>
@@ -3754,12 +3873,20 @@
     <row r="123" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
-      <c r="C123" s="28"/>
-      <c r="D123" s="29"/>
-      <c r="E123" s="29"/>
-      <c r="F123" s="30"/>
-      <c r="G123" s="30"/>
-      <c r="H123" s="25"/>
+      <c r="C123" s="5">
+        <v>79</v>
+      </c>
+      <c r="D123" s="4">
+        <v>7513143.2529999996</v>
+      </c>
+      <c r="E123" s="4">
+        <v>4691714.4639999997</v>
+      </c>
+      <c r="F123" s="59"/>
+      <c r="G123" s="59"/>
+      <c r="H123" s="26" t="s">
+        <v>8</v>
+      </c>
       <c r="I123" s="1"/>
       <c r="J123" s="1"/>
       <c r="K123" s="1"/>
@@ -3767,12 +3894,20 @@
     <row r="124" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
-      <c r="C124" s="28"/>
-      <c r="D124" s="29"/>
-      <c r="E124" s="29"/>
-      <c r="F124" s="30"/>
-      <c r="G124" s="30"/>
-      <c r="H124" s="25"/>
+      <c r="C124" s="5">
+        <v>80</v>
+      </c>
+      <c r="D124" s="4">
+        <v>7513136.3596000001</v>
+      </c>
+      <c r="E124" s="4">
+        <v>4691708.2016000003</v>
+      </c>
+      <c r="F124" s="59"/>
+      <c r="G124" s="59"/>
+      <c r="H124" s="26" t="s">
+        <v>8</v>
+      </c>
       <c r="I124" s="1"/>
       <c r="J124" s="1"/>
       <c r="K124" s="1"/>
@@ -3780,12 +3915,20 @@
     <row r="125" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
-      <c r="C125" s="28"/>
-      <c r="D125" s="29"/>
-      <c r="E125" s="29"/>
-      <c r="F125" s="30"/>
-      <c r="G125" s="30"/>
-      <c r="H125" s="25"/>
+      <c r="C125" s="5">
+        <v>82</v>
+      </c>
+      <c r="D125" s="4">
+        <v>7513133.0180000002</v>
+      </c>
+      <c r="E125" s="4">
+        <v>4691706.2857999997</v>
+      </c>
+      <c r="F125" s="59"/>
+      <c r="G125" s="59"/>
+      <c r="H125" s="26" t="s">
+        <v>8</v>
+      </c>
       <c r="I125" s="1"/>
       <c r="J125" s="1"/>
       <c r="K125" s="1"/>
@@ -3793,12 +3936,20 @@
     <row r="126" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
-      <c r="C126" s="28"/>
-      <c r="D126" s="29"/>
-      <c r="E126" s="29"/>
-      <c r="F126" s="30"/>
-      <c r="G126" s="30"/>
-      <c r="H126" s="25"/>
+      <c r="C126" s="5">
+        <v>106</v>
+      </c>
+      <c r="D126" s="4">
+        <v>7513135.1146999998</v>
+      </c>
+      <c r="E126" s="4">
+        <v>4691717.4736000001</v>
+      </c>
+      <c r="F126" s="59"/>
+      <c r="G126" s="59"/>
+      <c r="H126" s="26" t="s">
+        <v>8</v>
+      </c>
       <c r="I126" s="1"/>
       <c r="J126" s="1"/>
       <c r="K126" s="1"/>
@@ -3806,12 +3957,20 @@
     <row r="127" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
-      <c r="C127" s="28"/>
-      <c r="D127" s="29"/>
-      <c r="E127" s="29"/>
-      <c r="F127" s="30"/>
-      <c r="G127" s="30"/>
-      <c r="H127" s="25"/>
+      <c r="C127" s="5">
+        <v>107</v>
+      </c>
+      <c r="D127" s="4">
+        <v>7513131.0981999999</v>
+      </c>
+      <c r="E127" s="4">
+        <v>4691713.8247999996</v>
+      </c>
+      <c r="F127" s="59"/>
+      <c r="G127" s="59"/>
+      <c r="H127" s="26" t="s">
+        <v>8</v>
+      </c>
       <c r="I127" s="1"/>
       <c r="J127" s="1"/>
       <c r="K127" s="1"/>
@@ -3819,12 +3978,20 @@
     <row r="128" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
-      <c r="C128" s="28"/>
-      <c r="D128" s="29"/>
-      <c r="E128" s="29"/>
-      <c r="F128" s="30"/>
-      <c r="G128" s="30"/>
-      <c r="H128" s="25"/>
+      <c r="C128" s="6">
+        <v>109</v>
+      </c>
+      <c r="D128" s="7">
+        <v>7513133.3550000004</v>
+      </c>
+      <c r="E128" s="7">
+        <v>4691719.4106000001</v>
+      </c>
+      <c r="F128" s="60"/>
+      <c r="G128" s="60"/>
+      <c r="H128" s="27" t="s">
+        <v>8</v>
+      </c>
       <c r="I128" s="1"/>
       <c r="J128" s="1"/>
       <c r="K128" s="1"/>
@@ -3866,17 +4033,19 @@
       <c r="K130" s="71"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="25">
     <mergeCell ref="A68:K69"/>
     <mergeCell ref="A70:K73"/>
-    <mergeCell ref="C75:I77"/>
+    <mergeCell ref="C74:I76"/>
     <mergeCell ref="E129:G129"/>
     <mergeCell ref="H129:I130"/>
     <mergeCell ref="J129:K130"/>
     <mergeCell ref="A130:D130"/>
     <mergeCell ref="E130:G130"/>
-    <mergeCell ref="F97:F111"/>
-    <mergeCell ref="G97:G111"/>
+    <mergeCell ref="F95:F109"/>
+    <mergeCell ref="G95:G109"/>
+    <mergeCell ref="F112:F128"/>
+    <mergeCell ref="G112:G128"/>
     <mergeCell ref="A67:D67"/>
     <mergeCell ref="E67:G67"/>
     <mergeCell ref="C8:I10"/>
@@ -3885,8 +4054,8 @@
     <mergeCell ref="F33:F51"/>
     <mergeCell ref="G33:G51"/>
     <mergeCell ref="C54:I55"/>
-    <mergeCell ref="F80:F94"/>
-    <mergeCell ref="G80:G94"/>
+    <mergeCell ref="F78:F92"/>
+    <mergeCell ref="G78:G92"/>
     <mergeCell ref="E66:G66"/>
     <mergeCell ref="H66:I67"/>
     <mergeCell ref="J66:K67"/>

</xml_diff>

<commit_message>
perdhesa permiresi njesite done
</commit_message>
<xml_diff>
--- a/5-Njësite-banesore/regjistri/22-Koordinatat-për-pjesë-të-ndertesës.xlsx-2602-0-Albnori.xlsx
+++ b/5-Njësite-banesore/regjistri/22-Koordinatat-për-pjesë-të-ndertesës.xlsx-2602-0-Albnori.xlsx
@@ -688,6 +688,72 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -706,38 +772,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -750,45 +789,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1749,8 +1749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K130"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A121" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77:XFD77"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A29" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="N35" sqref="M33:Q51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1766,112 +1766,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="54"/>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
+      <c r="A1" s="38"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
     </row>
     <row r="2" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="54"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
     </row>
     <row r="4" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="53"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
-      <c r="K4" s="53"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
-      <c r="B5" s="53"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="53"/>
-      <c r="K5" s="53"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
-      <c r="B6" s="53"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="53"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="44"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="46"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="42"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="47"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="49"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="45"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="50"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="52"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="48"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
@@ -2322,10 +2322,10 @@
       <c r="E33" s="4">
         <v>4691722.8739999998</v>
       </c>
-      <c r="F33" s="55">
+      <c r="F33" s="68">
         <v>620.11199999999997</v>
       </c>
-      <c r="G33" s="55" t="s">
+      <c r="G33" s="68" t="s">
         <v>11</v>
       </c>
       <c r="H33" s="11" t="s">
@@ -2343,8 +2343,8 @@
       <c r="E34" s="4">
         <v>4691720.0990000004</v>
       </c>
-      <c r="F34" s="55"/>
-      <c r="G34" s="55"/>
+      <c r="F34" s="68"/>
+      <c r="G34" s="68"/>
       <c r="H34" s="11" t="s">
         <v>8</v>
       </c>
@@ -2360,8 +2360,8 @@
       <c r="E35" s="4">
         <v>4691719.3229999999</v>
       </c>
-      <c r="F35" s="55"/>
-      <c r="G35" s="55"/>
+      <c r="F35" s="68"/>
+      <c r="G35" s="68"/>
       <c r="H35" s="11" t="s">
         <v>8</v>
       </c>
@@ -2377,8 +2377,8 @@
       <c r="E36" s="4">
         <v>4691715.5049999999</v>
       </c>
-      <c r="F36" s="55"/>
-      <c r="G36" s="55"/>
+      <c r="F36" s="68"/>
+      <c r="G36" s="68"/>
       <c r="H36" s="11" t="s">
         <v>8</v>
       </c>
@@ -2386,16 +2386,16 @@
     </row>
     <row r="37" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C37" s="5">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D37" s="4">
-        <v>7513128.7640000004</v>
+        <v>7513130.5959999999</v>
       </c>
       <c r="E37" s="4">
-        <v>4691715.8310000002</v>
-      </c>
-      <c r="F37" s="55"/>
-      <c r="G37" s="55"/>
+        <v>4691713.7060000002</v>
+      </c>
+      <c r="F37" s="68"/>
+      <c r="G37" s="68"/>
       <c r="H37" s="11" t="s">
         <v>8</v>
       </c>
@@ -2404,16 +2404,16 @@
     <row r="38" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="C38" s="5">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D38" s="4">
-        <v>7513126.8399999999</v>
+        <v>7513129.4539999999</v>
       </c>
       <c r="E38" s="4">
-        <v>4691714.1189999999</v>
-      </c>
-      <c r="F38" s="55"/>
-      <c r="G38" s="55"/>
+        <v>4691712.6560000004</v>
+      </c>
+      <c r="F38" s="68"/>
+      <c r="G38" s="68"/>
       <c r="H38" s="11" t="s">
         <v>8</v>
       </c>
@@ -2423,16 +2423,16 @@
     <row r="39" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="C39" s="5">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D39" s="4">
-        <v>7513129.2566</v>
+        <v>7513129.1720000003</v>
       </c>
       <c r="E39" s="4">
-        <v>4691711.4588000001</v>
-      </c>
-      <c r="F39" s="55"/>
-      <c r="G39" s="55"/>
+        <v>4691712.0049999999</v>
+      </c>
+      <c r="F39" s="68"/>
+      <c r="G39" s="68"/>
       <c r="H39" s="11" t="s">
         <v>8</v>
       </c>
@@ -2442,16 +2442,16 @@
     <row r="40" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="C40" s="5">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D40" s="4">
-        <v>7513130.5959999999</v>
+        <v>7513129.6200000001</v>
       </c>
       <c r="E40" s="4">
-        <v>4691713.7060000002</v>
-      </c>
-      <c r="F40" s="55"/>
-      <c r="G40" s="55"/>
+        <v>4691710.9950000001</v>
+      </c>
+      <c r="F40" s="68"/>
+      <c r="G40" s="68"/>
       <c r="H40" s="11" t="s">
         <v>8</v>
       </c>
@@ -2461,16 +2461,16 @@
     <row r="41" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="C41" s="35">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D41" s="36">
-        <v>7513129.4539999999</v>
+        <v>7513132.6849999996</v>
       </c>
       <c r="E41" s="36">
-        <v>4691712.6560000004</v>
-      </c>
-      <c r="F41" s="56"/>
-      <c r="G41" s="56"/>
+        <v>4691707.6550000003</v>
+      </c>
+      <c r="F41" s="69"/>
+      <c r="G41" s="69"/>
       <c r="H41" s="37" t="s">
         <v>8</v>
       </c>
@@ -2480,16 +2480,16 @@
     <row r="42" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="C42" s="35">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="D42" s="36">
-        <v>7513129.1720000003</v>
+        <v>7513134.1550000003</v>
       </c>
       <c r="E42" s="36">
-        <v>4691712.0049999999</v>
-      </c>
-      <c r="F42" s="56"/>
-      <c r="G42" s="56"/>
+        <v>4691707.0219999999</v>
+      </c>
+      <c r="F42" s="69"/>
+      <c r="G42" s="69"/>
       <c r="H42" s="37" t="s">
         <v>8</v>
       </c>
@@ -2499,16 +2499,16 @@
     <row r="43" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="C43" s="35">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="D43" s="36">
-        <v>7513129.6200000001</v>
+        <v>7513135.8569999998</v>
       </c>
       <c r="E43" s="36">
-        <v>4691710.9950000001</v>
-      </c>
-      <c r="F43" s="56"/>
-      <c r="G43" s="56"/>
+        <v>4691707.7450000001</v>
+      </c>
+      <c r="F43" s="69"/>
+      <c r="G43" s="69"/>
       <c r="H43" s="37" t="s">
         <v>8</v>
       </c>
@@ -2518,16 +2518,16 @@
     <row r="44" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="C44" s="35">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="D44" s="36">
-        <v>7513132.6849999996</v>
+        <v>7513143.2529999996</v>
       </c>
       <c r="E44" s="36">
-        <v>4691707.6550000003</v>
-      </c>
-      <c r="F44" s="56"/>
-      <c r="G44" s="56"/>
+        <v>4691714.4639999997</v>
+      </c>
+      <c r="F44" s="69"/>
+      <c r="G44" s="69"/>
       <c r="H44" s="37" t="s">
         <v>8</v>
       </c>
@@ -2537,16 +2537,16 @@
     <row r="45" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="C45" s="35">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="D45" s="36">
-        <v>7513134.1550000003</v>
+        <v>7513138.2271999996</v>
       </c>
       <c r="E45" s="36">
-        <v>4691707.0219999999</v>
-      </c>
-      <c r="F45" s="56"/>
-      <c r="G45" s="56"/>
+        <v>4691719.9639999997</v>
+      </c>
+      <c r="F45" s="69"/>
+      <c r="G45" s="69"/>
       <c r="H45" s="37" t="s">
         <v>8</v>
       </c>
@@ -2556,16 +2556,16 @@
     <row r="46" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="C46" s="35">
-        <v>67</v>
+        <v>102</v>
       </c>
       <c r="D46" s="36">
-        <v>7513135.8569999998</v>
+        <v>7513134.8328999998</v>
       </c>
       <c r="E46" s="36">
-        <v>4691707.7450000001</v>
-      </c>
-      <c r="F46" s="56"/>
-      <c r="G46" s="56"/>
+        <v>4691717.6268999996</v>
+      </c>
+      <c r="F46" s="69"/>
+      <c r="G46" s="69"/>
       <c r="H46" s="37" t="s">
         <v>8</v>
       </c>
@@ -2575,16 +2575,16 @@
     <row r="47" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="C47" s="35">
-        <v>68</v>
+        <v>103</v>
       </c>
       <c r="D47" s="36">
-        <v>7513143.2529999996</v>
+        <v>7513135.2495999997</v>
       </c>
       <c r="E47" s="36">
-        <v>4691714.4639999997</v>
-      </c>
-      <c r="F47" s="56"/>
-      <c r="G47" s="56"/>
+        <v>4691717.1867000004</v>
+      </c>
+      <c r="F47" s="69"/>
+      <c r="G47" s="69"/>
       <c r="H47" s="37" t="s">
         <v>8</v>
       </c>
@@ -2594,16 +2594,16 @@
     <row r="48" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="C48" s="35">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D48" s="36">
-        <v>7513132.5939999996</v>
+        <v>7513131.2090999996</v>
       </c>
       <c r="E48" s="36">
-        <v>4691715.5387000004</v>
-      </c>
-      <c r="F48" s="56"/>
-      <c r="G48" s="56"/>
+        <v>4691717.4923</v>
+      </c>
+      <c r="F48" s="69"/>
+      <c r="G48" s="69"/>
       <c r="H48" s="37" t="s">
         <v>8</v>
       </c>
@@ -2613,16 +2613,16 @@
     <row r="49" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="C49" s="35">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="D49" s="36">
-        <v>7513131.9008999998</v>
+        <v>7513128.7640000004</v>
       </c>
       <c r="E49" s="36">
-        <v>4691716.2944</v>
-      </c>
-      <c r="F49" s="56"/>
-      <c r="G49" s="56"/>
+        <v>4691715.8310000002</v>
+      </c>
+      <c r="F49" s="69"/>
+      <c r="G49" s="69"/>
       <c r="H49" s="37" t="s">
         <v>8</v>
       </c>
@@ -2632,16 +2632,16 @@
     <row r="50" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="C50" s="35">
-        <v>103</v>
+        <v>9</v>
       </c>
       <c r="D50" s="36">
-        <v>7513132.1218999997</v>
+        <v>7513126.8399999999</v>
       </c>
       <c r="E50" s="36">
-        <v>4691716.4972000001</v>
-      </c>
-      <c r="F50" s="56"/>
-      <c r="G50" s="56"/>
+        <v>4691714.1189999999</v>
+      </c>
+      <c r="F50" s="69"/>
+      <c r="G50" s="69"/>
       <c r="H50" s="37" t="s">
         <v>8</v>
       </c>
@@ -2652,16 +2652,16 @@
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="6">
-        <v>104</v>
+        <v>10</v>
       </c>
       <c r="D51" s="7">
-        <v>7513131.2090999996</v>
+        <v>7513129.2566</v>
       </c>
       <c r="E51" s="7">
-        <v>4691717.4923</v>
-      </c>
-      <c r="F51" s="57"/>
-      <c r="G51" s="57"/>
+        <v>4691711.4588000001</v>
+      </c>
+      <c r="F51" s="70"/>
+      <c r="G51" s="70"/>
       <c r="H51" s="12" t="s">
         <v>8</v>
       </c>
@@ -2683,28 +2683,28 @@
     <row r="54" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
-      <c r="C54" s="58" t="s">
+      <c r="C54" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="D54" s="58"/>
-      <c r="E54" s="58"/>
-      <c r="F54" s="58"/>
-      <c r="G54" s="58"/>
-      <c r="H54" s="58"/>
-      <c r="I54" s="58"/>
+      <c r="D54" s="71"/>
+      <c r="E54" s="71"/>
+      <c r="F54" s="71"/>
+      <c r="G54" s="71"/>
+      <c r="H54" s="71"/>
+      <c r="I54" s="71"/>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
     </row>
     <row r="55" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
-      <c r="C55" s="58"/>
-      <c r="D55" s="58"/>
-      <c r="E55" s="58"/>
-      <c r="F55" s="58"/>
-      <c r="G55" s="58"/>
-      <c r="H55" s="58"/>
-      <c r="I55" s="58"/>
+      <c r="C55" s="71"/>
+      <c r="D55" s="71"/>
+      <c r="E55" s="71"/>
+      <c r="F55" s="71"/>
+      <c r="G55" s="71"/>
+      <c r="H55" s="71"/>
+      <c r="I55" s="71"/>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
     </row>
@@ -2775,141 +2775,141 @@
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
-      <c r="E66" s="61" t="s">
+      <c r="E66" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="F66" s="62"/>
-      <c r="G66" s="63"/>
-      <c r="H66" s="64" t="s">
+      <c r="F66" s="50"/>
+      <c r="G66" s="51"/>
+      <c r="H66" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="I66" s="65"/>
-      <c r="J66" s="68"/>
-      <c r="K66" s="69"/>
+      <c r="I66" s="53"/>
+      <c r="J66" s="56"/>
+      <c r="K66" s="57"/>
     </row>
     <row r="67" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="38" t="s">
+      <c r="A67" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B67" s="39"/>
-      <c r="C67" s="39"/>
-      <c r="D67" s="40"/>
-      <c r="E67" s="41">
+      <c r="B67" s="61"/>
+      <c r="C67" s="61"/>
+      <c r="D67" s="62"/>
+      <c r="E67" s="63">
         <v>152</v>
       </c>
-      <c r="F67" s="42"/>
-      <c r="G67" s="43"/>
-      <c r="H67" s="66"/>
-      <c r="I67" s="67"/>
-      <c r="J67" s="70"/>
-      <c r="K67" s="71"/>
+      <c r="F67" s="64"/>
+      <c r="G67" s="65"/>
+      <c r="H67" s="54"/>
+      <c r="I67" s="55"/>
+      <c r="J67" s="58"/>
+      <c r="K67" s="59"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="54"/>
-      <c r="B68" s="54"/>
-      <c r="C68" s="54"/>
-      <c r="D68" s="54"/>
-      <c r="E68" s="54"/>
-      <c r="F68" s="54"/>
-      <c r="G68" s="54"/>
-      <c r="H68" s="54"/>
-      <c r="I68" s="54"/>
-      <c r="J68" s="54"/>
-      <c r="K68" s="54"/>
+      <c r="A68" s="38"/>
+      <c r="B68" s="38"/>
+      <c r="C68" s="38"/>
+      <c r="D68" s="38"/>
+      <c r="E68" s="38"/>
+      <c r="F68" s="38"/>
+      <c r="G68" s="38"/>
+      <c r="H68" s="38"/>
+      <c r="I68" s="38"/>
+      <c r="J68" s="38"/>
+      <c r="K68" s="38"/>
     </row>
     <row r="69" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="54"/>
-      <c r="B69" s="54"/>
-      <c r="C69" s="54"/>
-      <c r="D69" s="54"/>
-      <c r="E69" s="54"/>
-      <c r="F69" s="54"/>
-      <c r="G69" s="54"/>
-      <c r="H69" s="54"/>
-      <c r="I69" s="54"/>
-      <c r="J69" s="54"/>
-      <c r="K69" s="54"/>
+      <c r="A69" s="38"/>
+      <c r="B69" s="38"/>
+      <c r="C69" s="38"/>
+      <c r="D69" s="38"/>
+      <c r="E69" s="38"/>
+      <c r="F69" s="38"/>
+      <c r="G69" s="38"/>
+      <c r="H69" s="38"/>
+      <c r="I69" s="38"/>
+      <c r="J69" s="38"/>
+      <c r="K69" s="38"/>
     </row>
     <row r="70" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="53" t="s">
+      <c r="A70" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="B70" s="53"/>
-      <c r="C70" s="53"/>
-      <c r="D70" s="53"/>
-      <c r="E70" s="53"/>
-      <c r="F70" s="53"/>
-      <c r="G70" s="53"/>
-      <c r="H70" s="53"/>
-      <c r="I70" s="53"/>
-      <c r="J70" s="53"/>
-      <c r="K70" s="53"/>
+      <c r="B70" s="39"/>
+      <c r="C70" s="39"/>
+      <c r="D70" s="39"/>
+      <c r="E70" s="39"/>
+      <c r="F70" s="39"/>
+      <c r="G70" s="39"/>
+      <c r="H70" s="39"/>
+      <c r="I70" s="39"/>
+      <c r="J70" s="39"/>
+      <c r="K70" s="39"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="53"/>
-      <c r="B71" s="53"/>
-      <c r="C71" s="53"/>
-      <c r="D71" s="53"/>
-      <c r="E71" s="53"/>
-      <c r="F71" s="53"/>
-      <c r="G71" s="53"/>
-      <c r="H71" s="53"/>
-      <c r="I71" s="53"/>
-      <c r="J71" s="53"/>
-      <c r="K71" s="53"/>
+      <c r="A71" s="39"/>
+      <c r="B71" s="39"/>
+      <c r="C71" s="39"/>
+      <c r="D71" s="39"/>
+      <c r="E71" s="39"/>
+      <c r="F71" s="39"/>
+      <c r="G71" s="39"/>
+      <c r="H71" s="39"/>
+      <c r="I71" s="39"/>
+      <c r="J71" s="39"/>
+      <c r="K71" s="39"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" s="53"/>
-      <c r="B72" s="53"/>
-      <c r="C72" s="53"/>
-      <c r="D72" s="53"/>
-      <c r="E72" s="53"/>
-      <c r="F72" s="53"/>
-      <c r="G72" s="53"/>
-      <c r="H72" s="53"/>
-      <c r="I72" s="53"/>
-      <c r="J72" s="53"/>
-      <c r="K72" s="53"/>
+      <c r="A72" s="39"/>
+      <c r="B72" s="39"/>
+      <c r="C72" s="39"/>
+      <c r="D72" s="39"/>
+      <c r="E72" s="39"/>
+      <c r="F72" s="39"/>
+      <c r="G72" s="39"/>
+      <c r="H72" s="39"/>
+      <c r="I72" s="39"/>
+      <c r="J72" s="39"/>
+      <c r="K72" s="39"/>
     </row>
     <row r="73" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="53"/>
-      <c r="B73" s="53"/>
-      <c r="C73" s="53"/>
-      <c r="D73" s="53"/>
-      <c r="E73" s="53"/>
-      <c r="F73" s="53"/>
-      <c r="G73" s="53"/>
-      <c r="H73" s="53"/>
-      <c r="I73" s="53"/>
-      <c r="J73" s="53"/>
-      <c r="K73" s="53"/>
+      <c r="A73" s="39"/>
+      <c r="B73" s="39"/>
+      <c r="C73" s="39"/>
+      <c r="D73" s="39"/>
+      <c r="E73" s="39"/>
+      <c r="F73" s="39"/>
+      <c r="G73" s="39"/>
+      <c r="H73" s="39"/>
+      <c r="I73" s="39"/>
+      <c r="J73" s="39"/>
+      <c r="K73" s="39"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C74" s="44"/>
-      <c r="D74" s="45"/>
-      <c r="E74" s="45"/>
-      <c r="F74" s="45"/>
-      <c r="G74" s="45"/>
-      <c r="H74" s="45"/>
-      <c r="I74" s="46"/>
+      <c r="C74" s="40"/>
+      <c r="D74" s="41"/>
+      <c r="E74" s="41"/>
+      <c r="F74" s="41"/>
+      <c r="G74" s="41"/>
+      <c r="H74" s="41"/>
+      <c r="I74" s="42"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C75" s="47"/>
-      <c r="D75" s="48"/>
-      <c r="E75" s="48"/>
-      <c r="F75" s="48"/>
-      <c r="G75" s="48"/>
-      <c r="H75" s="48"/>
-      <c r="I75" s="49"/>
+      <c r="C75" s="43"/>
+      <c r="D75" s="44"/>
+      <c r="E75" s="44"/>
+      <c r="F75" s="44"/>
+      <c r="G75" s="44"/>
+      <c r="H75" s="44"/>
+      <c r="I75" s="45"/>
     </row>
     <row r="76" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C76" s="50"/>
-      <c r="D76" s="51"/>
-      <c r="E76" s="51"/>
-      <c r="F76" s="51"/>
-      <c r="G76" s="51"/>
-      <c r="H76" s="51"/>
-      <c r="I76" s="52"/>
+      <c r="C76" s="46"/>
+      <c r="D76" s="47"/>
+      <c r="E76" s="47"/>
+      <c r="F76" s="47"/>
+      <c r="G76" s="47"/>
+      <c r="H76" s="47"/>
+      <c r="I76" s="48"/>
     </row>
     <row r="77" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
@@ -2946,10 +2946,10 @@
       <c r="E78" s="4">
         <v>4691722.8739999998</v>
       </c>
-      <c r="F78" s="59">
+      <c r="F78" s="66">
         <v>623.17399999999998</v>
       </c>
-      <c r="G78" s="59" t="s">
+      <c r="G78" s="66" t="s">
         <v>20</v>
       </c>
       <c r="H78" s="26" t="s">
@@ -2970,8 +2970,8 @@
       <c r="E79" s="4">
         <v>4691720.0990000004</v>
       </c>
-      <c r="F79" s="59"/>
-      <c r="G79" s="59"/>
+      <c r="F79" s="66"/>
+      <c r="G79" s="66"/>
       <c r="H79" s="26" t="s">
         <v>8</v>
       </c>
@@ -2990,8 +2990,8 @@
       <c r="E80" s="4">
         <v>4691715.5049999999</v>
       </c>
-      <c r="F80" s="59"/>
-      <c r="G80" s="59"/>
+      <c r="F80" s="66"/>
+      <c r="G80" s="66"/>
       <c r="H80" s="26" t="s">
         <v>8</v>
       </c>
@@ -3010,8 +3010,8 @@
       <c r="E81" s="4">
         <v>4691719.318</v>
       </c>
-      <c r="F81" s="59"/>
-      <c r="G81" s="59"/>
+      <c r="F81" s="66"/>
+      <c r="G81" s="66"/>
       <c r="H81" s="26" t="s">
         <v>8</v>
       </c>
@@ -3030,8 +3030,8 @@
       <c r="E82" s="4">
         <v>4691713.9479999999</v>
       </c>
-      <c r="F82" s="59"/>
-      <c r="G82" s="59"/>
+      <c r="F82" s="66"/>
+      <c r="G82" s="66"/>
       <c r="H82" s="26" t="s">
         <v>8</v>
       </c>
@@ -3050,8 +3050,8 @@
       <c r="E83" s="4">
         <v>4691712.1909999996</v>
       </c>
-      <c r="F83" s="59"/>
-      <c r="G83" s="59"/>
+      <c r="F83" s="66"/>
+      <c r="G83" s="66"/>
       <c r="H83" s="26" t="s">
         <v>8</v>
       </c>
@@ -3070,8 +3070,8 @@
       <c r="E84" s="4">
         <v>4691711.0889999997</v>
       </c>
-      <c r="F84" s="59"/>
-      <c r="G84" s="59"/>
+      <c r="F84" s="66"/>
+      <c r="G84" s="66"/>
       <c r="H84" s="26" t="s">
         <v>8</v>
       </c>
@@ -3090,8 +3090,8 @@
       <c r="E85" s="4">
         <v>4691706.8949999996</v>
       </c>
-      <c r="F85" s="59"/>
-      <c r="G85" s="59"/>
+      <c r="F85" s="66"/>
+      <c r="G85" s="66"/>
       <c r="H85" s="26" t="s">
         <v>8</v>
       </c>
@@ -3110,8 +3110,8 @@
       <c r="E86" s="4">
         <v>4691706.18</v>
       </c>
-      <c r="F86" s="59"/>
-      <c r="G86" s="59"/>
+      <c r="F86" s="66"/>
+      <c r="G86" s="66"/>
       <c r="H86" s="26" t="s">
         <v>8</v>
       </c>
@@ -3130,8 +3130,8 @@
       <c r="E87" s="4">
         <v>4691706.1939000003</v>
       </c>
-      <c r="F87" s="59"/>
-      <c r="G87" s="59"/>
+      <c r="F87" s="66"/>
+      <c r="G87" s="66"/>
       <c r="H87" s="26" t="s">
         <v>8</v>
       </c>
@@ -3150,8 +3150,8 @@
       <c r="E88" s="4">
         <v>4691707.7450000001</v>
       </c>
-      <c r="F88" s="59"/>
-      <c r="G88" s="59"/>
+      <c r="F88" s="66"/>
+      <c r="G88" s="66"/>
       <c r="H88" s="26" t="s">
         <v>8</v>
       </c>
@@ -3170,8 +3170,8 @@
       <c r="E89" s="4">
         <v>4691714.4639999997</v>
       </c>
-      <c r="F89" s="59"/>
-      <c r="G89" s="59"/>
+      <c r="F89" s="66"/>
+      <c r="G89" s="66"/>
       <c r="H89" s="26" t="s">
         <v>8</v>
       </c>
@@ -3190,8 +3190,8 @@
       <c r="E90" s="4">
         <v>4691715.8525</v>
       </c>
-      <c r="F90" s="59"/>
-      <c r="G90" s="59"/>
+      <c r="F90" s="66"/>
+      <c r="G90" s="66"/>
       <c r="H90" s="26" t="s">
         <v>8</v>
       </c>
@@ -3210,8 +3210,8 @@
       <c r="E91" s="4">
         <v>4691712.5202000001</v>
       </c>
-      <c r="F91" s="59"/>
-      <c r="G91" s="59"/>
+      <c r="F91" s="66"/>
+      <c r="G91" s="66"/>
       <c r="H91" s="26" t="s">
         <v>8</v>
       </c>
@@ -3231,8 +3231,8 @@
       <c r="E92" s="7">
         <v>4691715.9907</v>
       </c>
-      <c r="F92" s="60"/>
-      <c r="G92" s="60"/>
+      <c r="F92" s="67"/>
+      <c r="G92" s="67"/>
       <c r="H92" s="27" t="s">
         <v>8</v>
       </c>
@@ -3290,10 +3290,10 @@
       <c r="E95" s="4">
         <v>4691722.8739999998</v>
       </c>
-      <c r="F95" s="59">
+      <c r="F95" s="66">
         <v>626.09400000000005</v>
       </c>
-      <c r="G95" s="59" t="s">
+      <c r="G95" s="66" t="s">
         <v>23</v>
       </c>
       <c r="H95" s="26" t="s">
@@ -3315,8 +3315,8 @@
       <c r="E96" s="4">
         <v>4691720.0990000004</v>
       </c>
-      <c r="F96" s="59"/>
-      <c r="G96" s="59"/>
+      <c r="F96" s="66"/>
+      <c r="G96" s="66"/>
       <c r="H96" s="26" t="s">
         <v>8</v>
       </c>
@@ -3336,8 +3336,8 @@
       <c r="E97" s="4">
         <v>4691715.5049999999</v>
       </c>
-      <c r="F97" s="59"/>
-      <c r="G97" s="59"/>
+      <c r="F97" s="66"/>
+      <c r="G97" s="66"/>
       <c r="H97" s="26" t="s">
         <v>8</v>
       </c>
@@ -3357,8 +3357,8 @@
       <c r="E98" s="4">
         <v>4691719.318</v>
       </c>
-      <c r="F98" s="59"/>
-      <c r="G98" s="59"/>
+      <c r="F98" s="66"/>
+      <c r="G98" s="66"/>
       <c r="H98" s="26" t="s">
         <v>8</v>
       </c>
@@ -3378,8 +3378,8 @@
       <c r="E99" s="4">
         <v>4691713.9479999999</v>
       </c>
-      <c r="F99" s="59"/>
-      <c r="G99" s="59"/>
+      <c r="F99" s="66"/>
+      <c r="G99" s="66"/>
       <c r="H99" s="26" t="s">
         <v>8</v>
       </c>
@@ -3399,8 +3399,8 @@
       <c r="E100" s="4">
         <v>4691712.1909999996</v>
       </c>
-      <c r="F100" s="59"/>
-      <c r="G100" s="59"/>
+      <c r="F100" s="66"/>
+      <c r="G100" s="66"/>
       <c r="H100" s="26" t="s">
         <v>8</v>
       </c>
@@ -3420,8 +3420,8 @@
       <c r="E101" s="4">
         <v>4691711.0889999997</v>
       </c>
-      <c r="F101" s="59"/>
-      <c r="G101" s="59"/>
+      <c r="F101" s="66"/>
+      <c r="G101" s="66"/>
       <c r="H101" s="26" t="s">
         <v>8</v>
       </c>
@@ -3441,8 +3441,8 @@
       <c r="E102" s="4">
         <v>4691706.8949999996</v>
       </c>
-      <c r="F102" s="59"/>
-      <c r="G102" s="59"/>
+      <c r="F102" s="66"/>
+      <c r="G102" s="66"/>
       <c r="H102" s="26" t="s">
         <v>8</v>
       </c>
@@ -3462,8 +3462,8 @@
       <c r="E103" s="4">
         <v>4691706.18</v>
       </c>
-      <c r="F103" s="59"/>
-      <c r="G103" s="59"/>
+      <c r="F103" s="66"/>
+      <c r="G103" s="66"/>
       <c r="H103" s="26" t="s">
         <v>8</v>
       </c>
@@ -3483,8 +3483,8 @@
       <c r="E104" s="4">
         <v>4691706.1939000003</v>
       </c>
-      <c r="F104" s="59"/>
-      <c r="G104" s="59"/>
+      <c r="F104" s="66"/>
+      <c r="G104" s="66"/>
       <c r="H104" s="26" t="s">
         <v>8</v>
       </c>
@@ -3504,8 +3504,8 @@
       <c r="E105" s="4">
         <v>4691707.7450000001</v>
       </c>
-      <c r="F105" s="59"/>
-      <c r="G105" s="59"/>
+      <c r="F105" s="66"/>
+      <c r="G105" s="66"/>
       <c r="H105" s="26" t="s">
         <v>8</v>
       </c>
@@ -3525,8 +3525,8 @@
       <c r="E106" s="4">
         <v>4691714.4639999997</v>
       </c>
-      <c r="F106" s="59"/>
-      <c r="G106" s="59"/>
+      <c r="F106" s="66"/>
+      <c r="G106" s="66"/>
       <c r="H106" s="26" t="s">
         <v>8</v>
       </c>
@@ -3546,8 +3546,8 @@
       <c r="E107" s="4">
         <v>4691715.8525</v>
       </c>
-      <c r="F107" s="59"/>
-      <c r="G107" s="59"/>
+      <c r="F107" s="66"/>
+      <c r="G107" s="66"/>
       <c r="H107" s="26" t="s">
         <v>8</v>
       </c>
@@ -3567,8 +3567,8 @@
       <c r="E108" s="4">
         <v>4691712.5202000001</v>
       </c>
-      <c r="F108" s="59"/>
-      <c r="G108" s="59"/>
+      <c r="F108" s="66"/>
+      <c r="G108" s="66"/>
       <c r="H108" s="26" t="s">
         <v>8</v>
       </c>
@@ -3588,8 +3588,8 @@
       <c r="E109" s="7">
         <v>4691715.9907</v>
       </c>
-      <c r="F109" s="60"/>
-      <c r="G109" s="60"/>
+      <c r="F109" s="67"/>
+      <c r="G109" s="67"/>
       <c r="H109" s="27" t="s">
         <v>8</v>
       </c>
@@ -3647,10 +3647,10 @@
       <c r="E112" s="4">
         <v>4691714.3306</v>
       </c>
-      <c r="F112" s="59">
+      <c r="F112" s="66">
         <v>629.29999999999995</v>
       </c>
-      <c r="G112" s="59" t="s">
+      <c r="G112" s="66" t="s">
         <v>24</v>
       </c>
       <c r="H112" s="26" t="s">
@@ -3672,8 +3672,8 @@
       <c r="E113" s="4">
         <v>4691713.9479999999</v>
       </c>
-      <c r="F113" s="59"/>
-      <c r="G113" s="59"/>
+      <c r="F113" s="66"/>
+      <c r="G113" s="66"/>
       <c r="H113" s="26" t="s">
         <v>8</v>
       </c>
@@ -3693,8 +3693,8 @@
       <c r="E114" s="4">
         <v>4691712.3039999995</v>
       </c>
-      <c r="F114" s="59"/>
-      <c r="G114" s="59"/>
+      <c r="F114" s="66"/>
+      <c r="G114" s="66"/>
       <c r="H114" s="26" t="s">
         <v>8</v>
       </c>
@@ -3714,8 +3714,8 @@
       <c r="E115" s="4">
         <v>4691711.0889999997</v>
       </c>
-      <c r="F115" s="59"/>
-      <c r="G115" s="59"/>
+      <c r="F115" s="66"/>
+      <c r="G115" s="66"/>
       <c r="H115" s="26" t="s">
         <v>8</v>
       </c>
@@ -3735,8 +3735,8 @@
       <c r="E116" s="4">
         <v>4691706.8949999996</v>
       </c>
-      <c r="F116" s="59"/>
-      <c r="G116" s="59"/>
+      <c r="F116" s="66"/>
+      <c r="G116" s="66"/>
       <c r="H116" s="26" t="s">
         <v>8</v>
       </c>
@@ -3756,8 +3756,8 @@
       <c r="E117" s="4">
         <v>4691706.6350999996</v>
       </c>
-      <c r="F117" s="59"/>
-      <c r="G117" s="59"/>
+      <c r="F117" s="66"/>
+      <c r="G117" s="66"/>
       <c r="H117" s="26" t="s">
         <v>8</v>
       </c>
@@ -3777,8 +3777,8 @@
       <c r="E118" s="4">
         <v>4691706.1939000003</v>
       </c>
-      <c r="F118" s="59"/>
-      <c r="G118" s="59"/>
+      <c r="F118" s="66"/>
+      <c r="G118" s="66"/>
       <c r="H118" s="26" t="s">
         <v>8</v>
       </c>
@@ -3798,8 +3798,8 @@
       <c r="E119" s="4">
         <v>4691720.0990000004</v>
       </c>
-      <c r="F119" s="59"/>
-      <c r="G119" s="59"/>
+      <c r="F119" s="66"/>
+      <c r="G119" s="66"/>
       <c r="H119" s="26" t="s">
         <v>8</v>
       </c>
@@ -3819,8 +3819,8 @@
       <c r="E120" s="4">
         <v>4691719.3229999999</v>
       </c>
-      <c r="F120" s="59"/>
-      <c r="G120" s="59"/>
+      <c r="F120" s="66"/>
+      <c r="G120" s="66"/>
       <c r="H120" s="26" t="s">
         <v>8</v>
       </c>
@@ -3840,8 +3840,8 @@
       <c r="E121" s="4">
         <v>4691722.8739999998</v>
       </c>
-      <c r="F121" s="59"/>
-      <c r="G121" s="59"/>
+      <c r="F121" s="66"/>
+      <c r="G121" s="66"/>
       <c r="H121" s="26" t="s">
         <v>8</v>
       </c>
@@ -3861,8 +3861,8 @@
       <c r="E122" s="4">
         <v>4691715.7680000002</v>
       </c>
-      <c r="F122" s="59"/>
-      <c r="G122" s="59"/>
+      <c r="F122" s="66"/>
+      <c r="G122" s="66"/>
       <c r="H122" s="26" t="s">
         <v>8</v>
       </c>
@@ -3882,8 +3882,8 @@
       <c r="E123" s="4">
         <v>4691714.4639999997</v>
       </c>
-      <c r="F123" s="59"/>
-      <c r="G123" s="59"/>
+      <c r="F123" s="66"/>
+      <c r="G123" s="66"/>
       <c r="H123" s="26" t="s">
         <v>8</v>
       </c>
@@ -3903,8 +3903,8 @@
       <c r="E124" s="4">
         <v>4691708.2016000003</v>
       </c>
-      <c r="F124" s="59"/>
-      <c r="G124" s="59"/>
+      <c r="F124" s="66"/>
+      <c r="G124" s="66"/>
       <c r="H124" s="26" t="s">
         <v>8</v>
       </c>
@@ -3924,8 +3924,8 @@
       <c r="E125" s="4">
         <v>4691706.2857999997</v>
       </c>
-      <c r="F125" s="59"/>
-      <c r="G125" s="59"/>
+      <c r="F125" s="66"/>
+      <c r="G125" s="66"/>
       <c r="H125" s="26" t="s">
         <v>8</v>
       </c>
@@ -3945,8 +3945,8 @@
       <c r="E126" s="4">
         <v>4691717.4736000001</v>
       </c>
-      <c r="F126" s="59"/>
-      <c r="G126" s="59"/>
+      <c r="F126" s="66"/>
+      <c r="G126" s="66"/>
       <c r="H126" s="26" t="s">
         <v>8</v>
       </c>
@@ -3966,8 +3966,8 @@
       <c r="E127" s="4">
         <v>4691713.8247999996</v>
       </c>
-      <c r="F127" s="59"/>
-      <c r="G127" s="59"/>
+      <c r="F127" s="66"/>
+      <c r="G127" s="66"/>
       <c r="H127" s="26" t="s">
         <v>8</v>
       </c>
@@ -3987,8 +3987,8 @@
       <c r="E128" s="7">
         <v>4691719.4106000001</v>
       </c>
-      <c r="F128" s="60"/>
-      <c r="G128" s="60"/>
+      <c r="F128" s="67"/>
+      <c r="G128" s="67"/>
       <c r="H128" s="27" t="s">
         <v>8</v>
       </c>
@@ -4003,37 +4003,48 @@
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
       <c r="D129" s="3"/>
-      <c r="E129" s="61" t="s">
+      <c r="E129" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="F129" s="62"/>
-      <c r="G129" s="63"/>
-      <c r="H129" s="64" t="s">
+      <c r="F129" s="50"/>
+      <c r="G129" s="51"/>
+      <c r="H129" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="I129" s="65"/>
-      <c r="J129" s="68"/>
-      <c r="K129" s="69"/>
+      <c r="I129" s="53"/>
+      <c r="J129" s="56"/>
+      <c r="K129" s="57"/>
     </row>
     <row r="130" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A130" s="38" t="s">
+      <c r="A130" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B130" s="39"/>
-      <c r="C130" s="39"/>
-      <c r="D130" s="40"/>
-      <c r="E130" s="41">
+      <c r="B130" s="61"/>
+      <c r="C130" s="61"/>
+      <c r="D130" s="62"/>
+      <c r="E130" s="63">
         <v>152</v>
       </c>
-      <c r="F130" s="42"/>
-      <c r="G130" s="43"/>
-      <c r="H130" s="66"/>
-      <c r="I130" s="67"/>
-      <c r="J130" s="70"/>
-      <c r="K130" s="71"/>
+      <c r="F130" s="64"/>
+      <c r="G130" s="65"/>
+      <c r="H130" s="54"/>
+      <c r="I130" s="55"/>
+      <c r="J130" s="58"/>
+      <c r="K130" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A67:D67"/>
+    <mergeCell ref="E67:G67"/>
+    <mergeCell ref="C8:I10"/>
+    <mergeCell ref="A3:K6"/>
+    <mergeCell ref="A1:K2"/>
+    <mergeCell ref="F33:F51"/>
+    <mergeCell ref="G33:G51"/>
+    <mergeCell ref="C54:I55"/>
+    <mergeCell ref="E66:G66"/>
+    <mergeCell ref="H66:I67"/>
+    <mergeCell ref="J66:K67"/>
     <mergeCell ref="A68:K69"/>
     <mergeCell ref="A70:K73"/>
     <mergeCell ref="C74:I76"/>
@@ -4046,19 +4057,8 @@
     <mergeCell ref="G95:G109"/>
     <mergeCell ref="F112:F128"/>
     <mergeCell ref="G112:G128"/>
-    <mergeCell ref="A67:D67"/>
-    <mergeCell ref="E67:G67"/>
-    <mergeCell ref="C8:I10"/>
-    <mergeCell ref="A3:K6"/>
-    <mergeCell ref="A1:K2"/>
-    <mergeCell ref="F33:F51"/>
-    <mergeCell ref="G33:G51"/>
-    <mergeCell ref="C54:I55"/>
     <mergeCell ref="F78:F92"/>
     <mergeCell ref="G78:G92"/>
-    <mergeCell ref="E66:G66"/>
-    <mergeCell ref="H66:I67"/>
-    <mergeCell ref="J66:K67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="60" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
kati 1 njestite permirsaim
</commit_message>
<xml_diff>
--- a/5-Njësite-banesore/regjistri/22-Koordinatat-për-pjesë-të-ndertesës.xlsx-2602-0-Albnori.xlsx
+++ b/5-Njësite-banesore/regjistri/22-Koordinatat-për-pjesë-të-ndertesës.xlsx-2602-0-Albnori.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="25">
   <si>
     <t>Nr</t>
   </si>
@@ -597,7 +597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -657,19 +657,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1749,8 +1741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K130"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A29" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="N35" sqref="M33:Q51"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A118" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="Q91" sqref="Q91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1766,112 +1758,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38"/>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
+      <c r="A1" s="34"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
     </row>
     <row r="2" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
     </row>
     <row r="4" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="40"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="42"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="38"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="43"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="45"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="41"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="46"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="48"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="44"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
@@ -1990,278 +1982,278 @@
       </c>
     </row>
     <row r="18" spans="3:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C18" s="31">
+      <c r="C18" s="27">
         <v>11</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="28">
         <v>7513130.5959999999</v>
       </c>
-      <c r="E18" s="32">
+      <c r="E18" s="28">
         <v>4691713.7060000002</v>
       </c>
-      <c r="F18" s="32">
+      <c r="F18" s="28">
         <v>620.11199999999997</v>
       </c>
-      <c r="G18" s="33">
+      <c r="G18" s="29">
         <v>40</v>
       </c>
-      <c r="H18" s="33" t="s">
+      <c r="H18" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I18" s="34" t="s">
+      <c r="I18" s="30" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="3:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C19" s="31">
+      <c r="C19" s="27">
         <v>12</v>
       </c>
-      <c r="D19" s="32">
+      <c r="D19" s="28">
         <v>7513129.4539999999</v>
       </c>
-      <c r="E19" s="32">
+      <c r="E19" s="28">
         <v>4691712.6560000004</v>
       </c>
-      <c r="F19" s="32">
+      <c r="F19" s="28">
         <v>620.11199999999997</v>
       </c>
-      <c r="G19" s="33">
+      <c r="G19" s="29">
         <v>40</v>
       </c>
-      <c r="H19" s="33" t="s">
+      <c r="H19" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I19" s="34" t="s">
+      <c r="I19" s="30" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="20" spans="3:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C20" s="31">
+      <c r="C20" s="27">
         <v>13</v>
       </c>
-      <c r="D20" s="32">
+      <c r="D20" s="28">
         <v>7513129.1720000003</v>
       </c>
-      <c r="E20" s="32">
+      <c r="E20" s="28">
         <v>4691712.0049999999</v>
       </c>
-      <c r="F20" s="32">
+      <c r="F20" s="28">
         <v>620.11199999999997</v>
       </c>
-      <c r="G20" s="33">
+      <c r="G20" s="29">
         <v>40</v>
       </c>
-      <c r="H20" s="33" t="s">
+      <c r="H20" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I20" s="34" t="s">
+      <c r="I20" s="30" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="3:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C21" s="31">
+      <c r="C21" s="27">
         <v>14</v>
       </c>
-      <c r="D21" s="32">
+      <c r="D21" s="28">
         <v>7513129.6200000001</v>
       </c>
-      <c r="E21" s="32">
+      <c r="E21" s="28">
         <v>4691710.9950000001</v>
       </c>
-      <c r="F21" s="32">
+      <c r="F21" s="28">
         <v>620.11199999999997</v>
       </c>
-      <c r="G21" s="33">
+      <c r="G21" s="29">
         <v>40</v>
       </c>
-      <c r="H21" s="33" t="s">
+      <c r="H21" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I21" s="34" t="s">
+      <c r="I21" s="30" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="22" spans="3:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C22" s="31">
+      <c r="C22" s="27">
         <v>15</v>
       </c>
-      <c r="D22" s="32">
+      <c r="D22" s="28">
         <v>7513132.6849999996</v>
       </c>
-      <c r="E22" s="32">
+      <c r="E22" s="28">
         <v>4691707.6550000003</v>
       </c>
-      <c r="F22" s="32">
+      <c r="F22" s="28">
         <v>620.11199999999997</v>
       </c>
-      <c r="G22" s="33">
+      <c r="G22" s="29">
         <v>40</v>
       </c>
-      <c r="H22" s="33" t="s">
+      <c r="H22" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I22" s="34" t="s">
+      <c r="I22" s="30" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="3:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C23" s="31">
+      <c r="C23" s="27">
         <v>65</v>
       </c>
-      <c r="D23" s="32">
+      <c r="D23" s="28">
         <v>7513134.1550000003</v>
       </c>
-      <c r="E23" s="32">
+      <c r="E23" s="28">
         <v>4691707.0219999999</v>
       </c>
-      <c r="F23" s="32">
+      <c r="F23" s="28">
         <v>620.11199999999997</v>
       </c>
-      <c r="G23" s="33">
+      <c r="G23" s="29">
         <v>40</v>
       </c>
-      <c r="H23" s="33" t="s">
+      <c r="H23" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I23" s="34" t="s">
+      <c r="I23" s="30" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="24" spans="3:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C24" s="31">
+      <c r="C24" s="27">
         <v>67</v>
       </c>
-      <c r="D24" s="32">
+      <c r="D24" s="28">
         <v>7513135.8569999998</v>
       </c>
-      <c r="E24" s="32">
+      <c r="E24" s="28">
         <v>4691707.7450000001</v>
       </c>
-      <c r="F24" s="32">
+      <c r="F24" s="28">
         <v>620.11199999999997</v>
       </c>
-      <c r="G24" s="33">
+      <c r="G24" s="29">
         <v>40</v>
       </c>
-      <c r="H24" s="33" t="s">
+      <c r="H24" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I24" s="34" t="s">
+      <c r="I24" s="30" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="25" spans="3:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C25" s="31">
+      <c r="C25" s="27">
         <v>68</v>
       </c>
-      <c r="D25" s="32">
+      <c r="D25" s="28">
         <v>7513143.2529999996</v>
       </c>
-      <c r="E25" s="32">
+      <c r="E25" s="28">
         <v>4691714.4639999997</v>
       </c>
-      <c r="F25" s="32">
+      <c r="F25" s="28">
         <v>620.11199999999997</v>
       </c>
-      <c r="G25" s="33">
+      <c r="G25" s="29">
         <v>40</v>
       </c>
-      <c r="H25" s="33" t="s">
+      <c r="H25" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I25" s="34" t="s">
+      <c r="I25" s="30" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="26" spans="3:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C26" s="31">
-        <v>8</v>
-      </c>
-      <c r="D26" s="32">
+      <c r="C26" s="27">
+        <v>8</v>
+      </c>
+      <c r="D26" s="28">
         <v>7513128.7640000004</v>
       </c>
-      <c r="E26" s="32">
+      <c r="E26" s="28">
         <v>4691715.8310000002</v>
       </c>
-      <c r="F26" s="32">
+      <c r="F26" s="28">
         <v>620.11199999999997</v>
       </c>
-      <c r="G26" s="33">
+      <c r="G26" s="29">
         <v>40</v>
       </c>
-      <c r="H26" s="33" t="s">
+      <c r="H26" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I26" s="34" t="s">
+      <c r="I26" s="30" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="27" spans="3:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C27" s="31">
+      <c r="C27" s="27">
         <v>9</v>
       </c>
-      <c r="D27" s="32">
+      <c r="D27" s="28">
         <v>7513126.8399999999</v>
       </c>
-      <c r="E27" s="32">
+      <c r="E27" s="28">
         <v>4691714.1189999999</v>
       </c>
-      <c r="F27" s="32">
+      <c r="F27" s="28">
         <v>620.11199999999997</v>
       </c>
-      <c r="G27" s="33">
+      <c r="G27" s="29">
         <v>40</v>
       </c>
-      <c r="H27" s="33" t="s">
+      <c r="H27" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I27" s="34" t="s">
+      <c r="I27" s="30" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="28" spans="3:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C28" s="31">
+      <c r="C28" s="27">
         <v>10</v>
       </c>
-      <c r="D28" s="32">
+      <c r="D28" s="28">
         <v>7513129.2566</v>
       </c>
-      <c r="E28" s="32">
+      <c r="E28" s="28">
         <v>4691711.4588000001</v>
       </c>
-      <c r="F28" s="32">
+      <c r="F28" s="28">
         <v>620.11199999999997</v>
       </c>
-      <c r="G28" s="33">
+      <c r="G28" s="29">
         <v>40</v>
       </c>
-      <c r="H28" s="33" t="s">
+      <c r="H28" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I28" s="34" t="s">
+      <c r="I28" s="30" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="29" spans="3:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C29" s="31">
+      <c r="C29" s="27">
         <v>98</v>
       </c>
-      <c r="D29" s="32">
+      <c r="D29" s="28">
         <v>7513129.7910000002</v>
       </c>
-      <c r="E29" s="32">
+      <c r="E29" s="28">
         <v>4691714.6054999996</v>
       </c>
-      <c r="F29" s="32">
+      <c r="F29" s="28">
         <v>620.11199999999997</v>
       </c>
-      <c r="G29" s="33">
+      <c r="G29" s="29">
         <v>40</v>
       </c>
-      <c r="H29" s="33" t="s">
+      <c r="H29" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I29" s="34" t="s">
+      <c r="I29" s="30" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2322,10 +2314,10 @@
       <c r="E33" s="4">
         <v>4691722.8739999998</v>
       </c>
-      <c r="F33" s="68">
+      <c r="F33" s="64">
         <v>620.11199999999997</v>
       </c>
-      <c r="G33" s="68" t="s">
+      <c r="G33" s="64" t="s">
         <v>11</v>
       </c>
       <c r="H33" s="11" t="s">
@@ -2343,8 +2335,8 @@
       <c r="E34" s="4">
         <v>4691720.0990000004</v>
       </c>
-      <c r="F34" s="68"/>
-      <c r="G34" s="68"/>
+      <c r="F34" s="64"/>
+      <c r="G34" s="64"/>
       <c r="H34" s="11" t="s">
         <v>8</v>
       </c>
@@ -2360,8 +2352,8 @@
       <c r="E35" s="4">
         <v>4691719.3229999999</v>
       </c>
-      <c r="F35" s="68"/>
-      <c r="G35" s="68"/>
+      <c r="F35" s="64"/>
+      <c r="G35" s="64"/>
       <c r="H35" s="11" t="s">
         <v>8</v>
       </c>
@@ -2377,8 +2369,8 @@
       <c r="E36" s="4">
         <v>4691715.5049999999</v>
       </c>
-      <c r="F36" s="68"/>
-      <c r="G36" s="68"/>
+      <c r="F36" s="64"/>
+      <c r="G36" s="64"/>
       <c r="H36" s="11" t="s">
         <v>8</v>
       </c>
@@ -2394,8 +2386,8 @@
       <c r="E37" s="4">
         <v>4691713.7060000002</v>
       </c>
-      <c r="F37" s="68"/>
-      <c r="G37" s="68"/>
+      <c r="F37" s="64"/>
+      <c r="G37" s="64"/>
       <c r="H37" s="11" t="s">
         <v>8</v>
       </c>
@@ -2412,8 +2404,8 @@
       <c r="E38" s="4">
         <v>4691712.6560000004</v>
       </c>
-      <c r="F38" s="68"/>
-      <c r="G38" s="68"/>
+      <c r="F38" s="64"/>
+      <c r="G38" s="64"/>
       <c r="H38" s="11" t="s">
         <v>8</v>
       </c>
@@ -2431,8 +2423,8 @@
       <c r="E39" s="4">
         <v>4691712.0049999999</v>
       </c>
-      <c r="F39" s="68"/>
-      <c r="G39" s="68"/>
+      <c r="F39" s="64"/>
+      <c r="G39" s="64"/>
       <c r="H39" s="11" t="s">
         <v>8</v>
       </c>
@@ -2450,8 +2442,8 @@
       <c r="E40" s="4">
         <v>4691710.9950000001</v>
       </c>
-      <c r="F40" s="68"/>
-      <c r="G40" s="68"/>
+      <c r="F40" s="64"/>
+      <c r="G40" s="64"/>
       <c r="H40" s="11" t="s">
         <v>8</v>
       </c>
@@ -2460,18 +2452,18 @@
     </row>
     <row r="41" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
-      <c r="C41" s="35">
+      <c r="C41" s="31">
         <v>15</v>
       </c>
-      <c r="D41" s="36">
+      <c r="D41" s="32">
         <v>7513132.6849999996</v>
       </c>
-      <c r="E41" s="36">
+      <c r="E41" s="32">
         <v>4691707.6550000003</v>
       </c>
-      <c r="F41" s="69"/>
-      <c r="G41" s="69"/>
-      <c r="H41" s="37" t="s">
+      <c r="F41" s="65"/>
+      <c r="G41" s="65"/>
+      <c r="H41" s="33" t="s">
         <v>8</v>
       </c>
       <c r="I41" s="10"/>
@@ -2479,18 +2471,18 @@
     </row>
     <row r="42" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
-      <c r="C42" s="35">
+      <c r="C42" s="31">
         <v>65</v>
       </c>
-      <c r="D42" s="36">
+      <c r="D42" s="32">
         <v>7513134.1550000003</v>
       </c>
-      <c r="E42" s="36">
+      <c r="E42" s="32">
         <v>4691707.0219999999</v>
       </c>
-      <c r="F42" s="69"/>
-      <c r="G42" s="69"/>
-      <c r="H42" s="37" t="s">
+      <c r="F42" s="65"/>
+      <c r="G42" s="65"/>
+      <c r="H42" s="33" t="s">
         <v>8</v>
       </c>
       <c r="I42" s="10"/>
@@ -2498,18 +2490,18 @@
     </row>
     <row r="43" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
-      <c r="C43" s="35">
+      <c r="C43" s="31">
         <v>67</v>
       </c>
-      <c r="D43" s="36">
+      <c r="D43" s="32">
         <v>7513135.8569999998</v>
       </c>
-      <c r="E43" s="36">
+      <c r="E43" s="32">
         <v>4691707.7450000001</v>
       </c>
-      <c r="F43" s="69"/>
-      <c r="G43" s="69"/>
-      <c r="H43" s="37" t="s">
+      <c r="F43" s="65"/>
+      <c r="G43" s="65"/>
+      <c r="H43" s="33" t="s">
         <v>8</v>
       </c>
       <c r="I43" s="10"/>
@@ -2517,18 +2509,18 @@
     </row>
     <row r="44" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
-      <c r="C44" s="35">
+      <c r="C44" s="31">
         <v>68</v>
       </c>
-      <c r="D44" s="36">
+      <c r="D44" s="32">
         <v>7513143.2529999996</v>
       </c>
-      <c r="E44" s="36">
+      <c r="E44" s="32">
         <v>4691714.4639999997</v>
       </c>
-      <c r="F44" s="69"/>
-      <c r="G44" s="69"/>
-      <c r="H44" s="37" t="s">
+      <c r="F44" s="65"/>
+      <c r="G44" s="65"/>
+      <c r="H44" s="33" t="s">
         <v>8</v>
       </c>
       <c r="I44" s="10"/>
@@ -2536,18 +2528,18 @@
     </row>
     <row r="45" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
-      <c r="C45" s="35">
+      <c r="C45" s="31">
         <v>101</v>
       </c>
-      <c r="D45" s="36">
+      <c r="D45" s="32">
         <v>7513138.2271999996</v>
       </c>
-      <c r="E45" s="36">
+      <c r="E45" s="32">
         <v>4691719.9639999997</v>
       </c>
-      <c r="F45" s="69"/>
-      <c r="G45" s="69"/>
-      <c r="H45" s="37" t="s">
+      <c r="F45" s="65"/>
+      <c r="G45" s="65"/>
+      <c r="H45" s="33" t="s">
         <v>8</v>
       </c>
       <c r="I45" s="10"/>
@@ -2555,18 +2547,18 @@
     </row>
     <row r="46" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
-      <c r="C46" s="35">
+      <c r="C46" s="31">
         <v>102</v>
       </c>
-      <c r="D46" s="36">
+      <c r="D46" s="32">
         <v>7513134.8328999998</v>
       </c>
-      <c r="E46" s="36">
+      <c r="E46" s="32">
         <v>4691717.6268999996</v>
       </c>
-      <c r="F46" s="69"/>
-      <c r="G46" s="69"/>
-      <c r="H46" s="37" t="s">
+      <c r="F46" s="65"/>
+      <c r="G46" s="65"/>
+      <c r="H46" s="33" t="s">
         <v>8</v>
       </c>
       <c r="I46" s="10"/>
@@ -2574,18 +2566,18 @@
     </row>
     <row r="47" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
-      <c r="C47" s="35">
+      <c r="C47" s="31">
         <v>103</v>
       </c>
-      <c r="D47" s="36">
+      <c r="D47" s="32">
         <v>7513135.2495999997</v>
       </c>
-      <c r="E47" s="36">
+      <c r="E47" s="32">
         <v>4691717.1867000004</v>
       </c>
-      <c r="F47" s="69"/>
-      <c r="G47" s="69"/>
-      <c r="H47" s="37" t="s">
+      <c r="F47" s="65"/>
+      <c r="G47" s="65"/>
+      <c r="H47" s="33" t="s">
         <v>8</v>
       </c>
       <c r="I47" s="10"/>
@@ -2593,18 +2585,18 @@
     </row>
     <row r="48" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
-      <c r="C48" s="35">
+      <c r="C48" s="31">
         <v>104</v>
       </c>
-      <c r="D48" s="36">
+      <c r="D48" s="32">
         <v>7513131.2090999996</v>
       </c>
-      <c r="E48" s="36">
+      <c r="E48" s="32">
         <v>4691717.4923</v>
       </c>
-      <c r="F48" s="69"/>
-      <c r="G48" s="69"/>
-      <c r="H48" s="37" t="s">
+      <c r="F48" s="65"/>
+      <c r="G48" s="65"/>
+      <c r="H48" s="33" t="s">
         <v>8</v>
       </c>
       <c r="I48" s="10"/>
@@ -2612,18 +2604,18 @@
     </row>
     <row r="49" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
-      <c r="C49" s="35">
-        <v>8</v>
-      </c>
-      <c r="D49" s="36">
+      <c r="C49" s="31">
+        <v>8</v>
+      </c>
+      <c r="D49" s="32">
         <v>7513128.7640000004</v>
       </c>
-      <c r="E49" s="36">
+      <c r="E49" s="32">
         <v>4691715.8310000002</v>
       </c>
-      <c r="F49" s="69"/>
-      <c r="G49" s="69"/>
-      <c r="H49" s="37" t="s">
+      <c r="F49" s="65"/>
+      <c r="G49" s="65"/>
+      <c r="H49" s="33" t="s">
         <v>8</v>
       </c>
       <c r="I49" s="10"/>
@@ -2631,18 +2623,18 @@
     </row>
     <row r="50" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
-      <c r="C50" s="35">
+      <c r="C50" s="31">
         <v>9</v>
       </c>
-      <c r="D50" s="36">
+      <c r="D50" s="32">
         <v>7513126.8399999999</v>
       </c>
-      <c r="E50" s="36">
+      <c r="E50" s="32">
         <v>4691714.1189999999</v>
       </c>
-      <c r="F50" s="69"/>
-      <c r="G50" s="69"/>
-      <c r="H50" s="37" t="s">
+      <c r="F50" s="65"/>
+      <c r="G50" s="65"/>
+      <c r="H50" s="33" t="s">
         <v>8</v>
       </c>
       <c r="I50" s="10"/>
@@ -2660,8 +2652,8 @@
       <c r="E51" s="7">
         <v>4691711.4588000001</v>
       </c>
-      <c r="F51" s="70"/>
-      <c r="G51" s="70"/>
+      <c r="F51" s="66"/>
+      <c r="G51" s="66"/>
       <c r="H51" s="12" t="s">
         <v>8</v>
       </c>
@@ -2683,28 +2675,28 @@
     <row r="54" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
-      <c r="C54" s="71" t="s">
+      <c r="C54" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="D54" s="71"/>
-      <c r="E54" s="71"/>
-      <c r="F54" s="71"/>
-      <c r="G54" s="71"/>
-      <c r="H54" s="71"/>
-      <c r="I54" s="71"/>
+      <c r="D54" s="67"/>
+      <c r="E54" s="67"/>
+      <c r="F54" s="67"/>
+      <c r="G54" s="67"/>
+      <c r="H54" s="67"/>
+      <c r="I54" s="67"/>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
     </row>
     <row r="55" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
-      <c r="C55" s="71"/>
-      <c r="D55" s="71"/>
-      <c r="E55" s="71"/>
-      <c r="F55" s="71"/>
-      <c r="G55" s="71"/>
-      <c r="H55" s="71"/>
-      <c r="I55" s="71"/>
+      <c r="C55" s="67"/>
+      <c r="D55" s="67"/>
+      <c r="E55" s="67"/>
+      <c r="F55" s="67"/>
+      <c r="G55" s="67"/>
+      <c r="H55" s="67"/>
+      <c r="I55" s="67"/>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
     </row>
@@ -2775,141 +2767,141 @@
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
-      <c r="E66" s="49" t="s">
+      <c r="E66" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="F66" s="50"/>
-      <c r="G66" s="51"/>
-      <c r="H66" s="52" t="s">
+      <c r="F66" s="46"/>
+      <c r="G66" s="47"/>
+      <c r="H66" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="I66" s="53"/>
-      <c r="J66" s="56"/>
-      <c r="K66" s="57"/>
+      <c r="I66" s="49"/>
+      <c r="J66" s="52"/>
+      <c r="K66" s="53"/>
     </row>
     <row r="67" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="60" t="s">
+      <c r="A67" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B67" s="61"/>
-      <c r="C67" s="61"/>
-      <c r="D67" s="62"/>
-      <c r="E67" s="63">
+      <c r="B67" s="57"/>
+      <c r="C67" s="57"/>
+      <c r="D67" s="58"/>
+      <c r="E67" s="59">
         <v>152</v>
       </c>
-      <c r="F67" s="64"/>
-      <c r="G67" s="65"/>
-      <c r="H67" s="54"/>
-      <c r="I67" s="55"/>
-      <c r="J67" s="58"/>
-      <c r="K67" s="59"/>
+      <c r="F67" s="60"/>
+      <c r="G67" s="61"/>
+      <c r="H67" s="50"/>
+      <c r="I67" s="51"/>
+      <c r="J67" s="54"/>
+      <c r="K67" s="55"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="38"/>
-      <c r="B68" s="38"/>
-      <c r="C68" s="38"/>
-      <c r="D68" s="38"/>
-      <c r="E68" s="38"/>
-      <c r="F68" s="38"/>
-      <c r="G68" s="38"/>
-      <c r="H68" s="38"/>
-      <c r="I68" s="38"/>
-      <c r="J68" s="38"/>
-      <c r="K68" s="38"/>
-    </row>
-    <row r="69" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="38"/>
-      <c r="B69" s="38"/>
-      <c r="C69" s="38"/>
-      <c r="D69" s="38"/>
-      <c r="E69" s="38"/>
-      <c r="F69" s="38"/>
-      <c r="G69" s="38"/>
-      <c r="H69" s="38"/>
-      <c r="I69" s="38"/>
-      <c r="J69" s="38"/>
-      <c r="K69" s="38"/>
+      <c r="A68" s="34"/>
+      <c r="B68" s="34"/>
+      <c r="C68" s="34"/>
+      <c r="D68" s="34"/>
+      <c r="E68" s="34"/>
+      <c r="F68" s="34"/>
+      <c r="G68" s="34"/>
+      <c r="H68" s="34"/>
+      <c r="I68" s="34"/>
+      <c r="J68" s="34"/>
+      <c r="K68" s="34"/>
+    </row>
+    <row r="69" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="34"/>
+      <c r="B69" s="34"/>
+      <c r="C69" s="34"/>
+      <c r="D69" s="34"/>
+      <c r="E69" s="34"/>
+      <c r="F69" s="34"/>
+      <c r="G69" s="34"/>
+      <c r="H69" s="34"/>
+      <c r="I69" s="34"/>
+      <c r="J69" s="34"/>
+      <c r="K69" s="34"/>
     </row>
     <row r="70" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="39" t="s">
+      <c r="A70" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B70" s="39"/>
-      <c r="C70" s="39"/>
-      <c r="D70" s="39"/>
-      <c r="E70" s="39"/>
-      <c r="F70" s="39"/>
-      <c r="G70" s="39"/>
-      <c r="H70" s="39"/>
-      <c r="I70" s="39"/>
-      <c r="J70" s="39"/>
-      <c r="K70" s="39"/>
+      <c r="B70" s="35"/>
+      <c r="C70" s="35"/>
+      <c r="D70" s="35"/>
+      <c r="E70" s="35"/>
+      <c r="F70" s="35"/>
+      <c r="G70" s="35"/>
+      <c r="H70" s="35"/>
+      <c r="I70" s="35"/>
+      <c r="J70" s="35"/>
+      <c r="K70" s="35"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="39"/>
-      <c r="B71" s="39"/>
-      <c r="C71" s="39"/>
-      <c r="D71" s="39"/>
-      <c r="E71" s="39"/>
-      <c r="F71" s="39"/>
-      <c r="G71" s="39"/>
-      <c r="H71" s="39"/>
-      <c r="I71" s="39"/>
-      <c r="J71" s="39"/>
-      <c r="K71" s="39"/>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" s="39"/>
-      <c r="B72" s="39"/>
-      <c r="C72" s="39"/>
-      <c r="D72" s="39"/>
-      <c r="E72" s="39"/>
-      <c r="F72" s="39"/>
-      <c r="G72" s="39"/>
-      <c r="H72" s="39"/>
-      <c r="I72" s="39"/>
-      <c r="J72" s="39"/>
-      <c r="K72" s="39"/>
-    </row>
-    <row r="73" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="39"/>
-      <c r="B73" s="39"/>
-      <c r="C73" s="39"/>
-      <c r="D73" s="39"/>
-      <c r="E73" s="39"/>
-      <c r="F73" s="39"/>
-      <c r="G73" s="39"/>
-      <c r="H73" s="39"/>
-      <c r="I73" s="39"/>
-      <c r="J73" s="39"/>
-      <c r="K73" s="39"/>
+      <c r="A71" s="35"/>
+      <c r="B71" s="35"/>
+      <c r="C71" s="35"/>
+      <c r="D71" s="35"/>
+      <c r="E71" s="35"/>
+      <c r="F71" s="35"/>
+      <c r="G71" s="35"/>
+      <c r="H71" s="35"/>
+      <c r="I71" s="35"/>
+      <c r="J71" s="35"/>
+      <c r="K71" s="35"/>
+    </row>
+    <row r="72" spans="1:11" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="35"/>
+      <c r="B72" s="35"/>
+      <c r="C72" s="35"/>
+      <c r="D72" s="35"/>
+      <c r="E72" s="35"/>
+      <c r="F72" s="35"/>
+      <c r="G72" s="35"/>
+      <c r="H72" s="35"/>
+      <c r="I72" s="35"/>
+      <c r="J72" s="35"/>
+      <c r="K72" s="35"/>
+    </row>
+    <row r="73" spans="1:11" ht="8.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="35"/>
+      <c r="B73" s="35"/>
+      <c r="C73" s="35"/>
+      <c r="D73" s="35"/>
+      <c r="E73" s="35"/>
+      <c r="F73" s="35"/>
+      <c r="G73" s="35"/>
+      <c r="H73" s="35"/>
+      <c r="I73" s="35"/>
+      <c r="J73" s="35"/>
+      <c r="K73" s="35"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C74" s="40"/>
-      <c r="D74" s="41"/>
-      <c r="E74" s="41"/>
-      <c r="F74" s="41"/>
-      <c r="G74" s="41"/>
-      <c r="H74" s="41"/>
-      <c r="I74" s="42"/>
+      <c r="C74" s="36"/>
+      <c r="D74" s="37"/>
+      <c r="E74" s="37"/>
+      <c r="F74" s="37"/>
+      <c r="G74" s="37"/>
+      <c r="H74" s="37"/>
+      <c r="I74" s="38"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C75" s="43"/>
-      <c r="D75" s="44"/>
-      <c r="E75" s="44"/>
-      <c r="F75" s="44"/>
-      <c r="G75" s="44"/>
-      <c r="H75" s="44"/>
-      <c r="I75" s="45"/>
+      <c r="C75" s="39"/>
+      <c r="D75" s="40"/>
+      <c r="E75" s="40"/>
+      <c r="F75" s="40"/>
+      <c r="G75" s="40"/>
+      <c r="H75" s="40"/>
+      <c r="I75" s="41"/>
     </row>
     <row r="76" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C76" s="46"/>
-      <c r="D76" s="47"/>
-      <c r="E76" s="47"/>
-      <c r="F76" s="47"/>
-      <c r="G76" s="47"/>
-      <c r="H76" s="47"/>
-      <c r="I76" s="48"/>
+      <c r="C76" s="39"/>
+      <c r="D76" s="40"/>
+      <c r="E76" s="40"/>
+      <c r="F76" s="40"/>
+      <c r="G76" s="40"/>
+      <c r="H76" s="40"/>
+      <c r="I76" s="44"/>
     </row>
     <row r="77" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
@@ -2946,13 +2938,13 @@
       <c r="E78" s="4">
         <v>4691722.8739999998</v>
       </c>
-      <c r="F78" s="66">
+      <c r="F78" s="62">
         <v>623.17399999999998</v>
       </c>
-      <c r="G78" s="66" t="s">
+      <c r="G78" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="H78" s="26" t="s">
+      <c r="H78" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I78" s="1"/>
@@ -2970,9 +2962,9 @@
       <c r="E79" s="4">
         <v>4691720.0990000004</v>
       </c>
-      <c r="F79" s="66"/>
-      <c r="G79" s="66"/>
-      <c r="H79" s="26" t="s">
+      <c r="F79" s="62"/>
+      <c r="G79" s="62"/>
+      <c r="H79" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I79" s="1"/>
@@ -2990,9 +2982,9 @@
       <c r="E80" s="4">
         <v>4691715.5049999999</v>
       </c>
-      <c r="F80" s="66"/>
-      <c r="G80" s="66"/>
-      <c r="H80" s="26" t="s">
+      <c r="F80" s="62"/>
+      <c r="G80" s="62"/>
+      <c r="H80" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I80" s="1"/>
@@ -3010,9 +3002,9 @@
       <c r="E81" s="4">
         <v>4691719.318</v>
       </c>
-      <c r="F81" s="66"/>
-      <c r="G81" s="66"/>
-      <c r="H81" s="26" t="s">
+      <c r="F81" s="62"/>
+      <c r="G81" s="62"/>
+      <c r="H81" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I81" s="1"/>
@@ -3030,9 +3022,9 @@
       <c r="E82" s="4">
         <v>4691713.9479999999</v>
       </c>
-      <c r="F82" s="66"/>
-      <c r="G82" s="66"/>
-      <c r="H82" s="26" t="s">
+      <c r="F82" s="62"/>
+      <c r="G82" s="62"/>
+      <c r="H82" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I82" s="1"/>
@@ -3050,9 +3042,9 @@
       <c r="E83" s="4">
         <v>4691712.1909999996</v>
       </c>
-      <c r="F83" s="66"/>
-      <c r="G83" s="66"/>
-      <c r="H83" s="26" t="s">
+      <c r="F83" s="62"/>
+      <c r="G83" s="62"/>
+      <c r="H83" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I83" s="1"/>
@@ -3070,9 +3062,9 @@
       <c r="E84" s="4">
         <v>4691711.0889999997</v>
       </c>
-      <c r="F84" s="66"/>
-      <c r="G84" s="66"/>
-      <c r="H84" s="26" t="s">
+      <c r="F84" s="62"/>
+      <c r="G84" s="62"/>
+      <c r="H84" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I84" s="1"/>
@@ -3090,9 +3082,9 @@
       <c r="E85" s="4">
         <v>4691706.8949999996</v>
       </c>
-      <c r="F85" s="66"/>
-      <c r="G85" s="66"/>
-      <c r="H85" s="26" t="s">
+      <c r="F85" s="62"/>
+      <c r="G85" s="62"/>
+      <c r="H85" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I85" s="1"/>
@@ -3110,9 +3102,9 @@
       <c r="E86" s="4">
         <v>4691706.18</v>
       </c>
-      <c r="F86" s="66"/>
-      <c r="G86" s="66"/>
-      <c r="H86" s="26" t="s">
+      <c r="F86" s="62"/>
+      <c r="G86" s="62"/>
+      <c r="H86" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I86" s="1"/>
@@ -3130,9 +3122,9 @@
       <c r="E87" s="4">
         <v>4691706.1939000003</v>
       </c>
-      <c r="F87" s="66"/>
-      <c r="G87" s="66"/>
-      <c r="H87" s="26" t="s">
+      <c r="F87" s="62"/>
+      <c r="G87" s="62"/>
+      <c r="H87" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I87" s="1"/>
@@ -3150,9 +3142,9 @@
       <c r="E88" s="4">
         <v>4691707.7450000001</v>
       </c>
-      <c r="F88" s="66"/>
-      <c r="G88" s="66"/>
-      <c r="H88" s="26" t="s">
+      <c r="F88" s="62"/>
+      <c r="G88" s="62"/>
+      <c r="H88" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I88" s="1"/>
@@ -3170,9 +3162,9 @@
       <c r="E89" s="4">
         <v>4691714.4639999997</v>
       </c>
-      <c r="F89" s="66"/>
-      <c r="G89" s="66"/>
-      <c r="H89" s="26" t="s">
+      <c r="F89" s="62"/>
+      <c r="G89" s="62"/>
+      <c r="H89" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I89" s="1"/>
@@ -3185,14 +3177,14 @@
         <v>106</v>
       </c>
       <c r="D90" s="4">
-        <v>7513136.3592999997</v>
+        <v>7513135.0017999997</v>
       </c>
       <c r="E90" s="4">
-        <v>4691715.8525</v>
-      </c>
-      <c r="F90" s="66"/>
-      <c r="G90" s="66"/>
-      <c r="H90" s="26" t="s">
+        <v>4691717.3711000001</v>
+      </c>
+      <c r="F90" s="62"/>
+      <c r="G90" s="62"/>
+      <c r="H90" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I90" s="1"/>
@@ -3205,74 +3197,78 @@
         <v>107</v>
       </c>
       <c r="D91" s="4">
-        <v>7513132.6316</v>
+        <v>7513131.3008000003</v>
       </c>
       <c r="E91" s="4">
-        <v>4691712.5202000001</v>
-      </c>
-      <c r="F91" s="66"/>
-      <c r="G91" s="66"/>
-      <c r="H91" s="26" t="s">
+        <v>4691714.0088999998</v>
+      </c>
+      <c r="F91" s="62"/>
+      <c r="G91" s="62"/>
+      <c r="H91" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I91" s="1"/>
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
     </row>
-    <row r="92" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
-      <c r="C92" s="6">
+      <c r="C92" s="5">
         <v>108</v>
       </c>
-      <c r="D92" s="7">
+      <c r="D92" s="4">
         <v>7513129.5292999996</v>
       </c>
-      <c r="E92" s="7">
+      <c r="E92" s="4">
         <v>4691715.9907</v>
       </c>
-      <c r="F92" s="67"/>
-      <c r="G92" s="67"/>
-      <c r="H92" s="27" t="s">
+      <c r="F92" s="62"/>
+      <c r="G92" s="62"/>
+      <c r="H92" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I92" s="1"/>
       <c r="J92" s="1"/>
       <c r="K92" s="1"/>
     </row>
-    <row r="93" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
-      <c r="C93" s="28"/>
-      <c r="D93" s="29"/>
-      <c r="E93" s="29"/>
-      <c r="F93" s="30"/>
-      <c r="G93" s="30"/>
-      <c r="H93" s="25"/>
+      <c r="C93" s="5">
+        <v>109</v>
+      </c>
+      <c r="D93" s="4">
+        <v>7513131.2148000002</v>
+      </c>
+      <c r="E93" s="4">
+        <v>4691714.1052000001</v>
+      </c>
+      <c r="F93" s="62"/>
+      <c r="G93" s="62"/>
+      <c r="H93" s="25" t="s">
+        <v>8</v>
+      </c>
       <c r="I93" s="1"/>
       <c r="J93" s="1"/>
       <c r="K93" s="1"/>
     </row>
-    <row r="94" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
-      <c r="C94" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D94" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E94" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F94" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G94" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H94" s="13" t="s">
-        <v>3</v>
+      <c r="C94" s="6">
+        <v>110</v>
+      </c>
+      <c r="D94" s="7">
+        <v>7513128.0055</v>
+      </c>
+      <c r="E94" s="7">
+        <v>4691711.2202000003</v>
+      </c>
+      <c r="F94" s="63"/>
+      <c r="G94" s="63"/>
+      <c r="H94" s="26" t="s">
+        <v>8</v>
       </c>
       <c r="I94" s="1"/>
       <c r="J94" s="1"/>
@@ -3281,23 +3277,23 @@
     <row r="95" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
-      <c r="C95" s="5">
+      <c r="C95" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D95" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D95" s="4">
-        <v>7513135.568</v>
-      </c>
-      <c r="E95" s="4">
-        <v>4691722.8739999998</v>
-      </c>
-      <c r="F95" s="66">
-        <v>626.09400000000005</v>
-      </c>
-      <c r="G95" s="66" t="s">
-        <v>23</v>
-      </c>
-      <c r="H95" s="26" t="s">
-        <v>8</v>
+      <c r="E95" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F95" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G95" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H95" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="I95" s="1"/>
       <c r="J95" s="1"/>
@@ -3307,17 +3303,21 @@
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D96" s="4">
-        <v>7513132.5010000002</v>
+        <v>7513135.568</v>
       </c>
       <c r="E96" s="4">
-        <v>4691720.0990000004</v>
-      </c>
-      <c r="F96" s="66"/>
-      <c r="G96" s="66"/>
-      <c r="H96" s="26" t="s">
+        <v>4691722.8739999998</v>
+      </c>
+      <c r="F96" s="62">
+        <v>626.09400000000005</v>
+      </c>
+      <c r="G96" s="62" t="s">
+        <v>23</v>
+      </c>
+      <c r="H96" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I96" s="1"/>
@@ -3328,17 +3328,17 @@
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="5">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D97" s="4">
-        <v>7513128.9859999996</v>
+        <v>7513132.5010000002</v>
       </c>
       <c r="E97" s="4">
-        <v>4691715.5049999999</v>
-      </c>
-      <c r="F97" s="66"/>
-      <c r="G97" s="66"/>
-      <c r="H97" s="26" t="s">
+        <v>4691720.0990000004</v>
+      </c>
+      <c r="F97" s="62"/>
+      <c r="G97" s="62"/>
+      <c r="H97" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I97" s="1"/>
@@ -3349,17 +3349,17 @@
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="5">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D98" s="4">
-        <v>7513133.25</v>
+        <v>7513128.9859999996</v>
       </c>
       <c r="E98" s="4">
-        <v>4691719.318</v>
-      </c>
-      <c r="F98" s="66"/>
-      <c r="G98" s="66"/>
-      <c r="H98" s="26" t="s">
+        <v>4691715.5049999999</v>
+      </c>
+      <c r="F98" s="62"/>
+      <c r="G98" s="62"/>
+      <c r="H98" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I98" s="1"/>
@@ -3370,17 +3370,17 @@
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="5">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D99" s="4">
-        <v>7513127.2779999999</v>
+        <v>7513133.25</v>
       </c>
       <c r="E99" s="4">
-        <v>4691713.9479999999</v>
-      </c>
-      <c r="F99" s="66"/>
-      <c r="G99" s="66"/>
-      <c r="H99" s="26" t="s">
+        <v>4691719.318</v>
+      </c>
+      <c r="F99" s="62"/>
+      <c r="G99" s="62"/>
+      <c r="H99" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I99" s="1"/>
@@ -3391,17 +3391,17 @@
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="5">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D100" s="4">
-        <v>7513127.3820000002</v>
+        <v>7513127.2779999999</v>
       </c>
       <c r="E100" s="4">
-        <v>4691712.1909999996</v>
-      </c>
-      <c r="F100" s="66"/>
-      <c r="G100" s="66"/>
-      <c r="H100" s="26" t="s">
+        <v>4691713.9479999999</v>
+      </c>
+      <c r="F100" s="62"/>
+      <c r="G100" s="62"/>
+      <c r="H100" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I100" s="1"/>
@@ -3412,17 +3412,17 @@
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="5">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D101" s="4">
-        <v>7513128.142</v>
+        <v>7513127.3820000002</v>
       </c>
       <c r="E101" s="4">
-        <v>4691711.0889999997</v>
-      </c>
-      <c r="F101" s="66"/>
-      <c r="G101" s="66"/>
-      <c r="H101" s="26" t="s">
+        <v>4691712.1909999996</v>
+      </c>
+      <c r="F101" s="62"/>
+      <c r="G101" s="62"/>
+      <c r="H101" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I101" s="1"/>
@@ -3433,17 +3433,17 @@
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="5">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D102" s="4">
-        <v>7513132.0240000002</v>
+        <v>7513128.142</v>
       </c>
       <c r="E102" s="4">
-        <v>4691706.8949999996</v>
-      </c>
-      <c r="F102" s="66"/>
-      <c r="G102" s="66"/>
-      <c r="H102" s="26" t="s">
+        <v>4691711.0889999997</v>
+      </c>
+      <c r="F102" s="62"/>
+      <c r="G102" s="62"/>
+      <c r="H102" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I102" s="1"/>
@@ -3454,17 +3454,17 @@
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="5">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D103" s="4">
-        <v>7513133.5190000003</v>
+        <v>7513132.0240000002</v>
       </c>
       <c r="E103" s="4">
-        <v>4691706.18</v>
-      </c>
-      <c r="F103" s="66"/>
-      <c r="G103" s="66"/>
-      <c r="H103" s="26" t="s">
+        <v>4691706.8949999996</v>
+      </c>
+      <c r="F103" s="62"/>
+      <c r="G103" s="62"/>
+      <c r="H103" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I103" s="1"/>
@@ -3475,17 +3475,17 @@
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="5">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="D104" s="4">
-        <v>7513134.1436999999</v>
+        <v>7513133.5190000003</v>
       </c>
       <c r="E104" s="4">
-        <v>4691706.1939000003</v>
-      </c>
-      <c r="F104" s="66"/>
-      <c r="G104" s="66"/>
-      <c r="H104" s="26" t="s">
+        <v>4691706.18</v>
+      </c>
+      <c r="F104" s="62"/>
+      <c r="G104" s="62"/>
+      <c r="H104" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I104" s="1"/>
@@ -3496,17 +3496,17 @@
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="5">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D105" s="4">
-        <v>7513135.8569999998</v>
+        <v>7513134.1436999999</v>
       </c>
       <c r="E105" s="4">
-        <v>4691707.7450000001</v>
-      </c>
-      <c r="F105" s="66"/>
-      <c r="G105" s="66"/>
-      <c r="H105" s="26" t="s">
+        <v>4691706.1939000003</v>
+      </c>
+      <c r="F105" s="62"/>
+      <c r="G105" s="62"/>
+      <c r="H105" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I105" s="1"/>
@@ -3517,17 +3517,17 @@
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="5">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D106" s="4">
-        <v>7513143.2529999996</v>
+        <v>7513135.8569999998</v>
       </c>
       <c r="E106" s="4">
-        <v>4691714.4639999997</v>
-      </c>
-      <c r="F106" s="66"/>
-      <c r="G106" s="66"/>
-      <c r="H106" s="26" t="s">
+        <v>4691707.7450000001</v>
+      </c>
+      <c r="F106" s="62"/>
+      <c r="G106" s="62"/>
+      <c r="H106" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I106" s="1"/>
@@ -3538,17 +3538,17 @@
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="5">
-        <v>106</v>
+        <v>68</v>
       </c>
       <c r="D107" s="4">
-        <v>7513136.3592999997</v>
+        <v>7513143.2529999996</v>
       </c>
       <c r="E107" s="4">
-        <v>4691715.8525</v>
-      </c>
-      <c r="F107" s="66"/>
-      <c r="G107" s="66"/>
-      <c r="H107" s="26" t="s">
+        <v>4691714.4639999997</v>
+      </c>
+      <c r="F107" s="62"/>
+      <c r="G107" s="62"/>
+      <c r="H107" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I107" s="1"/>
@@ -3559,38 +3559,38 @@
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="5">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D108" s="4">
-        <v>7513132.6316</v>
+        <v>7513136.3592999997</v>
       </c>
       <c r="E108" s="4">
-        <v>4691712.5202000001</v>
-      </c>
-      <c r="F108" s="66"/>
-      <c r="G108" s="66"/>
-      <c r="H108" s="26" t="s">
+        <v>4691715.8525</v>
+      </c>
+      <c r="F108" s="62"/>
+      <c r="G108" s="62"/>
+      <c r="H108" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I108" s="1"/>
       <c r="J108" s="1"/>
       <c r="K108" s="1"/>
     </row>
-    <row r="109" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
-      <c r="C109" s="6">
-        <v>108</v>
-      </c>
-      <c r="D109" s="7">
-        <v>7513129.5292999996</v>
-      </c>
-      <c r="E109" s="7">
-        <v>4691715.9907</v>
-      </c>
-      <c r="F109" s="67"/>
-      <c r="G109" s="67"/>
-      <c r="H109" s="27" t="s">
+      <c r="C109" s="5">
+        <v>107</v>
+      </c>
+      <c r="D109" s="4">
+        <v>7513132.6316</v>
+      </c>
+      <c r="E109" s="4">
+        <v>4691712.5202000001</v>
+      </c>
+      <c r="F109" s="62"/>
+      <c r="G109" s="62"/>
+      <c r="H109" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I109" s="1"/>
@@ -3600,12 +3600,20 @@
     <row r="110" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
-      <c r="C110" s="28"/>
-      <c r="D110" s="29"/>
-      <c r="E110" s="29"/>
-      <c r="F110" s="30"/>
-      <c r="G110" s="30"/>
-      <c r="H110" s="25"/>
+      <c r="C110" s="6">
+        <v>108</v>
+      </c>
+      <c r="D110" s="7">
+        <v>7513129.5292999996</v>
+      </c>
+      <c r="E110" s="7">
+        <v>4691715.9907</v>
+      </c>
+      <c r="F110" s="63"/>
+      <c r="G110" s="63"/>
+      <c r="H110" s="26" t="s">
+        <v>8</v>
+      </c>
       <c r="I110" s="1"/>
       <c r="J110" s="1"/>
       <c r="K110" s="1"/>
@@ -3647,13 +3655,13 @@
       <c r="E112" s="4">
         <v>4691714.3306</v>
       </c>
-      <c r="F112" s="66">
+      <c r="F112" s="62">
         <v>629.29999999999995</v>
       </c>
-      <c r="G112" s="66" t="s">
+      <c r="G112" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="H112" s="26" t="s">
+      <c r="H112" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I112" s="1"/>
@@ -3672,9 +3680,9 @@
       <c r="E113" s="4">
         <v>4691713.9479999999</v>
       </c>
-      <c r="F113" s="66"/>
-      <c r="G113" s="66"/>
-      <c r="H113" s="26" t="s">
+      <c r="F113" s="62"/>
+      <c r="G113" s="62"/>
+      <c r="H113" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I113" s="1"/>
@@ -3693,9 +3701,9 @@
       <c r="E114" s="4">
         <v>4691712.3039999995</v>
       </c>
-      <c r="F114" s="66"/>
-      <c r="G114" s="66"/>
-      <c r="H114" s="26" t="s">
+      <c r="F114" s="62"/>
+      <c r="G114" s="62"/>
+      <c r="H114" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I114" s="1"/>
@@ -3714,9 +3722,9 @@
       <c r="E115" s="4">
         <v>4691711.0889999997</v>
       </c>
-      <c r="F115" s="66"/>
-      <c r="G115" s="66"/>
-      <c r="H115" s="26" t="s">
+      <c r="F115" s="62"/>
+      <c r="G115" s="62"/>
+      <c r="H115" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I115" s="1"/>
@@ -3735,9 +3743,9 @@
       <c r="E116" s="4">
         <v>4691706.8949999996</v>
       </c>
-      <c r="F116" s="66"/>
-      <c r="G116" s="66"/>
-      <c r="H116" s="26" t="s">
+      <c r="F116" s="62"/>
+      <c r="G116" s="62"/>
+      <c r="H116" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I116" s="1"/>
@@ -3756,9 +3764,9 @@
       <c r="E117" s="4">
         <v>4691706.6350999996</v>
       </c>
-      <c r="F117" s="66"/>
-      <c r="G117" s="66"/>
-      <c r="H117" s="26" t="s">
+      <c r="F117" s="62"/>
+      <c r="G117" s="62"/>
+      <c r="H117" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I117" s="1"/>
@@ -3777,9 +3785,9 @@
       <c r="E118" s="4">
         <v>4691706.1939000003</v>
       </c>
-      <c r="F118" s="66"/>
-      <c r="G118" s="66"/>
-      <c r="H118" s="26" t="s">
+      <c r="F118" s="62"/>
+      <c r="G118" s="62"/>
+      <c r="H118" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I118" s="1"/>
@@ -3798,9 +3806,9 @@
       <c r="E119" s="4">
         <v>4691720.0990000004</v>
       </c>
-      <c r="F119" s="66"/>
-      <c r="G119" s="66"/>
-      <c r="H119" s="26" t="s">
+      <c r="F119" s="62"/>
+      <c r="G119" s="62"/>
+      <c r="H119" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I119" s="1"/>
@@ -3819,9 +3827,9 @@
       <c r="E120" s="4">
         <v>4691719.3229999999</v>
       </c>
-      <c r="F120" s="66"/>
-      <c r="G120" s="66"/>
-      <c r="H120" s="26" t="s">
+      <c r="F120" s="62"/>
+      <c r="G120" s="62"/>
+      <c r="H120" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I120" s="1"/>
@@ -3840,9 +3848,9 @@
       <c r="E121" s="4">
         <v>4691722.8739999998</v>
       </c>
-      <c r="F121" s="66"/>
-      <c r="G121" s="66"/>
-      <c r="H121" s="26" t="s">
+      <c r="F121" s="62"/>
+      <c r="G121" s="62"/>
+      <c r="H121" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I121" s="1"/>
@@ -3861,9 +3869,9 @@
       <c r="E122" s="4">
         <v>4691715.7680000002</v>
       </c>
-      <c r="F122" s="66"/>
-      <c r="G122" s="66"/>
-      <c r="H122" s="26" t="s">
+      <c r="F122" s="62"/>
+      <c r="G122" s="62"/>
+      <c r="H122" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I122" s="1"/>
@@ -3882,9 +3890,9 @@
       <c r="E123" s="4">
         <v>4691714.4639999997</v>
       </c>
-      <c r="F123" s="66"/>
-      <c r="G123" s="66"/>
-      <c r="H123" s="26" t="s">
+      <c r="F123" s="62"/>
+      <c r="G123" s="62"/>
+      <c r="H123" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I123" s="1"/>
@@ -3903,9 +3911,9 @@
       <c r="E124" s="4">
         <v>4691708.2016000003</v>
       </c>
-      <c r="F124" s="66"/>
-      <c r="G124" s="66"/>
-      <c r="H124" s="26" t="s">
+      <c r="F124" s="62"/>
+      <c r="G124" s="62"/>
+      <c r="H124" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I124" s="1"/>
@@ -3924,9 +3932,9 @@
       <c r="E125" s="4">
         <v>4691706.2857999997</v>
       </c>
-      <c r="F125" s="66"/>
-      <c r="G125" s="66"/>
-      <c r="H125" s="26" t="s">
+      <c r="F125" s="62"/>
+      <c r="G125" s="62"/>
+      <c r="H125" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I125" s="1"/>
@@ -3945,9 +3953,9 @@
       <c r="E126" s="4">
         <v>4691717.4736000001</v>
       </c>
-      <c r="F126" s="66"/>
-      <c r="G126" s="66"/>
-      <c r="H126" s="26" t="s">
+      <c r="F126" s="62"/>
+      <c r="G126" s="62"/>
+      <c r="H126" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I126" s="1"/>
@@ -3966,9 +3974,9 @@
       <c r="E127" s="4">
         <v>4691713.8247999996</v>
       </c>
-      <c r="F127" s="66"/>
-      <c r="G127" s="66"/>
-      <c r="H127" s="26" t="s">
+      <c r="F127" s="62"/>
+      <c r="G127" s="62"/>
+      <c r="H127" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I127" s="1"/>
@@ -3987,9 +3995,9 @@
       <c r="E128" s="7">
         <v>4691719.4106000001</v>
       </c>
-      <c r="F128" s="67"/>
-      <c r="G128" s="67"/>
-      <c r="H128" s="27" t="s">
+      <c r="F128" s="63"/>
+      <c r="G128" s="63"/>
+      <c r="H128" s="26" t="s">
         <v>8</v>
       </c>
       <c r="I128" s="1"/>
@@ -4003,34 +4011,34 @@
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
       <c r="D129" s="3"/>
-      <c r="E129" s="49" t="s">
+      <c r="E129" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="F129" s="50"/>
-      <c r="G129" s="51"/>
-      <c r="H129" s="52" t="s">
+      <c r="F129" s="46"/>
+      <c r="G129" s="47"/>
+      <c r="H129" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="I129" s="53"/>
-      <c r="J129" s="56"/>
-      <c r="K129" s="57"/>
+      <c r="I129" s="49"/>
+      <c r="J129" s="52"/>
+      <c r="K129" s="53"/>
     </row>
     <row r="130" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A130" s="60" t="s">
+      <c r="A130" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B130" s="61"/>
-      <c r="C130" s="61"/>
-      <c r="D130" s="62"/>
-      <c r="E130" s="63">
+      <c r="B130" s="57"/>
+      <c r="C130" s="57"/>
+      <c r="D130" s="58"/>
+      <c r="E130" s="59">
         <v>152</v>
       </c>
-      <c r="F130" s="64"/>
-      <c r="G130" s="65"/>
-      <c r="H130" s="54"/>
-      <c r="I130" s="55"/>
-      <c r="J130" s="58"/>
-      <c r="K130" s="59"/>
+      <c r="F130" s="60"/>
+      <c r="G130" s="61"/>
+      <c r="H130" s="50"/>
+      <c r="I130" s="51"/>
+      <c r="J130" s="54"/>
+      <c r="K130" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="25">
@@ -4053,12 +4061,12 @@
     <mergeCell ref="J129:K130"/>
     <mergeCell ref="A130:D130"/>
     <mergeCell ref="E130:G130"/>
-    <mergeCell ref="F95:F109"/>
-    <mergeCell ref="G95:G109"/>
+    <mergeCell ref="F96:F110"/>
+    <mergeCell ref="G96:G110"/>
     <mergeCell ref="F112:F128"/>
     <mergeCell ref="G112:G128"/>
-    <mergeCell ref="F78:F92"/>
-    <mergeCell ref="G78:G92"/>
+    <mergeCell ref="F78:F94"/>
+    <mergeCell ref="G78:G94"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="60" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
njesite kati 2 done
</commit_message>
<xml_diff>
--- a/5-Njësite-banesore/regjistri/22-Koordinatat-për-pjesë-të-ndertesës.xlsx-2602-0-Albnori.xlsx
+++ b/5-Njësite-banesore/regjistri/22-Koordinatat-për-pjesë-të-ndertesës.xlsx-2602-0-Albnori.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="25">
   <si>
     <t>Nr</t>
   </si>
@@ -1739,10 +1739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K130"/>
+  <dimension ref="A1:U147"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A118" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="Q91" sqref="Q91"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A90" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G96" sqref="G96:G112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3562,10 +3562,10 @@
         <v>106</v>
       </c>
       <c r="D108" s="4">
-        <v>7513136.3592999997</v>
+        <v>7513135.0017999997</v>
       </c>
       <c r="E108" s="4">
-        <v>4691715.8525</v>
+        <v>4691717.3711000001</v>
       </c>
       <c r="F108" s="62"/>
       <c r="G108" s="62"/>
@@ -3583,10 +3583,10 @@
         <v>107</v>
       </c>
       <c r="D109" s="4">
-        <v>7513132.6316</v>
+        <v>7513131.3008000003</v>
       </c>
       <c r="E109" s="4">
-        <v>4691712.5202000001</v>
+        <v>4691714.0088999998</v>
       </c>
       <c r="F109" s="62"/>
       <c r="G109" s="62"/>
@@ -3597,21 +3597,21 @@
       <c r="J109" s="1"/>
       <c r="K109" s="1"/>
     </row>
-    <row r="110" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
-      <c r="C110" s="6">
+      <c r="C110" s="5">
         <v>108</v>
       </c>
-      <c r="D110" s="7">
+      <c r="D110" s="4">
         <v>7513129.5292999996</v>
       </c>
-      <c r="E110" s="7">
+      <c r="E110" s="4">
         <v>4691715.9907</v>
       </c>
-      <c r="F110" s="63"/>
-      <c r="G110" s="63"/>
-      <c r="H110" s="26" t="s">
+      <c r="F110" s="62"/>
+      <c r="G110" s="62"/>
+      <c r="H110" s="25" t="s">
         <v>8</v>
       </c>
       <c r="I110" s="1"/>
@@ -3621,47 +3621,39 @@
     <row r="111" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
-      <c r="C111" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D111" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E111" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F111" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G111" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H111" s="13" t="s">
-        <v>3</v>
+      <c r="C111" s="5">
+        <v>109</v>
+      </c>
+      <c r="D111" s="4">
+        <v>7513131.2148000002</v>
+      </c>
+      <c r="E111" s="4">
+        <v>4691714.1052000001</v>
+      </c>
+      <c r="F111" s="62"/>
+      <c r="G111" s="62"/>
+      <c r="H111" s="25" t="s">
+        <v>8</v>
       </c>
       <c r="I111" s="1"/>
       <c r="J111" s="1"/>
       <c r="K111" s="1"/>
     </row>
-    <row r="112" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
-      <c r="C112" s="5">
-        <v>42</v>
-      </c>
-      <c r="D112" s="4">
-        <v>7513127.6977000004</v>
-      </c>
-      <c r="E112" s="4">
-        <v>4691714.3306</v>
-      </c>
-      <c r="F112" s="62">
-        <v>629.29999999999995</v>
-      </c>
-      <c r="G112" s="62" t="s">
-        <v>24</v>
-      </c>
-      <c r="H112" s="25" t="s">
+      <c r="C112" s="6">
+        <v>110</v>
+      </c>
+      <c r="D112" s="7">
+        <v>7513128.0055</v>
+      </c>
+      <c r="E112" s="7">
+        <v>4691711.2202000003</v>
+      </c>
+      <c r="F112" s="63"/>
+      <c r="G112" s="63"/>
+      <c r="H112" s="26" t="s">
         <v>8</v>
       </c>
       <c r="I112" s="1"/>
@@ -3671,20 +3663,6 @@
     <row r="113" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
-      <c r="C113" s="5">
-        <v>43</v>
-      </c>
-      <c r="D113" s="4">
-        <v>7513127.2779999999</v>
-      </c>
-      <c r="E113" s="4">
-        <v>4691713.9479999999</v>
-      </c>
-      <c r="F113" s="62"/>
-      <c r="G113" s="62"/>
-      <c r="H113" s="25" t="s">
-        <v>8</v>
-      </c>
       <c r="I113" s="1"/>
       <c r="J113" s="1"/>
       <c r="K113" s="1"/>
@@ -3692,20 +3670,6 @@
     <row r="114" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
-      <c r="C114" s="5">
-        <v>44</v>
-      </c>
-      <c r="D114" s="4">
-        <v>7513127.3439999996</v>
-      </c>
-      <c r="E114" s="4">
-        <v>4691712.3039999995</v>
-      </c>
-      <c r="F114" s="62"/>
-      <c r="G114" s="62"/>
-      <c r="H114" s="25" t="s">
-        <v>8</v>
-      </c>
       <c r="I114" s="1"/>
       <c r="J114" s="1"/>
       <c r="K114" s="1"/>
@@ -3713,20 +3677,6 @@
     <row r="115" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
-      <c r="C115" s="5">
-        <v>45</v>
-      </c>
-      <c r="D115" s="4">
-        <v>7513128.142</v>
-      </c>
-      <c r="E115" s="4">
-        <v>4691711.0889999997</v>
-      </c>
-      <c r="F115" s="62"/>
-      <c r="G115" s="62"/>
-      <c r="H115" s="25" t="s">
-        <v>8</v>
-      </c>
       <c r="I115" s="1"/>
       <c r="J115" s="1"/>
       <c r="K115" s="1"/>
@@ -3734,20 +3684,6 @@
     <row r="116" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
-      <c r="C116" s="5">
-        <v>47</v>
-      </c>
-      <c r="D116" s="4">
-        <v>7513132.0240000002</v>
-      </c>
-      <c r="E116" s="4">
-        <v>4691706.8949999996</v>
-      </c>
-      <c r="F116" s="62"/>
-      <c r="G116" s="62"/>
-      <c r="H116" s="25" t="s">
-        <v>8</v>
-      </c>
       <c r="I116" s="1"/>
       <c r="J116" s="1"/>
       <c r="K116" s="1"/>
@@ -3755,20 +3691,6 @@
     <row r="117" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
-      <c r="C117" s="5">
-        <v>48</v>
-      </c>
-      <c r="D117" s="4">
-        <v>7513134.6310000001</v>
-      </c>
-      <c r="E117" s="4">
-        <v>4691706.6350999996</v>
-      </c>
-      <c r="F117" s="62"/>
-      <c r="G117" s="62"/>
-      <c r="H117" s="25" t="s">
-        <v>8</v>
-      </c>
       <c r="I117" s="1"/>
       <c r="J117" s="1"/>
       <c r="K117" s="1"/>
@@ -3776,20 +3698,6 @@
     <row r="118" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
-      <c r="C118" s="5">
-        <v>49</v>
-      </c>
-      <c r="D118" s="4">
-        <v>7513134.1436999999</v>
-      </c>
-      <c r="E118" s="4">
-        <v>4691706.1939000003</v>
-      </c>
-      <c r="F118" s="62"/>
-      <c r="G118" s="62"/>
-      <c r="H118" s="25" t="s">
-        <v>8</v>
-      </c>
       <c r="I118" s="1"/>
       <c r="J118" s="1"/>
       <c r="K118" s="1"/>
@@ -3797,20 +3705,6 @@
     <row r="119" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
-      <c r="C119" s="5">
-        <v>50</v>
-      </c>
-      <c r="D119" s="4">
-        <v>7513132.5010000002</v>
-      </c>
-      <c r="E119" s="4">
-        <v>4691720.0990000004</v>
-      </c>
-      <c r="F119" s="62"/>
-      <c r="G119" s="62"/>
-      <c r="H119" s="25" t="s">
-        <v>8</v>
-      </c>
       <c r="I119" s="1"/>
       <c r="J119" s="1"/>
       <c r="K119" s="1"/>
@@ -3818,20 +3712,6 @@
     <row r="120" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
-      <c r="C120" s="5">
-        <v>51</v>
-      </c>
-      <c r="D120" s="4">
-        <v>7513133.2570000002</v>
-      </c>
-      <c r="E120" s="4">
-        <v>4691719.3229999999</v>
-      </c>
-      <c r="F120" s="62"/>
-      <c r="G120" s="62"/>
-      <c r="H120" s="25" t="s">
-        <v>8</v>
-      </c>
       <c r="I120" s="1"/>
       <c r="J120" s="1"/>
       <c r="K120" s="1"/>
@@ -3839,20 +3719,6 @@
     <row r="121" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
-      <c r="C121" s="5">
-        <v>52</v>
-      </c>
-      <c r="D121" s="4">
-        <v>7513135.568</v>
-      </c>
-      <c r="E121" s="4">
-        <v>4691722.8739999998</v>
-      </c>
-      <c r="F121" s="62"/>
-      <c r="G121" s="62"/>
-      <c r="H121" s="25" t="s">
-        <v>8</v>
-      </c>
       <c r="I121" s="1"/>
       <c r="J121" s="1"/>
       <c r="K121" s="1"/>
@@ -3860,20 +3726,6 @@
     <row r="122" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
-      <c r="C122" s="5">
-        <v>78</v>
-      </c>
-      <c r="D122" s="4">
-        <v>7513129.2801999999</v>
-      </c>
-      <c r="E122" s="4">
-        <v>4691715.7680000002</v>
-      </c>
-      <c r="F122" s="62"/>
-      <c r="G122" s="62"/>
-      <c r="H122" s="25" t="s">
-        <v>8</v>
-      </c>
       <c r="I122" s="1"/>
       <c r="J122" s="1"/>
       <c r="K122" s="1"/>
@@ -3881,20 +3733,6 @@
     <row r="123" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
-      <c r="C123" s="5">
-        <v>79</v>
-      </c>
-      <c r="D123" s="4">
-        <v>7513143.2529999996</v>
-      </c>
-      <c r="E123" s="4">
-        <v>4691714.4639999997</v>
-      </c>
-      <c r="F123" s="62"/>
-      <c r="G123" s="62"/>
-      <c r="H123" s="25" t="s">
-        <v>8</v>
-      </c>
       <c r="I123" s="1"/>
       <c r="J123" s="1"/>
       <c r="K123" s="1"/>
@@ -3902,20 +3740,6 @@
     <row r="124" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
-      <c r="C124" s="5">
-        <v>80</v>
-      </c>
-      <c r="D124" s="4">
-        <v>7513136.3596000001</v>
-      </c>
-      <c r="E124" s="4">
-        <v>4691708.2016000003</v>
-      </c>
-      <c r="F124" s="62"/>
-      <c r="G124" s="62"/>
-      <c r="H124" s="25" t="s">
-        <v>8</v>
-      </c>
       <c r="I124" s="1"/>
       <c r="J124" s="1"/>
       <c r="K124" s="1"/>
@@ -3923,20 +3747,6 @@
     <row r="125" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
-      <c r="C125" s="5">
-        <v>82</v>
-      </c>
-      <c r="D125" s="4">
-        <v>7513133.0180000002</v>
-      </c>
-      <c r="E125" s="4">
-        <v>4691706.2857999997</v>
-      </c>
-      <c r="F125" s="62"/>
-      <c r="G125" s="62"/>
-      <c r="H125" s="25" t="s">
-        <v>8</v>
-      </c>
       <c r="I125" s="1"/>
       <c r="J125" s="1"/>
       <c r="K125" s="1"/>
@@ -3944,20 +3754,6 @@
     <row r="126" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
-      <c r="C126" s="5">
-        <v>106</v>
-      </c>
-      <c r="D126" s="4">
-        <v>7513135.1146999998</v>
-      </c>
-      <c r="E126" s="4">
-        <v>4691717.4736000001</v>
-      </c>
-      <c r="F126" s="62"/>
-      <c r="G126" s="62"/>
-      <c r="H126" s="25" t="s">
-        <v>8</v>
-      </c>
       <c r="I126" s="1"/>
       <c r="J126" s="1"/>
       <c r="K126" s="1"/>
@@ -3965,20 +3761,6 @@
     <row r="127" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
-      <c r="C127" s="5">
-        <v>107</v>
-      </c>
-      <c r="D127" s="4">
-        <v>7513131.0981999999</v>
-      </c>
-      <c r="E127" s="4">
-        <v>4691713.8247999996</v>
-      </c>
-      <c r="F127" s="62"/>
-      <c r="G127" s="62"/>
-      <c r="H127" s="25" t="s">
-        <v>8</v>
-      </c>
       <c r="I127" s="1"/>
       <c r="J127" s="1"/>
       <c r="K127" s="1"/>
@@ -3986,25 +3768,11 @@
     <row r="128" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
-      <c r="C128" s="6">
-        <v>109</v>
-      </c>
-      <c r="D128" s="7">
-        <v>7513133.3550000004</v>
-      </c>
-      <c r="E128" s="7">
-        <v>4691719.4106000001</v>
-      </c>
-      <c r="F128" s="63"/>
-      <c r="G128" s="63"/>
-      <c r="H128" s="26" t="s">
-        <v>8</v>
-      </c>
       <c r="I128" s="1"/>
       <c r="J128" s="1"/>
       <c r="K128" s="1"/>
     </row>
-    <row r="129" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A129" s="2" t="s">
         <v>4</v>
       </c>
@@ -4023,7 +3791,7 @@
       <c r="J129" s="52"/>
       <c r="K129" s="53"/>
     </row>
-    <row r="130" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A130" s="56" t="s">
         <v>5</v>
       </c>
@@ -4039,9 +3807,305 @@
       <c r="I130" s="51"/>
       <c r="J130" s="54"/>
       <c r="K130" s="55"/>
+      <c r="P130" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q130" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="R130" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="S130" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="T130" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="U130" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P131" s="5">
+        <v>42</v>
+      </c>
+      <c r="Q131" s="4">
+        <v>7513127.6977000004</v>
+      </c>
+      <c r="R131" s="4">
+        <v>4691714.3306</v>
+      </c>
+      <c r="S131" s="62">
+        <v>629.29999999999995</v>
+      </c>
+      <c r="T131" s="62" t="s">
+        <v>24</v>
+      </c>
+      <c r="U131" s="25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="132" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P132" s="5">
+        <v>43</v>
+      </c>
+      <c r="Q132" s="4">
+        <v>7513127.2779999999</v>
+      </c>
+      <c r="R132" s="4">
+        <v>4691713.9479999999</v>
+      </c>
+      <c r="S132" s="62"/>
+      <c r="T132" s="62"/>
+      <c r="U132" s="25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="133" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P133" s="5">
+        <v>44</v>
+      </c>
+      <c r="Q133" s="4">
+        <v>7513127.3439999996</v>
+      </c>
+      <c r="R133" s="4">
+        <v>4691712.3039999995</v>
+      </c>
+      <c r="S133" s="62"/>
+      <c r="T133" s="62"/>
+      <c r="U133" s="25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="134" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P134" s="5">
+        <v>45</v>
+      </c>
+      <c r="Q134" s="4">
+        <v>7513128.142</v>
+      </c>
+      <c r="R134" s="4">
+        <v>4691711.0889999997</v>
+      </c>
+      <c r="S134" s="62"/>
+      <c r="T134" s="62"/>
+      <c r="U134" s="25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="135" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P135" s="5">
+        <v>47</v>
+      </c>
+      <c r="Q135" s="4">
+        <v>7513132.0240000002</v>
+      </c>
+      <c r="R135" s="4">
+        <v>4691706.8949999996</v>
+      </c>
+      <c r="S135" s="62"/>
+      <c r="T135" s="62"/>
+      <c r="U135" s="25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="136" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P136" s="5">
+        <v>48</v>
+      </c>
+      <c r="Q136" s="4">
+        <v>7513134.6310000001</v>
+      </c>
+      <c r="R136" s="4">
+        <v>4691706.6350999996</v>
+      </c>
+      <c r="S136" s="62"/>
+      <c r="T136" s="62"/>
+      <c r="U136" s="25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="137" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P137" s="5">
+        <v>49</v>
+      </c>
+      <c r="Q137" s="4">
+        <v>7513134.1436999999</v>
+      </c>
+      <c r="R137" s="4">
+        <v>4691706.1939000003</v>
+      </c>
+      <c r="S137" s="62"/>
+      <c r="T137" s="62"/>
+      <c r="U137" s="25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="138" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P138" s="5">
+        <v>50</v>
+      </c>
+      <c r="Q138" s="4">
+        <v>7513132.5010000002</v>
+      </c>
+      <c r="R138" s="4">
+        <v>4691720.0990000004</v>
+      </c>
+      <c r="S138" s="62"/>
+      <c r="T138" s="62"/>
+      <c r="U138" s="25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="139" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P139" s="5">
+        <v>51</v>
+      </c>
+      <c r="Q139" s="4">
+        <v>7513133.2570000002</v>
+      </c>
+      <c r="R139" s="4">
+        <v>4691719.3229999999</v>
+      </c>
+      <c r="S139" s="62"/>
+      <c r="T139" s="62"/>
+      <c r="U139" s="25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="140" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P140" s="5">
+        <v>52</v>
+      </c>
+      <c r="Q140" s="4">
+        <v>7513135.568</v>
+      </c>
+      <c r="R140" s="4">
+        <v>4691722.8739999998</v>
+      </c>
+      <c r="S140" s="62"/>
+      <c r="T140" s="62"/>
+      <c r="U140" s="25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="141" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P141" s="5">
+        <v>78</v>
+      </c>
+      <c r="Q141" s="4">
+        <v>7513129.2801999999</v>
+      </c>
+      <c r="R141" s="4">
+        <v>4691715.7680000002</v>
+      </c>
+      <c r="S141" s="62"/>
+      <c r="T141" s="62"/>
+      <c r="U141" s="25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="142" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P142" s="5">
+        <v>79</v>
+      </c>
+      <c r="Q142" s="4">
+        <v>7513143.2529999996</v>
+      </c>
+      <c r="R142" s="4">
+        <v>4691714.4639999997</v>
+      </c>
+      <c r="S142" s="62"/>
+      <c r="T142" s="62"/>
+      <c r="U142" s="25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="143" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P143" s="5">
+        <v>80</v>
+      </c>
+      <c r="Q143" s="4">
+        <v>7513136.3596000001</v>
+      </c>
+      <c r="R143" s="4">
+        <v>4691708.2016000003</v>
+      </c>
+      <c r="S143" s="62"/>
+      <c r="T143" s="62"/>
+      <c r="U143" s="25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="144" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P144" s="5">
+        <v>82</v>
+      </c>
+      <c r="Q144" s="4">
+        <v>7513133.0180000002</v>
+      </c>
+      <c r="R144" s="4">
+        <v>4691706.2857999997</v>
+      </c>
+      <c r="S144" s="62"/>
+      <c r="T144" s="62"/>
+      <c r="U144" s="25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="145" spans="16:21" x14ac:dyDescent="0.25">
+      <c r="P145" s="5">
+        <v>106</v>
+      </c>
+      <c r="Q145" s="4">
+        <v>7513135.1146999998</v>
+      </c>
+      <c r="R145" s="4">
+        <v>4691717.4736000001</v>
+      </c>
+      <c r="S145" s="62"/>
+      <c r="T145" s="62"/>
+      <c r="U145" s="25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="146" spans="16:21" x14ac:dyDescent="0.25">
+      <c r="P146" s="5">
+        <v>107</v>
+      </c>
+      <c r="Q146" s="4">
+        <v>7513131.0981999999</v>
+      </c>
+      <c r="R146" s="4">
+        <v>4691713.8247999996</v>
+      </c>
+      <c r="S146" s="62"/>
+      <c r="T146" s="62"/>
+      <c r="U146" s="25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="147" spans="16:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P147" s="6">
+        <v>109</v>
+      </c>
+      <c r="Q147" s="7">
+        <v>7513133.3550000004</v>
+      </c>
+      <c r="R147" s="7">
+        <v>4691719.4106000001</v>
+      </c>
+      <c r="S147" s="63"/>
+      <c r="T147" s="63"/>
+      <c r="U147" s="26" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="F96:F112"/>
+    <mergeCell ref="G96:G112"/>
     <mergeCell ref="A67:D67"/>
     <mergeCell ref="E67:G67"/>
     <mergeCell ref="C8:I10"/>
@@ -4061,10 +4125,8 @@
     <mergeCell ref="J129:K130"/>
     <mergeCell ref="A130:D130"/>
     <mergeCell ref="E130:G130"/>
-    <mergeCell ref="F96:F110"/>
-    <mergeCell ref="G96:G110"/>
-    <mergeCell ref="F112:F128"/>
-    <mergeCell ref="G112:G128"/>
+    <mergeCell ref="S131:S147"/>
+    <mergeCell ref="T131:T147"/>
     <mergeCell ref="F78:F94"/>
     <mergeCell ref="G78:G94"/>
   </mergeCells>

</xml_diff>

<commit_message>
koordinatatt e katit nk vendosje
</commit_message>
<xml_diff>
--- a/5-Njësite-banesore/regjistri/22-Koordinatat-për-pjesë-të-ndertesës.xlsx-2602-0-Albnori.xlsx
+++ b/5-Njësite-banesore/regjistri/22-Koordinatat-për-pjesë-të-ndertesës.xlsx-2602-0-Albnori.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$130</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$132</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1739,10 +1739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U147"/>
+  <dimension ref="A1:K132"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A90" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G96" sqref="G96:G112"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A109" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="P127" sqref="P127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3663,6 +3663,24 @@
     <row r="113" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
+      <c r="C113" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D113" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E113" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F113" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G113" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H113" s="13" t="s">
+        <v>3</v>
+      </c>
       <c r="I113" s="1"/>
       <c r="J113" s="1"/>
       <c r="K113" s="1"/>
@@ -3670,6 +3688,24 @@
     <row r="114" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
+      <c r="C114" s="5">
+        <v>42</v>
+      </c>
+      <c r="D114" s="4">
+        <v>7513127.6977000004</v>
+      </c>
+      <c r="E114" s="4">
+        <v>4691714.3306</v>
+      </c>
+      <c r="F114" s="62">
+        <v>629.29999999999995</v>
+      </c>
+      <c r="G114" s="62" t="s">
+        <v>24</v>
+      </c>
+      <c r="H114" s="25" t="s">
+        <v>8</v>
+      </c>
       <c r="I114" s="1"/>
       <c r="J114" s="1"/>
       <c r="K114" s="1"/>
@@ -3677,6 +3713,20 @@
     <row r="115" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
+      <c r="C115" s="5">
+        <v>43</v>
+      </c>
+      <c r="D115" s="4">
+        <v>7513127.2779999999</v>
+      </c>
+      <c r="E115" s="4">
+        <v>4691713.9479999999</v>
+      </c>
+      <c r="F115" s="62"/>
+      <c r="G115" s="62"/>
+      <c r="H115" s="25" t="s">
+        <v>8</v>
+      </c>
       <c r="I115" s="1"/>
       <c r="J115" s="1"/>
       <c r="K115" s="1"/>
@@ -3684,6 +3734,20 @@
     <row r="116" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
+      <c r="C116" s="5">
+        <v>44</v>
+      </c>
+      <c r="D116" s="4">
+        <v>7513127.3439999996</v>
+      </c>
+      <c r="E116" s="4">
+        <v>4691712.3039999995</v>
+      </c>
+      <c r="F116" s="62"/>
+      <c r="G116" s="62"/>
+      <c r="H116" s="25" t="s">
+        <v>8</v>
+      </c>
       <c r="I116" s="1"/>
       <c r="J116" s="1"/>
       <c r="K116" s="1"/>
@@ -3691,6 +3755,20 @@
     <row r="117" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
+      <c r="C117" s="5">
+        <v>45</v>
+      </c>
+      <c r="D117" s="4">
+        <v>7513128.142</v>
+      </c>
+      <c r="E117" s="4">
+        <v>4691711.0889999997</v>
+      </c>
+      <c r="F117" s="62"/>
+      <c r="G117" s="62"/>
+      <c r="H117" s="25" t="s">
+        <v>8</v>
+      </c>
       <c r="I117" s="1"/>
       <c r="J117" s="1"/>
       <c r="K117" s="1"/>
@@ -3698,6 +3776,20 @@
     <row r="118" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
+      <c r="C118" s="5">
+        <v>47</v>
+      </c>
+      <c r="D118" s="4">
+        <v>7513132.0240000002</v>
+      </c>
+      <c r="E118" s="4">
+        <v>4691706.8949999996</v>
+      </c>
+      <c r="F118" s="62"/>
+      <c r="G118" s="62"/>
+      <c r="H118" s="25" t="s">
+        <v>8</v>
+      </c>
       <c r="I118" s="1"/>
       <c r="J118" s="1"/>
       <c r="K118" s="1"/>
@@ -3705,6 +3797,20 @@
     <row r="119" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
+      <c r="C119" s="5">
+        <v>48</v>
+      </c>
+      <c r="D119" s="4">
+        <v>7513134.6310000001</v>
+      </c>
+      <c r="E119" s="4">
+        <v>4691706.6350999996</v>
+      </c>
+      <c r="F119" s="62"/>
+      <c r="G119" s="62"/>
+      <c r="H119" s="25" t="s">
+        <v>8</v>
+      </c>
       <c r="I119" s="1"/>
       <c r="J119" s="1"/>
       <c r="K119" s="1"/>
@@ -3712,6 +3818,20 @@
     <row r="120" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
+      <c r="C120" s="5">
+        <v>49</v>
+      </c>
+      <c r="D120" s="4">
+        <v>7513134.1436999999</v>
+      </c>
+      <c r="E120" s="4">
+        <v>4691706.1939000003</v>
+      </c>
+      <c r="F120" s="62"/>
+      <c r="G120" s="62"/>
+      <c r="H120" s="25" t="s">
+        <v>8</v>
+      </c>
       <c r="I120" s="1"/>
       <c r="J120" s="1"/>
       <c r="K120" s="1"/>
@@ -3719,6 +3839,20 @@
     <row r="121" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
+      <c r="C121" s="5">
+        <v>50</v>
+      </c>
+      <c r="D121" s="4">
+        <v>7513132.5010000002</v>
+      </c>
+      <c r="E121" s="4">
+        <v>4691720.0990000004</v>
+      </c>
+      <c r="F121" s="62"/>
+      <c r="G121" s="62"/>
+      <c r="H121" s="25" t="s">
+        <v>8</v>
+      </c>
       <c r="I121" s="1"/>
       <c r="J121" s="1"/>
       <c r="K121" s="1"/>
@@ -3726,6 +3860,20 @@
     <row r="122" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
+      <c r="C122" s="5">
+        <v>51</v>
+      </c>
+      <c r="D122" s="4">
+        <v>7513133.2570000002</v>
+      </c>
+      <c r="E122" s="4">
+        <v>4691719.3229999999</v>
+      </c>
+      <c r="F122" s="62"/>
+      <c r="G122" s="62"/>
+      <c r="H122" s="25" t="s">
+        <v>8</v>
+      </c>
       <c r="I122" s="1"/>
       <c r="J122" s="1"/>
       <c r="K122" s="1"/>
@@ -3733,6 +3881,20 @@
     <row r="123" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
+      <c r="C123" s="5">
+        <v>52</v>
+      </c>
+      <c r="D123" s="4">
+        <v>7513135.568</v>
+      </c>
+      <c r="E123" s="4">
+        <v>4691722.8739999998</v>
+      </c>
+      <c r="F123" s="62"/>
+      <c r="G123" s="62"/>
+      <c r="H123" s="25" t="s">
+        <v>8</v>
+      </c>
       <c r="I123" s="1"/>
       <c r="J123" s="1"/>
       <c r="K123" s="1"/>
@@ -3740,6 +3902,20 @@
     <row r="124" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
+      <c r="C124" s="5">
+        <v>78</v>
+      </c>
+      <c r="D124" s="4">
+        <v>7513129.2801999999</v>
+      </c>
+      <c r="E124" s="4">
+        <v>4691715.7680000002</v>
+      </c>
+      <c r="F124" s="62"/>
+      <c r="G124" s="62"/>
+      <c r="H124" s="25" t="s">
+        <v>8</v>
+      </c>
       <c r="I124" s="1"/>
       <c r="J124" s="1"/>
       <c r="K124" s="1"/>
@@ -3747,6 +3923,20 @@
     <row r="125" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
+      <c r="C125" s="5">
+        <v>79</v>
+      </c>
+      <c r="D125" s="4">
+        <v>7513143.2529999996</v>
+      </c>
+      <c r="E125" s="4">
+        <v>4691714.4639999997</v>
+      </c>
+      <c r="F125" s="62"/>
+      <c r="G125" s="62"/>
+      <c r="H125" s="25" t="s">
+        <v>8</v>
+      </c>
       <c r="I125" s="1"/>
       <c r="J125" s="1"/>
       <c r="K125" s="1"/>
@@ -3754,6 +3944,20 @@
     <row r="126" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
+      <c r="C126" s="5">
+        <v>80</v>
+      </c>
+      <c r="D126" s="4">
+        <v>7513136.3596000001</v>
+      </c>
+      <c r="E126" s="4">
+        <v>4691708.2016000003</v>
+      </c>
+      <c r="F126" s="62"/>
+      <c r="G126" s="62"/>
+      <c r="H126" s="25" t="s">
+        <v>8</v>
+      </c>
       <c r="I126" s="1"/>
       <c r="J126" s="1"/>
       <c r="K126" s="1"/>
@@ -3761,346 +3965,122 @@
     <row r="127" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
+      <c r="C127" s="5">
+        <v>82</v>
+      </c>
+      <c r="D127" s="4">
+        <v>7513133.0180000002</v>
+      </c>
+      <c r="E127" s="4">
+        <v>4691706.2857999997</v>
+      </c>
+      <c r="F127" s="62"/>
+      <c r="G127" s="62"/>
+      <c r="H127" s="25" t="s">
+        <v>8</v>
+      </c>
       <c r="I127" s="1"/>
       <c r="J127" s="1"/>
       <c r="K127" s="1"/>
     </row>
-    <row r="128" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
+      <c r="C128" s="5">
+        <v>106</v>
+      </c>
+      <c r="D128" s="4">
+        <v>7513135.1146999998</v>
+      </c>
+      <c r="E128" s="4">
+        <v>4691717.4736000001</v>
+      </c>
+      <c r="F128" s="62"/>
+      <c r="G128" s="62"/>
+      <c r="H128" s="25" t="s">
+        <v>8</v>
+      </c>
       <c r="I128" s="1"/>
       <c r="J128" s="1"/>
       <c r="K128" s="1"/>
     </row>
-    <row r="129" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A129" s="2" t="s">
+    <row r="129" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A129" s="1"/>
+      <c r="B129" s="1"/>
+      <c r="C129" s="5">
+        <v>107</v>
+      </c>
+      <c r="D129" s="4">
+        <v>7513131.0981999999</v>
+      </c>
+      <c r="E129" s="4">
+        <v>4691713.8247999996</v>
+      </c>
+      <c r="F129" s="62"/>
+      <c r="G129" s="62"/>
+      <c r="H129" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="I129" s="1"/>
+      <c r="J129" s="1"/>
+      <c r="K129" s="1"/>
+    </row>
+    <row r="130" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A130" s="1"/>
+      <c r="B130" s="1"/>
+      <c r="C130" s="6">
+        <v>109</v>
+      </c>
+      <c r="D130" s="7">
+        <v>7513133.3550000004</v>
+      </c>
+      <c r="E130" s="7">
+        <v>4691719.4106000001</v>
+      </c>
+      <c r="F130" s="63"/>
+      <c r="G130" s="63"/>
+      <c r="H130" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="I130" s="1"/>
+      <c r="J130" s="1"/>
+      <c r="K130" s="1"/>
+    </row>
+    <row r="131" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A131" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B129" s="3"/>
-      <c r="C129" s="3"/>
-      <c r="D129" s="3"/>
-      <c r="E129" s="45" t="s">
+      <c r="B131" s="3"/>
+      <c r="C131" s="3"/>
+      <c r="D131" s="3"/>
+      <c r="E131" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="F129" s="46"/>
-      <c r="G129" s="47"/>
-      <c r="H129" s="48" t="s">
+      <c r="F131" s="46"/>
+      <c r="G131" s="47"/>
+      <c r="H131" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="I129" s="49"/>
-      <c r="J129" s="52"/>
-      <c r="K129" s="53"/>
-    </row>
-    <row r="130" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A130" s="56" t="s">
+      <c r="I131" s="49"/>
+      <c r="J131" s="52"/>
+      <c r="K131" s="53"/>
+    </row>
+    <row r="132" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A132" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B130" s="57"/>
-      <c r="C130" s="57"/>
-      <c r="D130" s="58"/>
-      <c r="E130" s="59">
+      <c r="B132" s="57"/>
+      <c r="C132" s="57"/>
+      <c r="D132" s="58"/>
+      <c r="E132" s="59">
         <v>152</v>
       </c>
-      <c r="F130" s="60"/>
-      <c r="G130" s="61"/>
-      <c r="H130" s="50"/>
-      <c r="I130" s="51"/>
-      <c r="J130" s="54"/>
-      <c r="K130" s="55"/>
-      <c r="P130" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q130" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="R130" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="S130" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="T130" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="U130" s="13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="131" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="P131" s="5">
-        <v>42</v>
-      </c>
-      <c r="Q131" s="4">
-        <v>7513127.6977000004</v>
-      </c>
-      <c r="R131" s="4">
-        <v>4691714.3306</v>
-      </c>
-      <c r="S131" s="62">
-        <v>629.29999999999995</v>
-      </c>
-      <c r="T131" s="62" t="s">
-        <v>24</v>
-      </c>
-      <c r="U131" s="25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="132" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="P132" s="5">
-        <v>43</v>
-      </c>
-      <c r="Q132" s="4">
-        <v>7513127.2779999999</v>
-      </c>
-      <c r="R132" s="4">
-        <v>4691713.9479999999</v>
-      </c>
-      <c r="S132" s="62"/>
-      <c r="T132" s="62"/>
-      <c r="U132" s="25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="133" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="P133" s="5">
-        <v>44</v>
-      </c>
-      <c r="Q133" s="4">
-        <v>7513127.3439999996</v>
-      </c>
-      <c r="R133" s="4">
-        <v>4691712.3039999995</v>
-      </c>
-      <c r="S133" s="62"/>
-      <c r="T133" s="62"/>
-      <c r="U133" s="25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="134" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="P134" s="5">
-        <v>45</v>
-      </c>
-      <c r="Q134" s="4">
-        <v>7513128.142</v>
-      </c>
-      <c r="R134" s="4">
-        <v>4691711.0889999997</v>
-      </c>
-      <c r="S134" s="62"/>
-      <c r="T134" s="62"/>
-      <c r="U134" s="25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="135" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="P135" s="5">
-        <v>47</v>
-      </c>
-      <c r="Q135" s="4">
-        <v>7513132.0240000002</v>
-      </c>
-      <c r="R135" s="4">
-        <v>4691706.8949999996</v>
-      </c>
-      <c r="S135" s="62"/>
-      <c r="T135" s="62"/>
-      <c r="U135" s="25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="136" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="P136" s="5">
-        <v>48</v>
-      </c>
-      <c r="Q136" s="4">
-        <v>7513134.6310000001</v>
-      </c>
-      <c r="R136" s="4">
-        <v>4691706.6350999996</v>
-      </c>
-      <c r="S136" s="62"/>
-      <c r="T136" s="62"/>
-      <c r="U136" s="25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="137" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="P137" s="5">
-        <v>49</v>
-      </c>
-      <c r="Q137" s="4">
-        <v>7513134.1436999999</v>
-      </c>
-      <c r="R137" s="4">
-        <v>4691706.1939000003</v>
-      </c>
-      <c r="S137" s="62"/>
-      <c r="T137" s="62"/>
-      <c r="U137" s="25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="138" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="P138" s="5">
-        <v>50</v>
-      </c>
-      <c r="Q138" s="4">
-        <v>7513132.5010000002</v>
-      </c>
-      <c r="R138" s="4">
-        <v>4691720.0990000004</v>
-      </c>
-      <c r="S138" s="62"/>
-      <c r="T138" s="62"/>
-      <c r="U138" s="25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="139" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="P139" s="5">
-        <v>51</v>
-      </c>
-      <c r="Q139" s="4">
-        <v>7513133.2570000002</v>
-      </c>
-      <c r="R139" s="4">
-        <v>4691719.3229999999</v>
-      </c>
-      <c r="S139" s="62"/>
-      <c r="T139" s="62"/>
-      <c r="U139" s="25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="140" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="P140" s="5">
-        <v>52</v>
-      </c>
-      <c r="Q140" s="4">
-        <v>7513135.568</v>
-      </c>
-      <c r="R140" s="4">
-        <v>4691722.8739999998</v>
-      </c>
-      <c r="S140" s="62"/>
-      <c r="T140" s="62"/>
-      <c r="U140" s="25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="141" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="P141" s="5">
-        <v>78</v>
-      </c>
-      <c r="Q141" s="4">
-        <v>7513129.2801999999</v>
-      </c>
-      <c r="R141" s="4">
-        <v>4691715.7680000002</v>
-      </c>
-      <c r="S141" s="62"/>
-      <c r="T141" s="62"/>
-      <c r="U141" s="25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="142" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="P142" s="5">
-        <v>79</v>
-      </c>
-      <c r="Q142" s="4">
-        <v>7513143.2529999996</v>
-      </c>
-      <c r="R142" s="4">
-        <v>4691714.4639999997</v>
-      </c>
-      <c r="S142" s="62"/>
-      <c r="T142" s="62"/>
-      <c r="U142" s="25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="143" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="P143" s="5">
-        <v>80</v>
-      </c>
-      <c r="Q143" s="4">
-        <v>7513136.3596000001</v>
-      </c>
-      <c r="R143" s="4">
-        <v>4691708.2016000003</v>
-      </c>
-      <c r="S143" s="62"/>
-      <c r="T143" s="62"/>
-      <c r="U143" s="25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="144" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="P144" s="5">
-        <v>82</v>
-      </c>
-      <c r="Q144" s="4">
-        <v>7513133.0180000002</v>
-      </c>
-      <c r="R144" s="4">
-        <v>4691706.2857999997</v>
-      </c>
-      <c r="S144" s="62"/>
-      <c r="T144" s="62"/>
-      <c r="U144" s="25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="145" spans="16:21" x14ac:dyDescent="0.25">
-      <c r="P145" s="5">
-        <v>106</v>
-      </c>
-      <c r="Q145" s="4">
-        <v>7513135.1146999998</v>
-      </c>
-      <c r="R145" s="4">
-        <v>4691717.4736000001</v>
-      </c>
-      <c r="S145" s="62"/>
-      <c r="T145" s="62"/>
-      <c r="U145" s="25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="146" spans="16:21" x14ac:dyDescent="0.25">
-      <c r="P146" s="5">
-        <v>107</v>
-      </c>
-      <c r="Q146" s="4">
-        <v>7513131.0981999999</v>
-      </c>
-      <c r="R146" s="4">
-        <v>4691713.8247999996</v>
-      </c>
-      <c r="S146" s="62"/>
-      <c r="T146" s="62"/>
-      <c r="U146" s="25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="147" spans="16:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P147" s="6">
-        <v>109</v>
-      </c>
-      <c r="Q147" s="7">
-        <v>7513133.3550000004</v>
-      </c>
-      <c r="R147" s="7">
-        <v>4691719.4106000001</v>
-      </c>
-      <c r="S147" s="63"/>
-      <c r="T147" s="63"/>
-      <c r="U147" s="26" t="s">
-        <v>8</v>
-      </c>
+      <c r="F132" s="60"/>
+      <c r="G132" s="61"/>
+      <c r="H132" s="50"/>
+      <c r="I132" s="51"/>
+      <c r="J132" s="54"/>
+      <c r="K132" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="25">
@@ -4120,13 +4100,13 @@
     <mergeCell ref="A68:K69"/>
     <mergeCell ref="A70:K73"/>
     <mergeCell ref="C74:I76"/>
-    <mergeCell ref="E129:G129"/>
-    <mergeCell ref="H129:I130"/>
-    <mergeCell ref="J129:K130"/>
-    <mergeCell ref="A130:D130"/>
-    <mergeCell ref="E130:G130"/>
-    <mergeCell ref="S131:S147"/>
-    <mergeCell ref="T131:T147"/>
+    <mergeCell ref="E131:G131"/>
+    <mergeCell ref="H131:I132"/>
+    <mergeCell ref="J131:K132"/>
+    <mergeCell ref="A132:D132"/>
+    <mergeCell ref="E132:G132"/>
+    <mergeCell ref="F114:F130"/>
+    <mergeCell ref="G114:G130"/>
     <mergeCell ref="F78:F94"/>
     <mergeCell ref="G78:G94"/>
   </mergeCells>

</xml_diff>